<commit_message>
Fix BRP in likelihood bug and added F init
Added species specific F init for non-equilibrium starting population age-structure (initMode = 3)
Added forecast switch so that the BRP likelihood would not be included in the jnll when estimating the hindcast
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1081,19 +1081,14 @@
       <c r="A21">
         <v>13</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
-      </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>est_M1</t>
+          <t>fleet_control</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Integer: switch to estimate residual (multi-species mode) or total natural mortality (single-species mode). 0 = use fixed natural mortality from M1_base, 1 = estimate sex- and age-invariant M1, 2 = sex-specific (two-sex model), age-invariant M1, 3 =   estimate sex- and age-specific M1.</t>
+          <t>Survey and fishery data specifications</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1118,12 +1113,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>fleet_control</t>
+          <t>srv_biom</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Survey and fishery data specifications</t>
+          <t>Survey index in weight (kg) or numbers data</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1148,12 +1143,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>srv_biom</t>
+          <t>fsh_biom</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Survey index in weight (kg) or numbers data</t>
+          <t>Total catch in weight (kg) or numbers data</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1178,12 +1173,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>fsh_biom</t>
+          <t>comp_data</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Total catch in weight (kg) or numbers data</t>
+          <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1208,12 +1203,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>comp_data</t>
+          <t>emp_sel</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
+          <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1238,12 +1233,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>emp_sel</t>
+          <t>age_trans_matrix</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
+          <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. Can have multiple matrices for a species specified by Age_transition_index.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1268,12 +1263,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>age_trans_matrix</t>
+          <t>age_error</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. Can have multiple matrices for a species specified by Age_transition_index.</t>
+          <t>Aging error matrices. Can have only one per species.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1298,12 +1293,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>age_error</t>
+          <t>wt</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Aging error matrices. Can have only one per species.</t>
+          <t>Weight-at-age (wt) to use for calculation of derived quantities (SSB, Consumption/Ration, Suitability, Total Catch, Survey Biomass, etc). Can have multiple weight-at-age data-sets for each species, but must be full for all years of the hindcast.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1328,12 +1323,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>wt</t>
+          <t>pmature</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Weight-at-age (wt) to use for calculation of derived quantities (SSB, Consumption/Ration, Suitability, Total Catch, Survey Biomass, etc). Can have multiple weight-at-age data-sets for each species, but must be full for all years of the hindcast.</t>
+          <t>Maturity-at-age for each species</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1358,12 +1353,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>pmature</t>
+          <t>propF</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Maturity-at-age for each species</t>
+          <t>Percent female at age for each species</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1383,12 +1378,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>propF</t>
+          <t>M1_base</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Percent female at age for each species</t>
+          <t>Residual natural mortality for each species</t>
         </is>
       </c>
     </row>
@@ -1398,12 +1393,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>M1_base</t>
+          <t>aLW</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Residual natural mortality for each species</t>
+          <t>Parameters for weight-at-length power function for each species. . Used when estimating time-variant length-based gamma suitability (suitMode = 2) or time-variant length-based lognormal suitability (suitMode = 5)</t>
         </is>
       </c>
     </row>
@@ -1411,14 +1406,19 @@
       <c r="A33">
         <v>25</v>
       </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>bioenergetics_control</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>aLW</t>
+          <t>Ceq</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Parameters for weight-at-length power function for each species. . Used when estimating time-variant length-based gamma suitability (suitMode = 2) or time-variant length-based lognormal suitability (suitMode = 5)</t>
+          <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979); 4 = 1 for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1438,12 +1438,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ceq</t>
+          <t>Cindex</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979); 4 = 1 for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
+          <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1463,12 +1463,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cindex</t>
+          <t>Pvalue</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
+          <t>Numeric: this scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1488,12 +1488,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Pvalue</t>
+          <t>fday</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Numeric: this scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
+          <t>Numeric: number of foraging days per year for each species</t>
         </is>
       </c>
     </row>
@@ -1508,12 +1508,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>fday</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Numeric: number of foraging days per year for each species</t>
+          <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
         </is>
       </c>
     </row>
@@ -1528,12 +1528,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
+          <t>Slope of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
         </is>
       </c>
     </row>
@@ -1548,12 +1548,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>Qc</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Slope of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
+          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Qc</t>
+          <t>Tco</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Tco</t>
+          <t>Tcm</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Tcm</t>
+          <t>Tcl</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Tcl</t>
+          <t>CK1</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CK1</t>
+          <t>CK4</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1661,19 +1661,14 @@
       <c r="A45">
         <v>37</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>bioenergetics_control</t>
-        </is>
-      </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CK4</t>
+          <t>env_data</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
+          <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5. Will use the mean for missing years. Temperature should be in celcius.</t>
         </is>
       </c>
     </row>
@@ -1683,12 +1678,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>env_data</t>
+          <t>Pyrs</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5. Will use the mean for missing years. Temperature should be in celcius.</t>
+          <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
         </is>
       </c>
     </row>
@@ -1698,25 +1693,10 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Pyrs</t>
+          <t>UobsWtAge</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
-        <is>
-          <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>40</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>UobsWtAge</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
         <is>
           <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
         </is>
@@ -78977,7 +78957,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -79240,22 +79220,6 @@
         <is>
           <t>sex_ratio_sigma</t>
         </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>est_M1</t>
-        </is>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update M priors and tests
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -4561,7 +4561,7 @@
         <v>0.6820565</v>
       </c>
       <c r="L2">
-        <v>0.8397521999999999</v>
+        <v>0.8397522</v>
       </c>
       <c r="M2">
         <v>0.9915121</v>
@@ -4616,7 +4616,7 @@
         <v>0.6820565</v>
       </c>
       <c r="L3">
-        <v>0.8397521999999999</v>
+        <v>0.8397522</v>
       </c>
       <c r="M3">
         <v>0.9915121</v>
@@ -4723,7 +4723,7 @@
         <v>0.428903178</v>
       </c>
       <c r="K5">
-        <v>0.668601968</v>
+        <v>0.6686019680000001</v>
       </c>
       <c r="L5">
         <v>1.004004033</v>
@@ -4781,7 +4781,7 @@
         <v>0.575604904</v>
       </c>
       <c r="L6">
-        <v>0.739416154</v>
+        <v>0.7394161540000001</v>
       </c>
       <c r="M6">
         <v>1.068567323</v>
@@ -4998,7 +4998,7 @@
         <v>0.434168571</v>
       </c>
       <c r="K10">
-        <v>0.5299755819999999</v>
+        <v>0.529975582</v>
       </c>
       <c r="L10">
         <v>0.703008924</v>
@@ -5010,7 +5010,7 @@
         <v>0.888000873</v>
       </c>
       <c r="O10">
-        <v>0.9856767239999999</v>
+        <v>0.985676724</v>
       </c>
       <c r="P10">
         <v>1.193588801</v>
@@ -5111,7 +5111,7 @@
         <v>0.5338019980000001</v>
       </c>
       <c r="L12">
-        <v>0.628037142</v>
+        <v>0.6280371420000001</v>
       </c>
       <c r="M12">
         <v>0.6833034650000001</v>
@@ -5160,7 +5160,7 @@
         <v>0.376630035</v>
       </c>
       <c r="J13">
-        <v>0.502998962</v>
+        <v>0.5029989620000001</v>
       </c>
       <c r="K13">
         <v>0.573065432</v>
@@ -5496,10 +5496,10 @@
         <v>0.596229054</v>
       </c>
       <c r="L19">
-        <v>0.733046551</v>
+        <v>0.7330465510000001</v>
       </c>
       <c r="M19">
-        <v>0.815006721</v>
+        <v>0.8150067210000001</v>
       </c>
       <c r="N19">
         <v>0.971352934</v>
@@ -5771,7 +5771,7 @@
         <v>0.617633322</v>
       </c>
       <c r="L24">
-        <v>0.773776635</v>
+        <v>0.7737766350000001</v>
       </c>
       <c r="M24">
         <v>0.820595866</v>
@@ -5887,7 +5887,7 @@
         <v>0.8321758970000001</v>
       </c>
       <c r="N26">
-        <v>0.884492856</v>
+        <v>0.8844928560000001</v>
       </c>
       <c r="O26">
         <v>0.961303653</v>
@@ -5933,7 +5933,7 @@
         <v>0.554839651</v>
       </c>
       <c r="K27">
-        <v>0.679600029</v>
+        <v>0.6796000290000001</v>
       </c>
       <c r="L27">
         <v>0.76519576</v>
@@ -5988,7 +5988,7 @@
         <v>0.516896768</v>
       </c>
       <c r="K28">
-        <v>0.608793965</v>
+        <v>0.6087939650000001</v>
       </c>
       <c r="L28">
         <v>0.702835715</v>
@@ -6040,7 +6040,7 @@
         <v>0.363608103</v>
       </c>
       <c r="J29">
-        <v>0.5175009699999999</v>
+        <v>0.51750097</v>
       </c>
       <c r="K29">
         <v>0.607355501</v>
@@ -6211,7 +6211,7 @@
         <v>0.669170666</v>
       </c>
       <c r="L32">
-        <v>0.8840580689999999</v>
+        <v>0.884058069</v>
       </c>
       <c r="M32">
         <v>1.009000445</v>
@@ -6263,13 +6263,13 @@
         <v>0.549263493</v>
       </c>
       <c r="K33">
-        <v>0.6792597379999999</v>
+        <v>0.679259738</v>
       </c>
       <c r="L33">
         <v>0.893518288</v>
       </c>
       <c r="M33">
-        <v>0.9821308989999999</v>
+        <v>0.982130899</v>
       </c>
       <c r="N33">
         <v>1.032776434</v>
@@ -6370,10 +6370,10 @@
         <v>0.358158972</v>
       </c>
       <c r="J35">
-        <v>0.533306122</v>
+        <v>0.5333061220000001</v>
       </c>
       <c r="K35">
-        <v>0.6707463299999999</v>
+        <v>0.67074633</v>
       </c>
       <c r="L35">
         <v>0.807299177</v>
@@ -6599,7 +6599,7 @@
         <v>0.698561299</v>
       </c>
       <c r="M39">
-        <v>0.782161587</v>
+        <v>0.7821615870000001</v>
       </c>
       <c r="N39">
         <v>0.844000541</v>
@@ -6651,7 +6651,7 @@
         <v>0.668715635</v>
       </c>
       <c r="L40">
-        <v>0.7591041509999999</v>
+        <v>0.759104151</v>
       </c>
       <c r="M40">
         <v>0.844249481</v>
@@ -6694,7 +6694,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H41">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I41">
         <v>1.344427</v>
@@ -6749,7 +6749,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H42">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I42">
         <v>1.344427</v>
@@ -6914,7 +6914,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H45">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I45">
         <v>1.344427</v>
@@ -7079,7 +7079,7 @@
         <v>0.2308979</v>
       </c>
       <c r="H48">
-        <v>0.644669</v>
+        <v>0.6446690000000001</v>
       </c>
       <c r="I48">
         <v>1.282862</v>
@@ -7158,7 +7158,7 @@
         <v>8.579815999999999</v>
       </c>
       <c r="P49">
-        <v>9.848017</v>
+        <v>9.848017000000001</v>
       </c>
       <c r="Q49">
         <v>11.71415</v>
@@ -7409,7 +7409,7 @@
         <v>0.2320311</v>
       </c>
       <c r="H54">
-        <v>0.6493004999999999</v>
+        <v>0.6493005</v>
       </c>
       <c r="I54">
         <v>1.294171</v>
@@ -7574,7 +7574,7 @@
         <v>0.2320815</v>
       </c>
       <c r="H57">
-        <v>0.6495069999999999</v>
+        <v>0.649507</v>
       </c>
       <c r="I57">
         <v>1.294676</v>
@@ -8475,7 +8475,7 @@
         <v>8.062624</v>
       </c>
       <c r="O73">
-        <v>9.553563</v>
+        <v>9.553563000000001</v>
       </c>
       <c r="P73">
         <v>11.0069</v>
@@ -8509,7 +8509,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H74">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I74">
         <v>1.344427</v>
@@ -8564,7 +8564,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H75">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I75">
         <v>1.344427</v>
@@ -8619,7 +8619,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H76">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I76">
         <v>1.344427</v>
@@ -8674,7 +8674,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H77">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I77">
         <v>1.344427</v>
@@ -8729,7 +8729,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H78">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I78">
         <v>1.344427</v>
@@ -8784,7 +8784,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H79">
-        <v>0.6697767999999999</v>
+        <v>0.6697768</v>
       </c>
       <c r="I79">
         <v>1.344427</v>
@@ -9173,7 +9173,7 @@
         <v>0.3249681</v>
       </c>
       <c r="J84">
-        <v>0.5305164999999999</v>
+        <v>0.5305165</v>
       </c>
       <c r="K84">
         <v>0.775014</v>
@@ -9328,7 +9328,7 @@
         <v>0.01321826</v>
       </c>
       <c r="G86">
-        <v>0.06417196999999999</v>
+        <v>0.06417197</v>
       </c>
       <c r="H86">
         <v>0.1684496</v>
@@ -9586,7 +9586,7 @@
         <v>0.5425362</v>
       </c>
       <c r="K89">
-        <v>0.7951762999999999</v>
+        <v>0.7951763</v>
       </c>
       <c r="L89">
         <v>1.079442</v>
@@ -9668,7 +9668,7 @@
         <v>0.5271326</v>
       </c>
       <c r="K90">
-        <v>0.7693524</v>
+        <v>0.7693524000000001</v>
       </c>
       <c r="L90">
         <v>1.040711</v>
@@ -10476,7 +10476,7 @@
         <v>0.01307071</v>
       </c>
       <c r="G100">
-        <v>0.06518728999999999</v>
+        <v>0.06518729</v>
       </c>
       <c r="H100">
         <v>0.1741539</v>
@@ -10895,7 +10895,7 @@
         <v>0.334899</v>
       </c>
       <c r="J105">
-        <v>0.5512337</v>
+        <v>0.5512337000000001</v>
       </c>
       <c r="K105">
         <v>0.8114404</v>
@@ -12201,7 +12201,7 @@
         <v>0.52816</v>
       </c>
       <c r="H3">
-        <v>0.7461449999999999</v>
+        <v>0.746145</v>
       </c>
       <c r="I3">
         <v>0.8852950000000001</v>
@@ -12242,7 +12242,7 @@
         <v>0.837937385</v>
       </c>
       <c r="H4">
-        <v>0.9734748009999999</v>
+        <v>0.973474801</v>
       </c>
       <c r="I4">
         <v>0.995967742</v>
@@ -12556,7 +12556,7 @@
         <v>0.93703</v>
       </c>
       <c r="U4">
-        <v>0.94532</v>
+        <v>0.9453200000000001</v>
       </c>
       <c r="V4">
         <v>0.95257</v>
@@ -13633,7 +13633,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G2">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H2">
         <v>77.2967</v>
@@ -13680,7 +13680,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G3">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H3">
         <v>77.2967</v>
@@ -13736,7 +13736,7 @@
         <v>78.2727</v>
       </c>
       <c r="J4">
-        <v>77.4492</v>
+        <v>77.44920000000001</v>
       </c>
       <c r="K4">
         <v>76.95440000000001</v>
@@ -13830,7 +13830,7 @@
         <v>69.9829</v>
       </c>
       <c r="J6">
-        <v>69.5498</v>
+        <v>69.54980000000001</v>
       </c>
       <c r="K6">
         <v>69.3948</v>
@@ -13886,7 +13886,7 @@
         <v>78.7354</v>
       </c>
       <c r="M7">
-        <v>79.0635</v>
+        <v>79.06350000000001</v>
       </c>
       <c r="N7">
         <v>79.617</v>
@@ -13959,7 +13959,7 @@
         <v>72.80289999999999</v>
       </c>
       <c r="F9">
-        <v>74.7373</v>
+        <v>74.73730000000001</v>
       </c>
       <c r="G9">
         <v>77.08110000000001</v>
@@ -13983,7 +13983,7 @@
         <v>81.12990000000001</v>
       </c>
       <c r="N9">
-        <v>82.0849</v>
+        <v>82.08490000000001</v>
       </c>
       <c r="O9">
         <v>83.8866</v>
@@ -14015,7 +14015,7 @@
         <v>79.38720000000001</v>
       </c>
       <c r="I10">
-        <v>78.4188</v>
+        <v>78.41880000000001</v>
       </c>
       <c r="J10">
         <v>77.9448</v>
@@ -14030,7 +14030,7 @@
         <v>78.1143</v>
       </c>
       <c r="N10">
-        <v>78.51739999999999</v>
+        <v>78.5174</v>
       </c>
       <c r="O10">
         <v>79.5454</v>
@@ -14056,7 +14056,7 @@
         <v>73.8518</v>
       </c>
       <c r="G11">
-        <v>76.11799999999999</v>
+        <v>76.118</v>
       </c>
       <c r="H11">
         <v>77.6767</v>
@@ -14065,7 +14065,7 @@
         <v>77.4243</v>
       </c>
       <c r="J11">
-        <v>77.6474</v>
+        <v>77.64740000000001</v>
       </c>
       <c r="K11">
         <v>78.16070000000001</v>
@@ -14262,7 +14262,7 @@
         <v>80.4949</v>
       </c>
       <c r="M15">
-        <v>81.51139999999999</v>
+        <v>81.5114</v>
       </c>
       <c r="N15">
         <v>82.59139999999999</v>
@@ -14312,7 +14312,7 @@
         <v>78.8276</v>
       </c>
       <c r="N16">
-        <v>79.3897</v>
+        <v>79.38970000000001</v>
       </c>
       <c r="O16">
         <v>80.6387</v>
@@ -14335,7 +14335,7 @@
         <v>74.57680000000001</v>
       </c>
       <c r="F17">
-        <v>76.68519999999999</v>
+        <v>76.6852</v>
       </c>
       <c r="G17">
         <v>79.24379999999999</v>
@@ -14470,7 +14470,7 @@
         <v>1997</v>
       </c>
       <c r="D20">
-        <v>65.9689</v>
+        <v>65.96890000000001</v>
       </c>
       <c r="E20">
         <v>66.9862</v>
@@ -14564,7 +14564,7 @@
         <v>1999</v>
       </c>
       <c r="D22">
-        <v>69.73999999999999</v>
+        <v>69.74</v>
       </c>
       <c r="E22">
         <v>71.24590000000001</v>
@@ -14588,7 +14588,7 @@
         <v>81.81359999999999</v>
       </c>
       <c r="L22">
-        <v>83.10429999999999</v>
+        <v>83.1043</v>
       </c>
       <c r="M22">
         <v>84.4646</v>
@@ -14670,7 +14670,7 @@
         <v>77.4251</v>
       </c>
       <c r="H24">
-        <v>79.00069999999999</v>
+        <v>79.0007</v>
       </c>
       <c r="I24">
         <v>78.27419999999999</v>
@@ -14717,7 +14717,7 @@
         <v>72.58969999999999</v>
       </c>
       <c r="H25">
-        <v>73.3439</v>
+        <v>73.34390000000001</v>
       </c>
       <c r="I25">
         <v>72.46639999999999</v>
@@ -14764,7 +14764,7 @@
         <v>78.33499999999999</v>
       </c>
       <c r="H26">
-        <v>78.40309999999999</v>
+        <v>78.4031</v>
       </c>
       <c r="I26">
         <v>77.1631</v>
@@ -14785,7 +14785,7 @@
         <v>76.13160000000001</v>
       </c>
       <c r="O26">
-        <v>76.97029999999999</v>
+        <v>76.9703</v>
       </c>
     </row>
     <row r="27">
@@ -14993,7 +14993,7 @@
         <v>69.634</v>
       </c>
       <c r="F31">
-        <v>71.8593</v>
+        <v>71.85930000000001</v>
       </c>
       <c r="G31">
         <v>74.5994</v>
@@ -15005,7 +15005,7 @@
         <v>76.62350000000001</v>
       </c>
       <c r="J31">
-        <v>77.4552</v>
+        <v>77.45520000000001</v>
       </c>
       <c r="K31">
         <v>78.58410000000001</v>
@@ -15014,7 +15014,7 @@
         <v>79.896</v>
       </c>
       <c r="M31">
-        <v>81.32089999999999</v>
+        <v>81.3209</v>
       </c>
       <c r="N31">
         <v>82.8138</v>
@@ -15055,13 +15055,13 @@
         <v>78.92570000000001</v>
       </c>
       <c r="K32">
-        <v>80.1825</v>
+        <v>80.18250000000001</v>
       </c>
       <c r="L32">
         <v>81.66549999999999</v>
       </c>
       <c r="M32">
-        <v>83.3135</v>
+        <v>83.31350000000001</v>
       </c>
       <c r="N32">
         <v>85.0881</v>
@@ -15096,10 +15096,10 @@
         <v>77.06610000000001</v>
       </c>
       <c r="I33">
-        <v>77.4796</v>
+        <v>77.47960000000001</v>
       </c>
       <c r="J33">
-        <v>78.4415</v>
+        <v>78.44150000000001</v>
       </c>
       <c r="K33">
         <v>79.7681</v>
@@ -15184,7 +15184,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G35">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H35">
         <v>77.2967</v>
@@ -15231,7 +15231,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G36">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H36">
         <v>77.2967</v>
@@ -15278,7 +15278,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G37">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H37">
         <v>77.2967</v>
@@ -15325,7 +15325,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G38">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H38">
         <v>77.2967</v>
@@ -15372,7 +15372,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G39">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H39">
         <v>77.2967</v>
@@ -15419,7 +15419,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G40">
-        <v>75.98699999999999</v>
+        <v>75.987</v>
       </c>
       <c r="H40">
         <v>77.2967</v>
@@ -17903,7 +17903,7 @@
         <v>78.5538</v>
       </c>
       <c r="K88">
-        <v>76.23699999999999</v>
+        <v>76.237</v>
       </c>
       <c r="L88">
         <v>77.447</v>
@@ -18048,7 +18048,7 @@
         <v>100.1932</v>
       </c>
       <c r="J90">
-        <v>94.4569</v>
+        <v>94.45690000000001</v>
       </c>
       <c r="K90">
         <v>92.7714</v>
@@ -18575,7 +18575,7 @@
         <v>71.59690000000001</v>
       </c>
       <c r="M97">
-        <v>75.22029999999999</v>
+        <v>75.2203</v>
       </c>
       <c r="N97">
         <v>82.2286</v>
@@ -18705,7 +18705,7 @@
         <v>99.7668</v>
       </c>
       <c r="G99">
-        <v>94.9081</v>
+        <v>94.90810000000001</v>
       </c>
       <c r="H99">
         <v>88.51600000000001</v>
@@ -19072,7 +19072,7 @@
         <v>101.9125</v>
       </c>
       <c r="F104">
-        <v>98.20959999999999</v>
+        <v>98.2096</v>
       </c>
       <c r="G104">
         <v>93.05410000000001</v>
@@ -29821,7 +29821,7 @@
         <v>20</v>
       </c>
       <c r="I332">
-        <v>4.61e-05</v>
+        <v>4.61e-005</v>
       </c>
     </row>
     <row r="333">
@@ -36259,7 +36259,7 @@
         <v>20</v>
       </c>
       <c r="I554">
-        <v>0.06434811999999999</v>
+        <v>0.06434812</v>
       </c>
     </row>
     <row r="555">
@@ -36665,7 +36665,7 @@
         <v>20</v>
       </c>
       <c r="I568">
-        <v>0.008836656999999999</v>
+        <v>0.008836657</v>
       </c>
     </row>
     <row r="569">
@@ -39507,7 +39507,7 @@
         <v>20</v>
       </c>
       <c r="I666">
-        <v>0.07907031</v>
+        <v>0.07907031000000001</v>
       </c>
     </row>
     <row r="667">
@@ -40058,7 +40058,7 @@
         <v>20</v>
       </c>
       <c r="I685">
-        <v>0.008198973999999999</v>
+        <v>0.008198974</v>
       </c>
     </row>
     <row r="686">
@@ -47308,7 +47308,7 @@
         <v>20</v>
       </c>
       <c r="I935">
-        <v>6e-05</v>
+        <v>6e-005</v>
       </c>
     </row>
     <row r="936">
@@ -51571,7 +51571,7 @@
         <v>20</v>
       </c>
       <c r="I1082">
-        <v>0.06884556999999999</v>
+        <v>0.06884557</v>
       </c>
     </row>
     <row r="1083">
@@ -54355,7 +54355,7 @@
         <v>20</v>
       </c>
       <c r="I1178">
-        <v>0.5632433999999999</v>
+        <v>0.5632434</v>
       </c>
     </row>
     <row r="1179">
@@ -79022,7 +79022,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>2050</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="6">
@@ -80143,7 +80143,7 @@
         <v>6550414.87</v>
       </c>
       <c r="I9">
-        <v>0.09211958435883832</v>
+        <v>0.09211958435883833</v>
       </c>
     </row>
     <row r="10">
@@ -80515,7 +80515,7 @@
         <v>4196853.9</v>
       </c>
       <c r="I21">
-        <v>0.08086190826834753</v>
+        <v>0.08086190826834754</v>
       </c>
     </row>
     <row r="22">
@@ -81166,7 +81166,7 @@
         <v>1189234.46</v>
       </c>
       <c r="I42">
-        <v>0.05849707555563897</v>
+        <v>0.05849707555563898</v>
       </c>
     </row>
     <row r="43">
@@ -81504,7 +81504,7 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>627150.55</v>
+        <v>627150.5500000001</v>
       </c>
       <c r="I53">
         <v>0.10876005261786</v>
@@ -81969,7 +81969,7 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>896401.0699999999</v>
+        <v>896401.07</v>
       </c>
       <c r="I68">
         <v>0.1117503487285052</v>
@@ -82220,7 +82220,7 @@
         <v>160396</v>
       </c>
       <c r="I76">
-        <v>0.1429792055649829</v>
+        <v>0.142979205564983</v>
       </c>
     </row>
     <row r="77">
@@ -82437,7 +82437,7 @@
         <v>298788.7</v>
       </c>
       <c r="I83">
-        <v>0.1261991044529835</v>
+        <v>0.1261991044529836</v>
       </c>
     </row>
     <row r="84">
@@ -82961,7 +82961,7 @@
         <v>1</v>
       </c>
       <c r="H100">
-        <v>530126.8</v>
+        <v>530126.8000000001</v>
       </c>
       <c r="I100">
         <v>0.08653101992209057</v>
@@ -83736,7 +83736,7 @@
         <v>1</v>
       </c>
       <c r="H125">
-        <v>923.8433659999999</v>
+        <v>923.843366</v>
       </c>
       <c r="I125">
         <v>0.2</v>
@@ -97937,7 +97937,7 @@
         <v>266522.0805</v>
       </c>
       <c r="S121">
-        <v>837292.7706</v>
+        <v>837292.7706000001</v>
       </c>
       <c r="T121">
         <v>426717.2484</v>
@@ -98440,7 +98440,7 @@
         <v>828292.9068999999</v>
       </c>
       <c r="P129">
-        <v>997103.8895</v>
+        <v>997103.8895000001</v>
       </c>
       <c r="Q129">
         <v>168652.0961</v>
@@ -98559,7 +98559,7 @@
         <v>1049901.396</v>
       </c>
       <c r="M131">
-        <v>598741.599</v>
+        <v>598741.5990000001</v>
       </c>
       <c r="N131">
         <v>1069230.855</v>
@@ -98629,7 +98629,7 @@
         <v>932167.5946</v>
       </c>
       <c r="O132">
-        <v>783151.0895999999</v>
+        <v>783151.0896</v>
       </c>
       <c r="P132">
         <v>2564040.645</v>
@@ -99141,7 +99141,7 @@
         <v>1134406.589</v>
       </c>
       <c r="O140">
-        <v>889090.1554</v>
+        <v>889090.1554000001</v>
       </c>
       <c r="P140">
         <v>618182.879</v>
@@ -99720,7 +99720,7 @@
         <v>861.2938481</v>
       </c>
       <c r="P149">
-        <v>774.2097027999999</v>
+        <v>774.2097028</v>
       </c>
       <c r="Q149">
         <v>918.7848015</v>
@@ -103295,7 +103295,7 @@
         <v>58696.237</v>
       </c>
       <c r="S184">
-        <v>76350.88</v>
+        <v>76350.88000000001</v>
       </c>
       <c r="T184">
         <v>127063.244</v>
@@ -107517,7 +107517,7 @@
         <v>293.253466</v>
       </c>
       <c r="O227">
-        <v>69.32888699999999</v>
+        <v>69.328887</v>
       </c>
       <c r="P227">
         <v>66.771672</v>
@@ -108026,7 +108026,7 @@
         <v>669.189032</v>
       </c>
       <c r="N235">
-        <v>588.8287127999999</v>
+        <v>588.8287128</v>
       </c>
       <c r="O235">
         <v>305.6689523</v>
@@ -108334,7 +108334,7 @@
         <v>4438.331215</v>
       </c>
       <c r="J240">
-        <v>8614.892229999999</v>
+        <v>8614.89223</v>
       </c>
       <c r="K240">
         <v>941.2751066</v>
@@ -108352,7 +108352,7 @@
         <v>316.9225225</v>
       </c>
       <c r="P240">
-        <v>66.89265564999999</v>
+        <v>66.89265565</v>
       </c>
       <c r="Q240">
         <v>21.47372183</v>
@@ -108608,7 +108608,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H3">
         <v>1.15234</v>
@@ -108663,7 +108663,7 @@
         <v>0.5</v>
       </c>
       <c r="G4">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H4">
         <v>1.15234</v>
@@ -108718,7 +108718,7 @@
         <v>0.5</v>
       </c>
       <c r="G5">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H5">
         <v>1.15234</v>
@@ -108773,7 +108773,7 @@
         <v>0.5</v>
       </c>
       <c r="G6">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H6">
         <v>1.15234</v>
@@ -108828,7 +108828,7 @@
         <v>0.5</v>
       </c>
       <c r="G7">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H7">
         <v>1.15234</v>
@@ -108883,7 +108883,7 @@
         <v>0.5</v>
       </c>
       <c r="G8">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H8">
         <v>1.15234</v>
@@ -108938,7 +108938,7 @@
         <v>0.5</v>
       </c>
       <c r="G9">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H9">
         <v>1.15234</v>
@@ -108993,7 +108993,7 @@
         <v>0.5</v>
       </c>
       <c r="G10">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H10">
         <v>1.15234</v>
@@ -109048,7 +109048,7 @@
         <v>0.5</v>
       </c>
       <c r="G11">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H11">
         <v>1.15234</v>
@@ -109103,7 +109103,7 @@
         <v>0.5</v>
       </c>
       <c r="G12">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H12">
         <v>1.15234</v>
@@ -109158,7 +109158,7 @@
         <v>0.5</v>
       </c>
       <c r="G13">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H13">
         <v>1.15234</v>
@@ -109213,7 +109213,7 @@
         <v>0.5</v>
       </c>
       <c r="G14">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H14">
         <v>1.15234</v>
@@ -109268,7 +109268,7 @@
         <v>0.5</v>
       </c>
       <c r="G15">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H15">
         <v>1.15234</v>
@@ -109323,7 +109323,7 @@
         <v>0.5</v>
       </c>
       <c r="G16">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H16">
         <v>1.15234</v>
@@ -109378,7 +109378,7 @@
         <v>0.5</v>
       </c>
       <c r="G17">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H17">
         <v>1.15234</v>
@@ -109433,7 +109433,7 @@
         <v>0.5</v>
       </c>
       <c r="G18">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H18">
         <v>1.15234</v>
@@ -109488,7 +109488,7 @@
         <v>0.5</v>
       </c>
       <c r="G19">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H19">
         <v>1.15234</v>
@@ -109543,7 +109543,7 @@
         <v>0.5</v>
       </c>
       <c r="G20">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H20">
         <v>1.15234</v>
@@ -109598,7 +109598,7 @@
         <v>0.5</v>
       </c>
       <c r="G21">
-        <v>0.9590689999999999</v>
+        <v>0.959069</v>
       </c>
       <c r="H21">
         <v>1.15234</v>
@@ -109958,7 +109958,7 @@
         <v>0.9994</v>
       </c>
       <c r="G2">
-        <v>0.0005999999999999999</v>
+        <v>0.0006</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -110013,7 +110013,7 @@
         <v>0.0224</v>
       </c>
       <c r="G3">
-        <v>0.8675</v>
+        <v>0.8675000000000001</v>
       </c>
       <c r="H3">
         <v>0.1096</v>
@@ -110291,7 +110291,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.0005999999999999999</v>
+        <v>0.0006</v>
       </c>
       <c r="I8">
         <v>0.0195</v>
@@ -111499,7 +111499,7 @@
         <v>0.024</v>
       </c>
       <c r="X22">
-        <v>0.07199999999999999</v>
+        <v>0.072</v>
       </c>
       <c r="Y22">
         <v>0.152</v>
@@ -111636,7 +111636,7 @@
         <v>0.9999116</v>
       </c>
       <c r="G24">
-        <v>8.839999999999999e-05</v>
+        <v>8.839999999999999e-005</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -111742,13 +111742,13 @@
         <v>0.001538802</v>
       </c>
       <c r="K25">
-        <v>5.68e-06</v>
+        <v>5.68e-006</v>
       </c>
       <c r="L25">
-        <v>2.91e-09</v>
+        <v>2.91e-009</v>
       </c>
       <c r="M25">
-        <v>1.97e-13</v>
+        <v>1.97e-013</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -111821,7 +111821,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>7.36e-08</v>
+        <v>7.36e-008</v>
       </c>
       <c r="G26">
         <v>0.000825826</v>
@@ -111848,16 +111848,16 @@
         <v>0.001564913</v>
       </c>
       <c r="O26">
-        <v>3.62e-05</v>
+        <v>3.62e-005</v>
       </c>
       <c r="P26">
-        <v>3.01e-07</v>
+        <v>3.01e-007</v>
       </c>
       <c r="Q26">
-        <v>8.77e-10</v>
+        <v>8.77e-010</v>
       </c>
       <c r="R26">
-        <v>8.96e-13</v>
+        <v>8.96e-013</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -111915,13 +111915,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>4.36e-11</v>
+        <v>4.36e-011</v>
       </c>
       <c r="G27">
-        <v>8.27e-07</v>
+        <v>8.27e-007</v>
       </c>
       <c r="H27">
-        <v>3.67e-05</v>
+        <v>3.67e-005</v>
       </c>
       <c r="I27">
         <v>0.000812507</v>
@@ -111954,16 +111954,16 @@
         <v>0.000690862</v>
       </c>
       <c r="S27">
-        <v>3.23e-05</v>
+        <v>3.23e-005</v>
       </c>
       <c r="T27">
-        <v>2.74e-07</v>
+        <v>2.74e-007</v>
       </c>
       <c r="U27">
-        <v>2.3e-10</v>
+        <v>2.3e-010</v>
       </c>
       <c r="V27">
-        <v>4.39e-14</v>
+        <v>4.39e-014</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -112009,16 +112009,16 @@
         <v>5</v>
       </c>
       <c r="F28">
-        <v>3.07e-13</v>
+        <v>3.07e-013</v>
       </c>
       <c r="G28">
-        <v>4.26e-09</v>
+        <v>4.26e-009</v>
       </c>
       <c r="H28">
-        <v>2.16e-07</v>
+        <v>2.16e-007</v>
       </c>
       <c r="I28">
-        <v>6.55e-06</v>
+        <v>6.55e-006</v>
       </c>
       <c r="J28">
         <v>0.000118811</v>
@@ -112057,16 +112057,16 @@
         <v>0.00035841</v>
       </c>
       <c r="V28">
-        <v>5.47e-06</v>
+        <v>5.47e-006</v>
       </c>
       <c r="W28">
-        <v>3.01e-08</v>
+        <v>3.01e-008</v>
       </c>
       <c r="X28">
-        <v>5.92e-11</v>
+        <v>5.92e-011</v>
       </c>
       <c r="Y28">
-        <v>4.14e-14</v>
+        <v>4.14e-014</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -112103,22 +112103,22 @@
         <v>6</v>
       </c>
       <c r="F29">
-        <v>1.12e-14</v>
+        <v>1.12e-014</v>
       </c>
       <c r="G29">
-        <v>9.42e-11</v>
+        <v>9.42e-011</v>
       </c>
       <c r="H29">
-        <v>4.42e-09</v>
+        <v>4.42e-009</v>
       </c>
       <c r="I29">
-        <v>1.4e-07</v>
+        <v>1.4e-007</v>
       </c>
       <c r="J29">
-        <v>2.91e-06</v>
+        <v>2.91e-006</v>
       </c>
       <c r="K29">
-        <v>4.07e-05</v>
+        <v>4.07e-005</v>
       </c>
       <c r="L29">
         <v>0.000381616</v>
@@ -112157,13 +112157,13 @@
         <v>0.00057203</v>
       </c>
       <c r="X29">
-        <v>1.82e-05</v>
+        <v>1.82e-005</v>
       </c>
       <c r="Y29">
-        <v>2.7e-07</v>
+        <v>2.7e-007</v>
       </c>
       <c r="Z29">
-        <v>1.9e-09</v>
+        <v>1.9e-009</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -112197,25 +112197,25 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>1.19e-15</v>
+        <v>1.19e-015</v>
       </c>
       <c r="G30">
-        <v>6.13e-12</v>
+        <v>6.13e-012</v>
       </c>
       <c r="H30">
-        <v>2.49e-10</v>
+        <v>2.49e-010</v>
       </c>
       <c r="I30">
-        <v>7.33e-09</v>
+        <v>7.33e-009</v>
       </c>
       <c r="J30">
-        <v>1.54e-07</v>
+        <v>1.54e-007</v>
       </c>
       <c r="K30">
-        <v>2.31e-06</v>
+        <v>2.31e-006</v>
       </c>
       <c r="L30">
-        <v>2.49e-05</v>
+        <v>2.49e-005</v>
       </c>
       <c r="M30">
         <v>0.000194666</v>
@@ -112257,13 +112257,13 @@
         <v>0.00051173</v>
       </c>
       <c r="Z30">
-        <v>2.5e-05</v>
+        <v>2.5e-005</v>
       </c>
       <c r="AA30">
-        <v>1.87e-11</v>
+        <v>1.87e-011</v>
       </c>
       <c r="AB30">
-        <v>3.5e-14</v>
+        <v>3.5e-014</v>
       </c>
       <c r="AC30">
         <v>0</v>
@@ -112291,28 +112291,28 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <v>2.71e-16</v>
+        <v>2.71e-016</v>
       </c>
       <c r="G31">
-        <v>8.74e-13</v>
+        <v>8.74e-013</v>
       </c>
       <c r="H31">
-        <v>3e-11</v>
+        <v>3e-011</v>
       </c>
       <c r="I31">
-        <v>7.92e-10</v>
+        <v>7.92e-010</v>
       </c>
       <c r="J31">
-        <v>1.57e-08</v>
+        <v>1.57e-008</v>
       </c>
       <c r="K31">
-        <v>2.35e-07</v>
+        <v>2.35e-007</v>
       </c>
       <c r="L31">
-        <v>2.64e-06</v>
+        <v>2.64e-006</v>
       </c>
       <c r="M31">
-        <v>2.25e-05</v>
+        <v>2.25e-005</v>
       </c>
       <c r="N31">
         <v>0.00014589</v>
@@ -112354,13 +112354,13 @@
         <v>0.003249649</v>
       </c>
       <c r="AA31">
-        <v>8.52e-08</v>
+        <v>8.52e-008</v>
       </c>
       <c r="AB31">
-        <v>8.21e-10</v>
+        <v>8.21e-010</v>
       </c>
       <c r="AC31">
-        <v>4.23e-12</v>
+        <v>4.23e-012</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -112385,31 +112385,31 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>1.09e-16</v>
+        <v>1.09e-016</v>
       </c>
       <c r="G32">
-        <v>2.21e-13</v>
+        <v>2.21e-013</v>
       </c>
       <c r="H32">
-        <v>6.48e-12</v>
+        <v>6.48e-012</v>
       </c>
       <c r="I32">
-        <v>1.52e-10</v>
+        <v>1.52e-010</v>
       </c>
       <c r="J32">
-        <v>2.77e-09</v>
+        <v>2.77e-009</v>
       </c>
       <c r="K32">
-        <v>3.97e-08</v>
+        <v>3.97e-008</v>
       </c>
       <c r="L32">
-        <v>4.42e-07</v>
+        <v>4.42e-007</v>
       </c>
       <c r="M32">
-        <v>3.87e-06</v>
+        <v>3.87e-006</v>
       </c>
       <c r="N32">
-        <v>2.66e-05</v>
+        <v>2.66e-005</v>
       </c>
       <c r="O32">
         <v>0.00014379</v>
@@ -112448,16 +112448,16 @@
         <v>0.038845033</v>
       </c>
       <c r="AA32">
-        <v>1.47e-05</v>
+        <v>1.47e-005</v>
       </c>
       <c r="AB32">
-        <v>4.34e-07</v>
+        <v>4.34e-007</v>
       </c>
       <c r="AC32">
-        <v>7.499999999999999e-09</v>
+        <v>7.499999999999999e-009</v>
       </c>
       <c r="AD32">
-        <v>1.42e-11</v>
+        <v>1.42e-011</v>
       </c>
     </row>
     <row r="33">
@@ -112479,34 +112479,34 @@
         <v>10</v>
       </c>
       <c r="F33">
-        <v>5.82e-17</v>
+        <v>5.82e-017</v>
       </c>
       <c r="G33">
-        <v>9.02e-14</v>
+        <v>9.02e-014</v>
       </c>
       <c r="H33">
-        <v>2.27e-12</v>
+        <v>2.27e-012</v>
       </c>
       <c r="I33">
-        <v>4.71e-11</v>
+        <v>4.71e-011</v>
       </c>
       <c r="J33">
-        <v>7.89e-10</v>
+        <v>7.89e-010</v>
       </c>
       <c r="K33">
-        <v>1.06e-08</v>
+        <v>1.06e-008</v>
       </c>
       <c r="L33">
-        <v>1.14e-07</v>
+        <v>1.14e-007</v>
       </c>
       <c r="M33">
-        <v>9.86e-07</v>
+        <v>9.86e-007</v>
       </c>
       <c r="N33">
-        <v>6.91e-06</v>
+        <v>6.91e-006</v>
       </c>
       <c r="O33">
-        <v>3.9e-05</v>
+        <v>3.9e-005</v>
       </c>
       <c r="P33">
         <v>0.000178483</v>
@@ -112545,13 +112545,13 @@
         <v>0.000401548</v>
       </c>
       <c r="AB33">
-        <v>2.61e-05</v>
+        <v>2.61e-005</v>
       </c>
       <c r="AC33">
-        <v>1.08e-06</v>
+        <v>1.08e-006</v>
       </c>
       <c r="AD33">
-        <v>7.07e-09</v>
+        <v>7.07e-009</v>
       </c>
     </row>
     <row r="34">
@@ -112573,37 +112573,37 @@
         <v>11</v>
       </c>
       <c r="F34">
-        <v>6.86e-17</v>
+        <v>6.86e-017</v>
       </c>
       <c r="G34">
-        <v>5.58e-14</v>
+        <v>5.58e-014</v>
       </c>
       <c r="H34">
-        <v>1.22e-12</v>
+        <v>1.22e-012</v>
       </c>
       <c r="I34">
-        <v>2.26e-11</v>
+        <v>2.26e-011</v>
       </c>
       <c r="J34">
-        <v>3.45e-10</v>
+        <v>3.45e-010</v>
       </c>
       <c r="K34">
-        <v>4.32e-09</v>
+        <v>4.32e-009</v>
       </c>
       <c r="L34">
-        <v>4.44e-08</v>
+        <v>4.44e-008</v>
       </c>
       <c r="M34">
-        <v>3.73e-07</v>
+        <v>3.73e-007</v>
       </c>
       <c r="N34">
-        <v>2.6e-06</v>
+        <v>2.6e-006</v>
       </c>
       <c r="O34">
-        <v>1.49e-05</v>
+        <v>1.49e-005</v>
       </c>
       <c r="P34">
-        <v>7.02e-05</v>
+        <v>7.02e-005</v>
       </c>
       <c r="Q34">
         <v>0.000274962</v>
@@ -112621,7 +112621,7 @@
         <v>0.035171443</v>
       </c>
       <c r="V34">
-        <v>0.07568430199999999</v>
+        <v>0.075684302</v>
       </c>
       <c r="W34">
         <v>0.140531213</v>
@@ -112642,10 +112642,10 @@
         <v>0.000448222</v>
       </c>
       <c r="AC34">
-        <v>3.51e-05</v>
+        <v>3.51e-005</v>
       </c>
       <c r="AD34">
-        <v>5.77e-07</v>
+        <v>5.77e-007</v>
       </c>
     </row>
     <row r="35">
@@ -112667,37 +112667,37 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <v>8.84e-17</v>
+        <v>8.84e-017</v>
       </c>
       <c r="G35">
-        <v>4.8e-14</v>
+        <v>4.8e-014</v>
       </c>
       <c r="H35">
-        <v>9.21e-13</v>
+        <v>9.21e-013</v>
       </c>
       <c r="I35">
-        <v>1.54e-11</v>
+        <v>1.54e-011</v>
       </c>
       <c r="J35">
-        <v>2.14e-10</v>
+        <v>2.14e-010</v>
       </c>
       <c r="K35">
-        <v>2.49e-09</v>
+        <v>2.49e-009</v>
       </c>
       <c r="L35">
-        <v>2.42e-08</v>
+        <v>2.42e-008</v>
       </c>
       <c r="M35">
-        <v>1.97e-07</v>
+        <v>1.97e-007</v>
       </c>
       <c r="N35">
-        <v>1.34e-06</v>
+        <v>1.34e-006</v>
       </c>
       <c r="O35">
-        <v>7.63e-06</v>
+        <v>7.63e-006</v>
       </c>
       <c r="P35">
-        <v>3.65e-05</v>
+        <v>3.65e-005</v>
       </c>
       <c r="Q35">
         <v>0.000146448</v>
@@ -112739,7 +112739,7 @@
         <v>0.000454477</v>
       </c>
       <c r="AD35">
-        <v>1.5e-05</v>
+        <v>1.5e-005</v>
       </c>
     </row>
     <row r="36">
@@ -112761,40 +112761,40 @@
         <v>13</v>
       </c>
       <c r="F36">
-        <v>1.16e-16</v>
+        <v>1.16e-016</v>
       </c>
       <c r="G36">
-        <v>5.07e-14</v>
+        <v>5.07e-014</v>
       </c>
       <c r="H36">
-        <v>8.66e-13</v>
+        <v>8.660000000000001e-013</v>
       </c>
       <c r="I36">
-        <v>1.31e-11</v>
+        <v>1.31e-011</v>
       </c>
       <c r="J36">
-        <v>1.67e-10</v>
+        <v>1.67e-010</v>
       </c>
       <c r="K36">
-        <v>1.81e-09</v>
+        <v>1.81e-009</v>
       </c>
       <c r="L36">
-        <v>1.66e-08</v>
+        <v>1.66e-008</v>
       </c>
       <c r="M36">
-        <v>1.3e-07</v>
+        <v>1.3e-007</v>
       </c>
       <c r="N36">
-        <v>8.53e-07</v>
+        <v>8.53e-007</v>
       </c>
       <c r="O36">
-        <v>4.8e-06</v>
+        <v>4.8e-006</v>
       </c>
       <c r="P36">
-        <v>2.29e-05</v>
+        <v>2.29e-005</v>
       </c>
       <c r="Q36">
-        <v>9.26e-05</v>
+        <v>9.26e-005</v>
       </c>
       <c r="R36">
         <v>0.000320283</v>
@@ -112855,40 +112855,40 @@
         <v>14</v>
       </c>
       <c r="F37">
-        <v>1.45e-16</v>
+        <v>1.45e-016</v>
       </c>
       <c r="G37">
-        <v>5.819999999999999e-14</v>
+        <v>5.819999999999999e-014</v>
       </c>
       <c r="H37">
-        <v>8.93e-13</v>
+        <v>8.93e-013</v>
       </c>
       <c r="I37">
-        <v>1.23e-11</v>
+        <v>1.23e-011</v>
       </c>
       <c r="J37">
-        <v>1.45e-10</v>
+        <v>1.45e-010</v>
       </c>
       <c r="K37">
-        <v>1.47e-09</v>
+        <v>1.47e-009</v>
       </c>
       <c r="L37">
-        <v>1.27e-08</v>
+        <v>1.27e-008</v>
       </c>
       <c r="M37">
-        <v>9.49e-08</v>
+        <v>9.49e-008</v>
       </c>
       <c r="N37">
-        <v>6.03e-07</v>
+        <v>6.03e-007</v>
       </c>
       <c r="O37">
-        <v>3.31e-06</v>
+        <v>3.31e-006</v>
       </c>
       <c r="P37">
-        <v>1.56e-05</v>
+        <v>1.56e-005</v>
       </c>
       <c r="Q37">
-        <v>6.3e-05</v>
+        <v>6.3e-005</v>
       </c>
       <c r="R37">
         <v>0.000219607</v>
@@ -112949,40 +112949,40 @@
         <v>15</v>
       </c>
       <c r="F38">
-        <v>1.61e-16</v>
+        <v>1.61e-016</v>
       </c>
       <c r="G38">
-        <v>6.71e-14</v>
+        <v>6.71e-014</v>
       </c>
       <c r="H38">
-        <v>9.300000000000001e-13</v>
+        <v>9.300000000000001e-013</v>
       </c>
       <c r="I38">
-        <v>1.17e-11</v>
+        <v>1.17e-011</v>
       </c>
       <c r="J38">
-        <v>1.29e-10</v>
+        <v>1.29e-010</v>
       </c>
       <c r="K38">
-        <v>1.22e-09</v>
+        <v>1.22e-009</v>
       </c>
       <c r="L38">
-        <v>9.980000000000001e-09</v>
+        <v>9.980000000000001e-009</v>
       </c>
       <c r="M38">
-        <v>7.08e-08</v>
+        <v>7.08e-008</v>
       </c>
       <c r="N38">
-        <v>4.35e-07</v>
+        <v>4.35e-007</v>
       </c>
       <c r="O38">
-        <v>2.32e-06</v>
+        <v>2.32e-006</v>
       </c>
       <c r="P38">
-        <v>1.07e-05</v>
+        <v>1.07e-005</v>
       </c>
       <c r="Q38">
-        <v>4.3e-05</v>
+        <v>4.3e-005</v>
       </c>
       <c r="R38">
         <v>0.000149742</v>
@@ -113043,40 +113043,40 @@
         <v>16</v>
       </c>
       <c r="F39">
-        <v>3.23e-16</v>
+        <v>3.23e-016</v>
       </c>
       <c r="G39">
-        <v>7.59e-14</v>
+        <v>7.59e-014</v>
       </c>
       <c r="H39">
-        <v>9.590000000000001e-13</v>
+        <v>9.590000000000001e-013</v>
       </c>
       <c r="I39">
-        <v>1.12e-11</v>
+        <v>1.12e-011</v>
       </c>
       <c r="J39">
-        <v>1.14e-10</v>
+        <v>1.14e-010</v>
       </c>
       <c r="K39">
-        <v>1.02e-09</v>
+        <v>1.02e-009</v>
       </c>
       <c r="L39">
-        <v>7.87e-09</v>
+        <v>7.87e-009</v>
       </c>
       <c r="M39">
-        <v>5.33e-08</v>
+        <v>5.33e-008</v>
       </c>
       <c r="N39">
-        <v>3.15e-07</v>
+        <v>3.15e-007</v>
       </c>
       <c r="O39">
-        <v>1.63e-06</v>
+        <v>1.63e-006</v>
       </c>
       <c r="P39">
-        <v>7.37e-06</v>
+        <v>7.37e-006</v>
       </c>
       <c r="Q39">
-        <v>2.91e-05</v>
+        <v>2.91e-005</v>
       </c>
       <c r="R39">
         <v>0.000100803</v>
@@ -113137,43 +113137,43 @@
         <v>17</v>
       </c>
       <c r="F40">
-        <v>3.04e-16</v>
+        <v>3.04e-016</v>
       </c>
       <c r="G40">
-        <v>8.65e-14</v>
+        <v>8.65e-014</v>
       </c>
       <c r="H40">
-        <v>1e-12</v>
+        <v>1e-012</v>
       </c>
       <c r="I40">
-        <v>1.09e-11</v>
+        <v>1.09e-011</v>
       </c>
       <c r="J40">
-        <v>1.04e-10</v>
+        <v>1.04e-010</v>
       </c>
       <c r="K40">
-        <v>8.67e-10</v>
+        <v>8.67e-010</v>
       </c>
       <c r="L40">
-        <v>6.38e-09</v>
+        <v>6.38e-009</v>
       </c>
       <c r="M40">
-        <v>4.13e-08</v>
+        <v>4.13e-008</v>
       </c>
       <c r="N40">
-        <v>2.35e-07</v>
+        <v>2.35e-007</v>
       </c>
       <c r="O40">
-        <v>1.17e-06</v>
+        <v>1.17e-006</v>
       </c>
       <c r="P40">
-        <v>5.21e-06</v>
+        <v>5.21e-006</v>
       </c>
       <c r="Q40">
-        <v>2.01e-05</v>
+        <v>2.01e-005</v>
       </c>
       <c r="R40">
-        <v>6.889999999999999e-05</v>
+        <v>6.889999999999999e-005</v>
       </c>
       <c r="S40">
         <v>0.000309476</v>
@@ -113231,43 +113231,43 @@
         <v>18</v>
       </c>
       <c r="F41">
-        <v>4.2e-16</v>
+        <v>4.2e-016</v>
       </c>
       <c r="G41">
-        <v>1.01e-13</v>
+        <v>1.01e-013</v>
       </c>
       <c r="H41">
-        <v>1.08e-12</v>
+        <v>1.08e-012</v>
       </c>
       <c r="I41">
-        <v>1.09e-11</v>
+        <v>1.09e-011</v>
       </c>
       <c r="J41">
-        <v>9.83e-11</v>
+        <v>9.83e-011</v>
       </c>
       <c r="K41">
-        <v>7.76e-10</v>
+        <v>7.76e-010</v>
       </c>
       <c r="L41">
-        <v>5.43e-09</v>
+        <v>5.43e-009</v>
       </c>
       <c r="M41">
-        <v>3.36e-08</v>
+        <v>3.36e-008</v>
       </c>
       <c r="N41">
-        <v>1.84e-07</v>
+        <v>1.84e-007</v>
       </c>
       <c r="O41">
-        <v>8.92e-07</v>
+        <v>8.92e-007</v>
       </c>
       <c r="P41">
-        <v>3.84e-06</v>
+        <v>3.84e-006</v>
       </c>
       <c r="Q41">
-        <v>1.46e-05</v>
+        <v>1.46e-005</v>
       </c>
       <c r="R41">
-        <v>4.92e-05</v>
+        <v>4.92e-005</v>
       </c>
       <c r="S41">
         <v>0.000218751</v>
@@ -113325,43 +113325,43 @@
         <v>19</v>
       </c>
       <c r="F42">
-        <v>6.44e-16</v>
+        <v>6.44e-016</v>
       </c>
       <c r="G42">
-        <v>1.23e-13</v>
+        <v>1.23e-013</v>
       </c>
       <c r="H42">
-        <v>1.22e-12</v>
+        <v>1.22e-012</v>
       </c>
       <c r="I42">
-        <v>1.16e-11</v>
+        <v>1.16e-011</v>
       </c>
       <c r="J42">
-        <v>9.78e-11</v>
+        <v>9.78e-011</v>
       </c>
       <c r="K42">
-        <v>7.340000000000001e-10</v>
+        <v>7.340000000000001e-010</v>
       </c>
       <c r="L42">
-        <v>4.9e-09</v>
+        <v>4.9e-009</v>
       </c>
       <c r="M42">
-        <v>2.9e-08</v>
+        <v>2.9e-008</v>
       </c>
       <c r="N42">
-        <v>1.53e-07</v>
+        <v>1.53e-007</v>
       </c>
       <c r="O42">
-        <v>7.180000000000001e-07</v>
+        <v>7.180000000000001e-007</v>
       </c>
       <c r="P42">
-        <v>3.01e-06</v>
+        <v>3.01e-006</v>
       </c>
       <c r="Q42">
-        <v>1.12e-05</v>
+        <v>1.12e-005</v>
       </c>
       <c r="R42">
-        <v>3.71e-05</v>
+        <v>3.71e-005</v>
       </c>
       <c r="S42">
         <v>0.00016277</v>
@@ -113419,43 +113419,43 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <v>9.549999999999999e-16</v>
+        <v>9.549999999999999e-016</v>
       </c>
       <c r="G43">
-        <v>1.56e-13</v>
+        <v>1.56e-013</v>
       </c>
       <c r="H43">
-        <v>1.44e-12</v>
+        <v>1.44e-012</v>
       </c>
       <c r="I43">
-        <v>1.29e-11</v>
+        <v>1.29e-011</v>
       </c>
       <c r="J43">
-        <v>1.03e-10</v>
+        <v>1.03e-010</v>
       </c>
       <c r="K43">
-        <v>7.37e-10</v>
+        <v>7.37e-010</v>
       </c>
       <c r="L43">
-        <v>4.67e-09</v>
+        <v>4.67e-009</v>
       </c>
       <c r="M43">
-        <v>2.66e-08</v>
+        <v>2.66e-008</v>
       </c>
       <c r="N43">
-        <v>1.35e-07</v>
+        <v>1.35e-007</v>
       </c>
       <c r="O43">
-        <v>6.16e-07</v>
+        <v>6.16e-007</v>
       </c>
       <c r="P43">
-        <v>2.49e-06</v>
+        <v>2.49e-006</v>
       </c>
       <c r="Q43">
-        <v>9.07e-06</v>
+        <v>9.07e-006</v>
       </c>
       <c r="R43">
-        <v>2.96e-05</v>
+        <v>2.96e-005</v>
       </c>
       <c r="S43">
         <v>0.000127693</v>
@@ -113513,43 +113513,43 @@
         <v>21</v>
       </c>
       <c r="F44">
-        <v>1.45e-15</v>
+        <v>1.45e-015</v>
       </c>
       <c r="G44">
-        <v>2.05e-13</v>
+        <v>2.05e-013</v>
       </c>
       <c r="H44">
-        <v>1.76e-12</v>
+        <v>1.76e-012</v>
       </c>
       <c r="I44">
-        <v>1.49e-11</v>
+        <v>1.49e-011</v>
       </c>
       <c r="J44">
-        <v>1.13e-10</v>
+        <v>1.13e-010</v>
       </c>
       <c r="K44">
-        <v>7.67e-10</v>
+        <v>7.67e-010</v>
       </c>
       <c r="L44">
-        <v>4.67e-09</v>
+        <v>4.67e-009</v>
       </c>
       <c r="M44">
-        <v>2.56e-08</v>
+        <v>2.56e-008</v>
       </c>
       <c r="N44">
-        <v>1.25e-07</v>
+        <v>1.25e-007</v>
       </c>
       <c r="O44">
-        <v>5.51e-07</v>
+        <v>5.51e-007</v>
       </c>
       <c r="P44">
-        <v>2.18e-06</v>
+        <v>2.18e-006</v>
       </c>
       <c r="Q44">
-        <v>7.77e-06</v>
+        <v>7.77e-006</v>
       </c>
       <c r="R44">
-        <v>2.48e-05</v>
+        <v>2.48e-005</v>
       </c>
       <c r="S44">
         <v>0.000105218</v>

</xml_diff>

<commit_message>
added, PFMC HCR for multi-species mode
Used depletion based HCRs rather than SPR based
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -688,7 +688,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 0 = no, 1 = penalized deviates given sel_sd_prior, 2 = random effect, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity.</t>
+          <t>Wether a time-varying selectivity should be estimated for logistic, double logistic selectivity,  descending logistic , or non-parametric (Selectivity = 5). 0 = no, 1 = penalized deviates given sel_sd_prior, 3 = time blocks with no penality, 4 = random walk following Dorn, 5 = random walk on ascending portion of double logistic only. If selectivity is set to type = 2 (non-parametric) this value will be the 1st penalty on selectivity. "random_sel" treats random deviates and random walk parameters as random effects.</t>
         </is>
       </c>
     </row>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 2 = random effect, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y</t>
+          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
         </is>
       </c>
     </row>
@@ -4561,7 +4561,7 @@
         <v>0.6820565</v>
       </c>
       <c r="L2">
-        <v>0.8397522</v>
+        <v>0.8397521999999999</v>
       </c>
       <c r="M2">
         <v>0.9915121</v>
@@ -4616,7 +4616,7 @@
         <v>0.6820565</v>
       </c>
       <c r="L3">
-        <v>0.8397522</v>
+        <v>0.8397521999999999</v>
       </c>
       <c r="M3">
         <v>0.9915121</v>
@@ -4723,7 +4723,7 @@
         <v>0.428903178</v>
       </c>
       <c r="K5">
-        <v>0.6686019680000001</v>
+        <v>0.668601968</v>
       </c>
       <c r="L5">
         <v>1.004004033</v>
@@ -4781,7 +4781,7 @@
         <v>0.575604904</v>
       </c>
       <c r="L6">
-        <v>0.7394161540000001</v>
+        <v>0.739416154</v>
       </c>
       <c r="M6">
         <v>1.068567323</v>
@@ -4998,7 +4998,7 @@
         <v>0.434168571</v>
       </c>
       <c r="K10">
-        <v>0.529975582</v>
+        <v>0.5299755819999999</v>
       </c>
       <c r="L10">
         <v>0.703008924</v>
@@ -5010,7 +5010,7 @@
         <v>0.888000873</v>
       </c>
       <c r="O10">
-        <v>0.985676724</v>
+        <v>0.9856767239999999</v>
       </c>
       <c r="P10">
         <v>1.193588801</v>
@@ -5111,7 +5111,7 @@
         <v>0.5338019980000001</v>
       </c>
       <c r="L12">
-        <v>0.6280371420000001</v>
+        <v>0.628037142</v>
       </c>
       <c r="M12">
         <v>0.6833034650000001</v>
@@ -5160,7 +5160,7 @@
         <v>0.376630035</v>
       </c>
       <c r="J13">
-        <v>0.5029989620000001</v>
+        <v>0.502998962</v>
       </c>
       <c r="K13">
         <v>0.573065432</v>
@@ -5496,10 +5496,10 @@
         <v>0.596229054</v>
       </c>
       <c r="L19">
-        <v>0.7330465510000001</v>
+        <v>0.733046551</v>
       </c>
       <c r="M19">
-        <v>0.8150067210000001</v>
+        <v>0.815006721</v>
       </c>
       <c r="N19">
         <v>0.971352934</v>
@@ -5771,7 +5771,7 @@
         <v>0.617633322</v>
       </c>
       <c r="L24">
-        <v>0.7737766350000001</v>
+        <v>0.773776635</v>
       </c>
       <c r="M24">
         <v>0.820595866</v>
@@ -5887,7 +5887,7 @@
         <v>0.8321758970000001</v>
       </c>
       <c r="N26">
-        <v>0.8844928560000001</v>
+        <v>0.884492856</v>
       </c>
       <c r="O26">
         <v>0.961303653</v>
@@ -5933,7 +5933,7 @@
         <v>0.554839651</v>
       </c>
       <c r="K27">
-        <v>0.6796000290000001</v>
+        <v>0.679600029</v>
       </c>
       <c r="L27">
         <v>0.76519576</v>
@@ -5988,7 +5988,7 @@
         <v>0.516896768</v>
       </c>
       <c r="K28">
-        <v>0.6087939650000001</v>
+        <v>0.608793965</v>
       </c>
       <c r="L28">
         <v>0.702835715</v>
@@ -6040,7 +6040,7 @@
         <v>0.363608103</v>
       </c>
       <c r="J29">
-        <v>0.51750097</v>
+        <v>0.5175009699999999</v>
       </c>
       <c r="K29">
         <v>0.607355501</v>
@@ -6211,7 +6211,7 @@
         <v>0.669170666</v>
       </c>
       <c r="L32">
-        <v>0.884058069</v>
+        <v>0.8840580689999999</v>
       </c>
       <c r="M32">
         <v>1.009000445</v>
@@ -6263,13 +6263,13 @@
         <v>0.549263493</v>
       </c>
       <c r="K33">
-        <v>0.679259738</v>
+        <v>0.6792597379999999</v>
       </c>
       <c r="L33">
         <v>0.893518288</v>
       </c>
       <c r="M33">
-        <v>0.982130899</v>
+        <v>0.9821308989999999</v>
       </c>
       <c r="N33">
         <v>1.032776434</v>
@@ -6370,10 +6370,10 @@
         <v>0.358158972</v>
       </c>
       <c r="J35">
-        <v>0.5333061220000001</v>
+        <v>0.533306122</v>
       </c>
       <c r="K35">
-        <v>0.67074633</v>
+        <v>0.6707463299999999</v>
       </c>
       <c r="L35">
         <v>0.807299177</v>
@@ -6599,7 +6599,7 @@
         <v>0.698561299</v>
       </c>
       <c r="M39">
-        <v>0.7821615870000001</v>
+        <v>0.782161587</v>
       </c>
       <c r="N39">
         <v>0.844000541</v>
@@ -6651,7 +6651,7 @@
         <v>0.668715635</v>
       </c>
       <c r="L40">
-        <v>0.759104151</v>
+        <v>0.7591041509999999</v>
       </c>
       <c r="M40">
         <v>0.844249481</v>
@@ -6694,7 +6694,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H41">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I41">
         <v>1.344427</v>
@@ -6749,7 +6749,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H42">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I42">
         <v>1.344427</v>
@@ -6914,7 +6914,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H45">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I45">
         <v>1.344427</v>
@@ -7079,7 +7079,7 @@
         <v>0.2308979</v>
       </c>
       <c r="H48">
-        <v>0.6446690000000001</v>
+        <v>0.644669</v>
       </c>
       <c r="I48">
         <v>1.282862</v>
@@ -7158,7 +7158,7 @@
         <v>8.579815999999999</v>
       </c>
       <c r="P49">
-        <v>9.848017000000001</v>
+        <v>9.848017</v>
       </c>
       <c r="Q49">
         <v>11.71415</v>
@@ -7409,7 +7409,7 @@
         <v>0.2320311</v>
       </c>
       <c r="H54">
-        <v>0.6493005</v>
+        <v>0.6493004999999999</v>
       </c>
       <c r="I54">
         <v>1.294171</v>
@@ -7574,7 +7574,7 @@
         <v>0.2320815</v>
       </c>
       <c r="H57">
-        <v>0.649507</v>
+        <v>0.6495069999999999</v>
       </c>
       <c r="I57">
         <v>1.294676</v>
@@ -8475,7 +8475,7 @@
         <v>8.062624</v>
       </c>
       <c r="O73">
-        <v>9.553563000000001</v>
+        <v>9.553563</v>
       </c>
       <c r="P73">
         <v>11.0069</v>
@@ -8509,7 +8509,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H74">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I74">
         <v>1.344427</v>
@@ -8564,7 +8564,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H75">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I75">
         <v>1.344427</v>
@@ -8619,7 +8619,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H76">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I76">
         <v>1.344427</v>
@@ -8674,7 +8674,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H77">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I77">
         <v>1.344427</v>
@@ -8729,7 +8729,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H78">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I78">
         <v>1.344427</v>
@@ -8784,7 +8784,7 @@
         <v>0.2370012</v>
       </c>
       <c r="H79">
-        <v>0.6697768</v>
+        <v>0.6697767999999999</v>
       </c>
       <c r="I79">
         <v>1.344427</v>
@@ -9173,7 +9173,7 @@
         <v>0.3249681</v>
       </c>
       <c r="J84">
-        <v>0.5305165</v>
+        <v>0.5305164999999999</v>
       </c>
       <c r="K84">
         <v>0.775014</v>
@@ -9328,7 +9328,7 @@
         <v>0.01321826</v>
       </c>
       <c r="G86">
-        <v>0.06417197</v>
+        <v>0.06417196999999999</v>
       </c>
       <c r="H86">
         <v>0.1684496</v>
@@ -9586,7 +9586,7 @@
         <v>0.5425362</v>
       </c>
       <c r="K89">
-        <v>0.7951763</v>
+        <v>0.7951762999999999</v>
       </c>
       <c r="L89">
         <v>1.079442</v>
@@ -9668,7 +9668,7 @@
         <v>0.5271326</v>
       </c>
       <c r="K90">
-        <v>0.7693524000000001</v>
+        <v>0.7693524</v>
       </c>
       <c r="L90">
         <v>1.040711</v>
@@ -10476,7 +10476,7 @@
         <v>0.01307071</v>
       </c>
       <c r="G100">
-        <v>0.06518729</v>
+        <v>0.06518728999999999</v>
       </c>
       <c r="H100">
         <v>0.1741539</v>
@@ -10895,7 +10895,7 @@
         <v>0.334899</v>
       </c>
       <c r="J105">
-        <v>0.5512337000000001</v>
+        <v>0.5512337</v>
       </c>
       <c r="K105">
         <v>0.8114404</v>
@@ -12201,7 +12201,7 @@
         <v>0.52816</v>
       </c>
       <c r="H3">
-        <v>0.746145</v>
+        <v>0.7461449999999999</v>
       </c>
       <c r="I3">
         <v>0.8852950000000001</v>
@@ -12242,7 +12242,7 @@
         <v>0.837937385</v>
       </c>
       <c r="H4">
-        <v>0.973474801</v>
+        <v>0.9734748009999999</v>
       </c>
       <c r="I4">
         <v>0.995967742</v>
@@ -12556,7 +12556,7 @@
         <v>0.93703</v>
       </c>
       <c r="U4">
-        <v>0.9453200000000001</v>
+        <v>0.94532</v>
       </c>
       <c r="V4">
         <v>0.95257</v>
@@ -13633,7 +13633,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G2">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H2">
         <v>77.2967</v>
@@ -13680,7 +13680,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G3">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H3">
         <v>77.2967</v>
@@ -13736,7 +13736,7 @@
         <v>78.2727</v>
       </c>
       <c r="J4">
-        <v>77.44920000000001</v>
+        <v>77.4492</v>
       </c>
       <c r="K4">
         <v>76.95440000000001</v>
@@ -13830,7 +13830,7 @@
         <v>69.9829</v>
       </c>
       <c r="J6">
-        <v>69.54980000000001</v>
+        <v>69.5498</v>
       </c>
       <c r="K6">
         <v>69.3948</v>
@@ -13886,7 +13886,7 @@
         <v>78.7354</v>
       </c>
       <c r="M7">
-        <v>79.06350000000001</v>
+        <v>79.0635</v>
       </c>
       <c r="N7">
         <v>79.617</v>
@@ -13959,7 +13959,7 @@
         <v>72.80289999999999</v>
       </c>
       <c r="F9">
-        <v>74.73730000000001</v>
+        <v>74.7373</v>
       </c>
       <c r="G9">
         <v>77.08110000000001</v>
@@ -13983,7 +13983,7 @@
         <v>81.12990000000001</v>
       </c>
       <c r="N9">
-        <v>82.08490000000001</v>
+        <v>82.0849</v>
       </c>
       <c r="O9">
         <v>83.8866</v>
@@ -14015,7 +14015,7 @@
         <v>79.38720000000001</v>
       </c>
       <c r="I10">
-        <v>78.41880000000001</v>
+        <v>78.4188</v>
       </c>
       <c r="J10">
         <v>77.9448</v>
@@ -14030,7 +14030,7 @@
         <v>78.1143</v>
       </c>
       <c r="N10">
-        <v>78.5174</v>
+        <v>78.51739999999999</v>
       </c>
       <c r="O10">
         <v>79.5454</v>
@@ -14056,7 +14056,7 @@
         <v>73.8518</v>
       </c>
       <c r="G11">
-        <v>76.118</v>
+        <v>76.11799999999999</v>
       </c>
       <c r="H11">
         <v>77.6767</v>
@@ -14065,7 +14065,7 @@
         <v>77.4243</v>
       </c>
       <c r="J11">
-        <v>77.64740000000001</v>
+        <v>77.6474</v>
       </c>
       <c r="K11">
         <v>78.16070000000001</v>
@@ -14262,7 +14262,7 @@
         <v>80.4949</v>
       </c>
       <c r="M15">
-        <v>81.5114</v>
+        <v>81.51139999999999</v>
       </c>
       <c r="N15">
         <v>82.59139999999999</v>
@@ -14312,7 +14312,7 @@
         <v>78.8276</v>
       </c>
       <c r="N16">
-        <v>79.38970000000001</v>
+        <v>79.3897</v>
       </c>
       <c r="O16">
         <v>80.6387</v>
@@ -14335,7 +14335,7 @@
         <v>74.57680000000001</v>
       </c>
       <c r="F17">
-        <v>76.6852</v>
+        <v>76.68519999999999</v>
       </c>
       <c r="G17">
         <v>79.24379999999999</v>
@@ -14470,7 +14470,7 @@
         <v>1997</v>
       </c>
       <c r="D20">
-        <v>65.96890000000001</v>
+        <v>65.9689</v>
       </c>
       <c r="E20">
         <v>66.9862</v>
@@ -14564,7 +14564,7 @@
         <v>1999</v>
       </c>
       <c r="D22">
-        <v>69.74</v>
+        <v>69.73999999999999</v>
       </c>
       <c r="E22">
         <v>71.24590000000001</v>
@@ -14588,7 +14588,7 @@
         <v>81.81359999999999</v>
       </c>
       <c r="L22">
-        <v>83.1043</v>
+        <v>83.10429999999999</v>
       </c>
       <c r="M22">
         <v>84.4646</v>
@@ -14670,7 +14670,7 @@
         <v>77.4251</v>
       </c>
       <c r="H24">
-        <v>79.0007</v>
+        <v>79.00069999999999</v>
       </c>
       <c r="I24">
         <v>78.27419999999999</v>
@@ -14717,7 +14717,7 @@
         <v>72.58969999999999</v>
       </c>
       <c r="H25">
-        <v>73.34390000000001</v>
+        <v>73.3439</v>
       </c>
       <c r="I25">
         <v>72.46639999999999</v>
@@ -14764,7 +14764,7 @@
         <v>78.33499999999999</v>
       </c>
       <c r="H26">
-        <v>78.4031</v>
+        <v>78.40309999999999</v>
       </c>
       <c r="I26">
         <v>77.1631</v>
@@ -14785,7 +14785,7 @@
         <v>76.13160000000001</v>
       </c>
       <c r="O26">
-        <v>76.9703</v>
+        <v>76.97029999999999</v>
       </c>
     </row>
     <row r="27">
@@ -14993,7 +14993,7 @@
         <v>69.634</v>
       </c>
       <c r="F31">
-        <v>71.85930000000001</v>
+        <v>71.8593</v>
       </c>
       <c r="G31">
         <v>74.5994</v>
@@ -15005,7 +15005,7 @@
         <v>76.62350000000001</v>
       </c>
       <c r="J31">
-        <v>77.45520000000001</v>
+        <v>77.4552</v>
       </c>
       <c r="K31">
         <v>78.58410000000001</v>
@@ -15014,7 +15014,7 @@
         <v>79.896</v>
       </c>
       <c r="M31">
-        <v>81.3209</v>
+        <v>81.32089999999999</v>
       </c>
       <c r="N31">
         <v>82.8138</v>
@@ -15055,13 +15055,13 @@
         <v>78.92570000000001</v>
       </c>
       <c r="K32">
-        <v>80.18250000000001</v>
+        <v>80.1825</v>
       </c>
       <c r="L32">
         <v>81.66549999999999</v>
       </c>
       <c r="M32">
-        <v>83.31350000000001</v>
+        <v>83.3135</v>
       </c>
       <c r="N32">
         <v>85.0881</v>
@@ -15096,10 +15096,10 @@
         <v>77.06610000000001</v>
       </c>
       <c r="I33">
-        <v>77.47960000000001</v>
+        <v>77.4796</v>
       </c>
       <c r="J33">
-        <v>78.44150000000001</v>
+        <v>78.4415</v>
       </c>
       <c r="K33">
         <v>79.7681</v>
@@ -15184,7 +15184,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G35">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H35">
         <v>77.2967</v>
@@ -15231,7 +15231,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G36">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H36">
         <v>77.2967</v>
@@ -15278,7 +15278,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G37">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H37">
         <v>77.2967</v>
@@ -15325,7 +15325,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G38">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H38">
         <v>77.2967</v>
@@ -15372,7 +15372,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G39">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H39">
         <v>77.2967</v>
@@ -15419,7 +15419,7 @@
         <v>73.88549999999999</v>
       </c>
       <c r="G40">
-        <v>75.987</v>
+        <v>75.98699999999999</v>
       </c>
       <c r="H40">
         <v>77.2967</v>
@@ -17903,7 +17903,7 @@
         <v>78.5538</v>
       </c>
       <c r="K88">
-        <v>76.237</v>
+        <v>76.23699999999999</v>
       </c>
       <c r="L88">
         <v>77.447</v>
@@ -18048,7 +18048,7 @@
         <v>100.1932</v>
       </c>
       <c r="J90">
-        <v>94.45690000000001</v>
+        <v>94.4569</v>
       </c>
       <c r="K90">
         <v>92.7714</v>
@@ -18575,7 +18575,7 @@
         <v>71.59690000000001</v>
       </c>
       <c r="M97">
-        <v>75.2203</v>
+        <v>75.22029999999999</v>
       </c>
       <c r="N97">
         <v>82.2286</v>
@@ -18705,7 +18705,7 @@
         <v>99.7668</v>
       </c>
       <c r="G99">
-        <v>94.90810000000001</v>
+        <v>94.9081</v>
       </c>
       <c r="H99">
         <v>88.51600000000001</v>
@@ -19072,7 +19072,7 @@
         <v>101.9125</v>
       </c>
       <c r="F104">
-        <v>98.2096</v>
+        <v>98.20959999999999</v>
       </c>
       <c r="G104">
         <v>93.05410000000001</v>
@@ -29821,7 +29821,7 @@
         <v>20</v>
       </c>
       <c r="I332">
-        <v>4.61e-005</v>
+        <v>4.61e-05</v>
       </c>
     </row>
     <row r="333">
@@ -36259,7 +36259,7 @@
         <v>20</v>
       </c>
       <c r="I554">
-        <v>0.06434812</v>
+        <v>0.06434811999999999</v>
       </c>
     </row>
     <row r="555">
@@ -36665,7 +36665,7 @@
         <v>20</v>
       </c>
       <c r="I568">
-        <v>0.008836657</v>
+        <v>0.008836656999999999</v>
       </c>
     </row>
     <row r="569">
@@ -39507,7 +39507,7 @@
         <v>20</v>
       </c>
       <c r="I666">
-        <v>0.07907031000000001</v>
+        <v>0.07907031</v>
       </c>
     </row>
     <row r="667">
@@ -40058,7 +40058,7 @@
         <v>20</v>
       </c>
       <c r="I685">
-        <v>0.008198974</v>
+        <v>0.008198973999999999</v>
       </c>
     </row>
     <row r="686">
@@ -47308,7 +47308,7 @@
         <v>20</v>
       </c>
       <c r="I935">
-        <v>6e-005</v>
+        <v>6e-05</v>
       </c>
     </row>
     <row r="936">
@@ -51571,7 +51571,7 @@
         <v>20</v>
       </c>
       <c r="I1082">
-        <v>0.06884557</v>
+        <v>0.06884556999999999</v>
       </c>
     </row>
     <row r="1083">
@@ -54355,7 +54355,7 @@
         <v>20</v>
       </c>
       <c r="I1178">
-        <v>0.5632434</v>
+        <v>0.5632433999999999</v>
       </c>
     </row>
     <row r="1179">
@@ -80143,7 +80143,7 @@
         <v>6550414.87</v>
       </c>
       <c r="I9">
-        <v>0.09211958435883833</v>
+        <v>0.09211958435883832</v>
       </c>
     </row>
     <row r="10">
@@ -80515,7 +80515,7 @@
         <v>4196853.9</v>
       </c>
       <c r="I21">
-        <v>0.08086190826834754</v>
+        <v>0.08086190826834753</v>
       </c>
     </row>
     <row r="22">
@@ -81166,7 +81166,7 @@
         <v>1189234.46</v>
       </c>
       <c r="I42">
-        <v>0.05849707555563898</v>
+        <v>0.05849707555563897</v>
       </c>
     </row>
     <row r="43">
@@ -81504,7 +81504,7 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>627150.5500000001</v>
+        <v>627150.55</v>
       </c>
       <c r="I53">
         <v>0.10876005261786</v>
@@ -81969,7 +81969,7 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>896401.07</v>
+        <v>896401.0699999999</v>
       </c>
       <c r="I68">
         <v>0.1117503487285052</v>
@@ -82220,7 +82220,7 @@
         <v>160396</v>
       </c>
       <c r="I76">
-        <v>0.142979205564983</v>
+        <v>0.1429792055649829</v>
       </c>
     </row>
     <row r="77">
@@ -82437,7 +82437,7 @@
         <v>298788.7</v>
       </c>
       <c r="I83">
-        <v>0.1261991044529836</v>
+        <v>0.1261991044529835</v>
       </c>
     </row>
     <row r="84">
@@ -82961,7 +82961,7 @@
         <v>1</v>
       </c>
       <c r="H100">
-        <v>530126.8000000001</v>
+        <v>530126.8</v>
       </c>
       <c r="I100">
         <v>0.08653101992209057</v>
@@ -83736,7 +83736,7 @@
         <v>1</v>
       </c>
       <c r="H125">
-        <v>923.843366</v>
+        <v>923.8433659999999</v>
       </c>
       <c r="I125">
         <v>0.2</v>
@@ -97937,7 +97937,7 @@
         <v>266522.0805</v>
       </c>
       <c r="S121">
-        <v>837292.7706000001</v>
+        <v>837292.7706</v>
       </c>
       <c r="T121">
         <v>426717.2484</v>
@@ -98440,7 +98440,7 @@
         <v>828292.9068999999</v>
       </c>
       <c r="P129">
-        <v>997103.8895000001</v>
+        <v>997103.8895</v>
       </c>
       <c r="Q129">
         <v>168652.0961</v>
@@ -98559,7 +98559,7 @@
         <v>1049901.396</v>
       </c>
       <c r="M131">
-        <v>598741.5990000001</v>
+        <v>598741.599</v>
       </c>
       <c r="N131">
         <v>1069230.855</v>
@@ -98629,7 +98629,7 @@
         <v>932167.5946</v>
       </c>
       <c r="O132">
-        <v>783151.0896</v>
+        <v>783151.0895999999</v>
       </c>
       <c r="P132">
         <v>2564040.645</v>
@@ -99141,7 +99141,7 @@
         <v>1134406.589</v>
       </c>
       <c r="O140">
-        <v>889090.1554000001</v>
+        <v>889090.1554</v>
       </c>
       <c r="P140">
         <v>618182.879</v>
@@ -99720,7 +99720,7 @@
         <v>861.2938481</v>
       </c>
       <c r="P149">
-        <v>774.2097028</v>
+        <v>774.2097027999999</v>
       </c>
       <c r="Q149">
         <v>918.7848015</v>
@@ -103295,7 +103295,7 @@
         <v>58696.237</v>
       </c>
       <c r="S184">
-        <v>76350.88000000001</v>
+        <v>76350.88</v>
       </c>
       <c r="T184">
         <v>127063.244</v>
@@ -107517,7 +107517,7 @@
         <v>293.253466</v>
       </c>
       <c r="O227">
-        <v>69.328887</v>
+        <v>69.32888699999999</v>
       </c>
       <c r="P227">
         <v>66.771672</v>
@@ -108026,7 +108026,7 @@
         <v>669.189032</v>
       </c>
       <c r="N235">
-        <v>588.8287128</v>
+        <v>588.8287127999999</v>
       </c>
       <c r="O235">
         <v>305.6689523</v>
@@ -108334,7 +108334,7 @@
         <v>4438.331215</v>
       </c>
       <c r="J240">
-        <v>8614.89223</v>
+        <v>8614.892229999999</v>
       </c>
       <c r="K240">
         <v>941.2751066</v>
@@ -108352,7 +108352,7 @@
         <v>316.9225225</v>
       </c>
       <c r="P240">
-        <v>66.89265565</v>
+        <v>66.89265564999999</v>
       </c>
       <c r="Q240">
         <v>21.47372183</v>
@@ -108608,7 +108608,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H3">
         <v>1.15234</v>
@@ -108663,7 +108663,7 @@
         <v>0.5</v>
       </c>
       <c r="G4">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H4">
         <v>1.15234</v>
@@ -108718,7 +108718,7 @@
         <v>0.5</v>
       </c>
       <c r="G5">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H5">
         <v>1.15234</v>
@@ -108773,7 +108773,7 @@
         <v>0.5</v>
       </c>
       <c r="G6">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H6">
         <v>1.15234</v>
@@ -108828,7 +108828,7 @@
         <v>0.5</v>
       </c>
       <c r="G7">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H7">
         <v>1.15234</v>
@@ -108883,7 +108883,7 @@
         <v>0.5</v>
       </c>
       <c r="G8">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H8">
         <v>1.15234</v>
@@ -108938,7 +108938,7 @@
         <v>0.5</v>
       </c>
       <c r="G9">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H9">
         <v>1.15234</v>
@@ -108993,7 +108993,7 @@
         <v>0.5</v>
       </c>
       <c r="G10">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H10">
         <v>1.15234</v>
@@ -109048,7 +109048,7 @@
         <v>0.5</v>
       </c>
       <c r="G11">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H11">
         <v>1.15234</v>
@@ -109103,7 +109103,7 @@
         <v>0.5</v>
       </c>
       <c r="G12">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H12">
         <v>1.15234</v>
@@ -109158,7 +109158,7 @@
         <v>0.5</v>
       </c>
       <c r="G13">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H13">
         <v>1.15234</v>
@@ -109213,7 +109213,7 @@
         <v>0.5</v>
       </c>
       <c r="G14">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H14">
         <v>1.15234</v>
@@ -109268,7 +109268,7 @@
         <v>0.5</v>
       </c>
       <c r="G15">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H15">
         <v>1.15234</v>
@@ -109323,7 +109323,7 @@
         <v>0.5</v>
       </c>
       <c r="G16">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H16">
         <v>1.15234</v>
@@ -109378,7 +109378,7 @@
         <v>0.5</v>
       </c>
       <c r="G17">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H17">
         <v>1.15234</v>
@@ -109433,7 +109433,7 @@
         <v>0.5</v>
       </c>
       <c r="G18">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H18">
         <v>1.15234</v>
@@ -109488,7 +109488,7 @@
         <v>0.5</v>
       </c>
       <c r="G19">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H19">
         <v>1.15234</v>
@@ -109543,7 +109543,7 @@
         <v>0.5</v>
       </c>
       <c r="G20">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H20">
         <v>1.15234</v>
@@ -109598,7 +109598,7 @@
         <v>0.5</v>
       </c>
       <c r="G21">
-        <v>0.959069</v>
+        <v>0.9590689999999999</v>
       </c>
       <c r="H21">
         <v>1.15234</v>
@@ -109958,7 +109958,7 @@
         <v>0.9994</v>
       </c>
       <c r="G2">
-        <v>0.0006</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -110013,7 +110013,7 @@
         <v>0.0224</v>
       </c>
       <c r="G3">
-        <v>0.8675000000000001</v>
+        <v>0.8675</v>
       </c>
       <c r="H3">
         <v>0.1096</v>
@@ -110291,7 +110291,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.0006</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="I8">
         <v>0.0195</v>
@@ -111499,7 +111499,7 @@
         <v>0.024</v>
       </c>
       <c r="X22">
-        <v>0.072</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="Y22">
         <v>0.152</v>
@@ -111636,7 +111636,7 @@
         <v>0.9999116</v>
       </c>
       <c r="G24">
-        <v>8.839999999999999e-005</v>
+        <v>8.839999999999999e-05</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -111742,13 +111742,13 @@
         <v>0.001538802</v>
       </c>
       <c r="K25">
-        <v>5.68e-006</v>
+        <v>5.68e-06</v>
       </c>
       <c r="L25">
-        <v>2.91e-009</v>
+        <v>2.91e-09</v>
       </c>
       <c r="M25">
-        <v>1.97e-013</v>
+        <v>1.97e-13</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -111821,7 +111821,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>7.36e-008</v>
+        <v>7.36e-08</v>
       </c>
       <c r="G26">
         <v>0.000825826</v>
@@ -111848,16 +111848,16 @@
         <v>0.001564913</v>
       </c>
       <c r="O26">
-        <v>3.62e-005</v>
+        <v>3.62e-05</v>
       </c>
       <c r="P26">
-        <v>3.01e-007</v>
+        <v>3.01e-07</v>
       </c>
       <c r="Q26">
-        <v>8.77e-010</v>
+        <v>8.77e-10</v>
       </c>
       <c r="R26">
-        <v>8.96e-013</v>
+        <v>8.96e-13</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -111915,13 +111915,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>4.36e-011</v>
+        <v>4.36e-11</v>
       </c>
       <c r="G27">
-        <v>8.27e-007</v>
+        <v>8.27e-07</v>
       </c>
       <c r="H27">
-        <v>3.67e-005</v>
+        <v>3.67e-05</v>
       </c>
       <c r="I27">
         <v>0.000812507</v>
@@ -111954,16 +111954,16 @@
         <v>0.000690862</v>
       </c>
       <c r="S27">
-        <v>3.23e-005</v>
+        <v>3.23e-05</v>
       </c>
       <c r="T27">
-        <v>2.74e-007</v>
+        <v>2.74e-07</v>
       </c>
       <c r="U27">
-        <v>2.3e-010</v>
+        <v>2.3e-10</v>
       </c>
       <c r="V27">
-        <v>4.39e-014</v>
+        <v>4.39e-14</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -112009,16 +112009,16 @@
         <v>5</v>
       </c>
       <c r="F28">
-        <v>3.07e-013</v>
+        <v>3.07e-13</v>
       </c>
       <c r="G28">
-        <v>4.26e-009</v>
+        <v>4.26e-09</v>
       </c>
       <c r="H28">
-        <v>2.16e-007</v>
+        <v>2.16e-07</v>
       </c>
       <c r="I28">
-        <v>6.55e-006</v>
+        <v>6.55e-06</v>
       </c>
       <c r="J28">
         <v>0.000118811</v>
@@ -112057,16 +112057,16 @@
         <v>0.00035841</v>
       </c>
       <c r="V28">
-        <v>5.47e-006</v>
+        <v>5.47e-06</v>
       </c>
       <c r="W28">
-        <v>3.01e-008</v>
+        <v>3.01e-08</v>
       </c>
       <c r="X28">
-        <v>5.92e-011</v>
+        <v>5.92e-11</v>
       </c>
       <c r="Y28">
-        <v>4.14e-014</v>
+        <v>4.14e-14</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -112103,22 +112103,22 @@
         <v>6</v>
       </c>
       <c r="F29">
-        <v>1.12e-014</v>
+        <v>1.12e-14</v>
       </c>
       <c r="G29">
-        <v>9.42e-011</v>
+        <v>9.42e-11</v>
       </c>
       <c r="H29">
-        <v>4.42e-009</v>
+        <v>4.42e-09</v>
       </c>
       <c r="I29">
-        <v>1.4e-007</v>
+        <v>1.4e-07</v>
       </c>
       <c r="J29">
-        <v>2.91e-006</v>
+        <v>2.91e-06</v>
       </c>
       <c r="K29">
-        <v>4.07e-005</v>
+        <v>4.07e-05</v>
       </c>
       <c r="L29">
         <v>0.000381616</v>
@@ -112157,13 +112157,13 @@
         <v>0.00057203</v>
       </c>
       <c r="X29">
-        <v>1.82e-005</v>
+        <v>1.82e-05</v>
       </c>
       <c r="Y29">
-        <v>2.7e-007</v>
+        <v>2.7e-07</v>
       </c>
       <c r="Z29">
-        <v>1.9e-009</v>
+        <v>1.9e-09</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -112197,25 +112197,25 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>1.19e-015</v>
+        <v>1.19e-15</v>
       </c>
       <c r="G30">
-        <v>6.13e-012</v>
+        <v>6.13e-12</v>
       </c>
       <c r="H30">
-        <v>2.49e-010</v>
+        <v>2.49e-10</v>
       </c>
       <c r="I30">
-        <v>7.33e-009</v>
+        <v>7.33e-09</v>
       </c>
       <c r="J30">
-        <v>1.54e-007</v>
+        <v>1.54e-07</v>
       </c>
       <c r="K30">
-        <v>2.31e-006</v>
+        <v>2.31e-06</v>
       </c>
       <c r="L30">
-        <v>2.49e-005</v>
+        <v>2.49e-05</v>
       </c>
       <c r="M30">
         <v>0.000194666</v>
@@ -112257,13 +112257,13 @@
         <v>0.00051173</v>
       </c>
       <c r="Z30">
-        <v>2.5e-005</v>
+        <v>2.5e-05</v>
       </c>
       <c r="AA30">
-        <v>1.87e-011</v>
+        <v>1.87e-11</v>
       </c>
       <c r="AB30">
-        <v>3.5e-014</v>
+        <v>3.5e-14</v>
       </c>
       <c r="AC30">
         <v>0</v>
@@ -112291,28 +112291,28 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <v>2.71e-016</v>
+        <v>2.71e-16</v>
       </c>
       <c r="G31">
-        <v>8.74e-013</v>
+        <v>8.74e-13</v>
       </c>
       <c r="H31">
-        <v>3e-011</v>
+        <v>3e-11</v>
       </c>
       <c r="I31">
-        <v>7.92e-010</v>
+        <v>7.92e-10</v>
       </c>
       <c r="J31">
-        <v>1.57e-008</v>
+        <v>1.57e-08</v>
       </c>
       <c r="K31">
-        <v>2.35e-007</v>
+        <v>2.35e-07</v>
       </c>
       <c r="L31">
-        <v>2.64e-006</v>
+        <v>2.64e-06</v>
       </c>
       <c r="M31">
-        <v>2.25e-005</v>
+        <v>2.25e-05</v>
       </c>
       <c r="N31">
         <v>0.00014589</v>
@@ -112354,13 +112354,13 @@
         <v>0.003249649</v>
       </c>
       <c r="AA31">
-        <v>8.52e-008</v>
+        <v>8.52e-08</v>
       </c>
       <c r="AB31">
-        <v>8.21e-010</v>
+        <v>8.21e-10</v>
       </c>
       <c r="AC31">
-        <v>4.23e-012</v>
+        <v>4.23e-12</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -112385,31 +112385,31 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>1.09e-016</v>
+        <v>1.09e-16</v>
       </c>
       <c r="G32">
-        <v>2.21e-013</v>
+        <v>2.21e-13</v>
       </c>
       <c r="H32">
-        <v>6.48e-012</v>
+        <v>6.48e-12</v>
       </c>
       <c r="I32">
-        <v>1.52e-010</v>
+        <v>1.52e-10</v>
       </c>
       <c r="J32">
-        <v>2.77e-009</v>
+        <v>2.77e-09</v>
       </c>
       <c r="K32">
-        <v>3.97e-008</v>
+        <v>3.97e-08</v>
       </c>
       <c r="L32">
-        <v>4.42e-007</v>
+        <v>4.42e-07</v>
       </c>
       <c r="M32">
-        <v>3.87e-006</v>
+        <v>3.87e-06</v>
       </c>
       <c r="N32">
-        <v>2.66e-005</v>
+        <v>2.66e-05</v>
       </c>
       <c r="O32">
         <v>0.00014379</v>
@@ -112448,16 +112448,16 @@
         <v>0.038845033</v>
       </c>
       <c r="AA32">
-        <v>1.47e-005</v>
+        <v>1.47e-05</v>
       </c>
       <c r="AB32">
-        <v>4.34e-007</v>
+        <v>4.34e-07</v>
       </c>
       <c r="AC32">
-        <v>7.499999999999999e-009</v>
+        <v>7.499999999999999e-09</v>
       </c>
       <c r="AD32">
-        <v>1.42e-011</v>
+        <v>1.42e-11</v>
       </c>
     </row>
     <row r="33">
@@ -112479,34 +112479,34 @@
         <v>10</v>
       </c>
       <c r="F33">
-        <v>5.82e-017</v>
+        <v>5.82e-17</v>
       </c>
       <c r="G33">
-        <v>9.02e-014</v>
+        <v>9.02e-14</v>
       </c>
       <c r="H33">
-        <v>2.27e-012</v>
+        <v>2.27e-12</v>
       </c>
       <c r="I33">
-        <v>4.71e-011</v>
+        <v>4.71e-11</v>
       </c>
       <c r="J33">
-        <v>7.89e-010</v>
+        <v>7.89e-10</v>
       </c>
       <c r="K33">
-        <v>1.06e-008</v>
+        <v>1.06e-08</v>
       </c>
       <c r="L33">
-        <v>1.14e-007</v>
+        <v>1.14e-07</v>
       </c>
       <c r="M33">
-        <v>9.86e-007</v>
+        <v>9.86e-07</v>
       </c>
       <c r="N33">
-        <v>6.91e-006</v>
+        <v>6.91e-06</v>
       </c>
       <c r="O33">
-        <v>3.9e-005</v>
+        <v>3.9e-05</v>
       </c>
       <c r="P33">
         <v>0.000178483</v>
@@ -112545,13 +112545,13 @@
         <v>0.000401548</v>
       </c>
       <c r="AB33">
-        <v>2.61e-005</v>
+        <v>2.61e-05</v>
       </c>
       <c r="AC33">
-        <v>1.08e-006</v>
+        <v>1.08e-06</v>
       </c>
       <c r="AD33">
-        <v>7.07e-009</v>
+        <v>7.07e-09</v>
       </c>
     </row>
     <row r="34">
@@ -112573,37 +112573,37 @@
         <v>11</v>
       </c>
       <c r="F34">
-        <v>6.86e-017</v>
+        <v>6.86e-17</v>
       </c>
       <c r="G34">
-        <v>5.58e-014</v>
+        <v>5.58e-14</v>
       </c>
       <c r="H34">
-        <v>1.22e-012</v>
+        <v>1.22e-12</v>
       </c>
       <c r="I34">
-        <v>2.26e-011</v>
+        <v>2.26e-11</v>
       </c>
       <c r="J34">
-        <v>3.45e-010</v>
+        <v>3.45e-10</v>
       </c>
       <c r="K34">
-        <v>4.32e-009</v>
+        <v>4.32e-09</v>
       </c>
       <c r="L34">
-        <v>4.44e-008</v>
+        <v>4.44e-08</v>
       </c>
       <c r="M34">
-        <v>3.73e-007</v>
+        <v>3.73e-07</v>
       </c>
       <c r="N34">
-        <v>2.6e-006</v>
+        <v>2.6e-06</v>
       </c>
       <c r="O34">
-        <v>1.49e-005</v>
+        <v>1.49e-05</v>
       </c>
       <c r="P34">
-        <v>7.02e-005</v>
+        <v>7.02e-05</v>
       </c>
       <c r="Q34">
         <v>0.000274962</v>
@@ -112621,7 +112621,7 @@
         <v>0.035171443</v>
       </c>
       <c r="V34">
-        <v>0.075684302</v>
+        <v>0.07568430199999999</v>
       </c>
       <c r="W34">
         <v>0.140531213</v>
@@ -112642,10 +112642,10 @@
         <v>0.000448222</v>
       </c>
       <c r="AC34">
-        <v>3.51e-005</v>
+        <v>3.51e-05</v>
       </c>
       <c r="AD34">
-        <v>5.77e-007</v>
+        <v>5.77e-07</v>
       </c>
     </row>
     <row r="35">
@@ -112667,37 +112667,37 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <v>8.84e-017</v>
+        <v>8.84e-17</v>
       </c>
       <c r="G35">
-        <v>4.8e-014</v>
+        <v>4.8e-14</v>
       </c>
       <c r="H35">
-        <v>9.21e-013</v>
+        <v>9.21e-13</v>
       </c>
       <c r="I35">
-        <v>1.54e-011</v>
+        <v>1.54e-11</v>
       </c>
       <c r="J35">
-        <v>2.14e-010</v>
+        <v>2.14e-10</v>
       </c>
       <c r="K35">
-        <v>2.49e-009</v>
+        <v>2.49e-09</v>
       </c>
       <c r="L35">
-        <v>2.42e-008</v>
+        <v>2.42e-08</v>
       </c>
       <c r="M35">
-        <v>1.97e-007</v>
+        <v>1.97e-07</v>
       </c>
       <c r="N35">
-        <v>1.34e-006</v>
+        <v>1.34e-06</v>
       </c>
       <c r="O35">
-        <v>7.63e-006</v>
+        <v>7.63e-06</v>
       </c>
       <c r="P35">
-        <v>3.65e-005</v>
+        <v>3.65e-05</v>
       </c>
       <c r="Q35">
         <v>0.000146448</v>
@@ -112739,7 +112739,7 @@
         <v>0.000454477</v>
       </c>
       <c r="AD35">
-        <v>1.5e-005</v>
+        <v>1.5e-05</v>
       </c>
     </row>
     <row r="36">
@@ -112761,40 +112761,40 @@
         <v>13</v>
       </c>
       <c r="F36">
-        <v>1.16e-016</v>
+        <v>1.16e-16</v>
       </c>
       <c r="G36">
-        <v>5.07e-014</v>
+        <v>5.07e-14</v>
       </c>
       <c r="H36">
-        <v>8.660000000000001e-013</v>
+        <v>8.66e-13</v>
       </c>
       <c r="I36">
-        <v>1.31e-011</v>
+        <v>1.31e-11</v>
       </c>
       <c r="J36">
-        <v>1.67e-010</v>
+        <v>1.67e-10</v>
       </c>
       <c r="K36">
-        <v>1.81e-009</v>
+        <v>1.81e-09</v>
       </c>
       <c r="L36">
-        <v>1.66e-008</v>
+        <v>1.66e-08</v>
       </c>
       <c r="M36">
-        <v>1.3e-007</v>
+        <v>1.3e-07</v>
       </c>
       <c r="N36">
-        <v>8.53e-007</v>
+        <v>8.53e-07</v>
       </c>
       <c r="O36">
-        <v>4.8e-006</v>
+        <v>4.8e-06</v>
       </c>
       <c r="P36">
-        <v>2.29e-005</v>
+        <v>2.29e-05</v>
       </c>
       <c r="Q36">
-        <v>9.26e-005</v>
+        <v>9.26e-05</v>
       </c>
       <c r="R36">
         <v>0.000320283</v>
@@ -112855,40 +112855,40 @@
         <v>14</v>
       </c>
       <c r="F37">
-        <v>1.45e-016</v>
+        <v>1.45e-16</v>
       </c>
       <c r="G37">
-        <v>5.819999999999999e-014</v>
+        <v>5.819999999999999e-14</v>
       </c>
       <c r="H37">
-        <v>8.93e-013</v>
+        <v>8.93e-13</v>
       </c>
       <c r="I37">
-        <v>1.23e-011</v>
+        <v>1.23e-11</v>
       </c>
       <c r="J37">
-        <v>1.45e-010</v>
+        <v>1.45e-10</v>
       </c>
       <c r="K37">
-        <v>1.47e-009</v>
+        <v>1.47e-09</v>
       </c>
       <c r="L37">
-        <v>1.27e-008</v>
+        <v>1.27e-08</v>
       </c>
       <c r="M37">
-        <v>9.49e-008</v>
+        <v>9.49e-08</v>
       </c>
       <c r="N37">
-        <v>6.03e-007</v>
+        <v>6.03e-07</v>
       </c>
       <c r="O37">
-        <v>3.31e-006</v>
+        <v>3.31e-06</v>
       </c>
       <c r="P37">
-        <v>1.56e-005</v>
+        <v>1.56e-05</v>
       </c>
       <c r="Q37">
-        <v>6.3e-005</v>
+        <v>6.3e-05</v>
       </c>
       <c r="R37">
         <v>0.000219607</v>
@@ -112949,40 +112949,40 @@
         <v>15</v>
       </c>
       <c r="F38">
-        <v>1.61e-016</v>
+        <v>1.61e-16</v>
       </c>
       <c r="G38">
-        <v>6.71e-014</v>
+        <v>6.71e-14</v>
       </c>
       <c r="H38">
-        <v>9.300000000000001e-013</v>
+        <v>9.300000000000001e-13</v>
       </c>
       <c r="I38">
-        <v>1.17e-011</v>
+        <v>1.17e-11</v>
       </c>
       <c r="J38">
-        <v>1.29e-010</v>
+        <v>1.29e-10</v>
       </c>
       <c r="K38">
-        <v>1.22e-009</v>
+        <v>1.22e-09</v>
       </c>
       <c r="L38">
-        <v>9.980000000000001e-009</v>
+        <v>9.980000000000001e-09</v>
       </c>
       <c r="M38">
-        <v>7.08e-008</v>
+        <v>7.08e-08</v>
       </c>
       <c r="N38">
-        <v>4.35e-007</v>
+        <v>4.35e-07</v>
       </c>
       <c r="O38">
-        <v>2.32e-006</v>
+        <v>2.32e-06</v>
       </c>
       <c r="P38">
-        <v>1.07e-005</v>
+        <v>1.07e-05</v>
       </c>
       <c r="Q38">
-        <v>4.3e-005</v>
+        <v>4.3e-05</v>
       </c>
       <c r="R38">
         <v>0.000149742</v>
@@ -113043,40 +113043,40 @@
         <v>16</v>
       </c>
       <c r="F39">
-        <v>3.23e-016</v>
+        <v>3.23e-16</v>
       </c>
       <c r="G39">
-        <v>7.59e-014</v>
+        <v>7.59e-14</v>
       </c>
       <c r="H39">
-        <v>9.590000000000001e-013</v>
+        <v>9.590000000000001e-13</v>
       </c>
       <c r="I39">
-        <v>1.12e-011</v>
+        <v>1.12e-11</v>
       </c>
       <c r="J39">
-        <v>1.14e-010</v>
+        <v>1.14e-10</v>
       </c>
       <c r="K39">
-        <v>1.02e-009</v>
+        <v>1.02e-09</v>
       </c>
       <c r="L39">
-        <v>7.87e-009</v>
+        <v>7.87e-09</v>
       </c>
       <c r="M39">
-        <v>5.33e-008</v>
+        <v>5.33e-08</v>
       </c>
       <c r="N39">
-        <v>3.15e-007</v>
+        <v>3.15e-07</v>
       </c>
       <c r="O39">
-        <v>1.63e-006</v>
+        <v>1.63e-06</v>
       </c>
       <c r="P39">
-        <v>7.37e-006</v>
+        <v>7.37e-06</v>
       </c>
       <c r="Q39">
-        <v>2.91e-005</v>
+        <v>2.91e-05</v>
       </c>
       <c r="R39">
         <v>0.000100803</v>
@@ -113137,43 +113137,43 @@
         <v>17</v>
       </c>
       <c r="F40">
-        <v>3.04e-016</v>
+        <v>3.04e-16</v>
       </c>
       <c r="G40">
-        <v>8.65e-014</v>
+        <v>8.65e-14</v>
       </c>
       <c r="H40">
-        <v>1e-012</v>
+        <v>1e-12</v>
       </c>
       <c r="I40">
-        <v>1.09e-011</v>
+        <v>1.09e-11</v>
       </c>
       <c r="J40">
-        <v>1.04e-010</v>
+        <v>1.04e-10</v>
       </c>
       <c r="K40">
-        <v>8.67e-010</v>
+        <v>8.67e-10</v>
       </c>
       <c r="L40">
-        <v>6.38e-009</v>
+        <v>6.38e-09</v>
       </c>
       <c r="M40">
-        <v>4.13e-008</v>
+        <v>4.13e-08</v>
       </c>
       <c r="N40">
-        <v>2.35e-007</v>
+        <v>2.35e-07</v>
       </c>
       <c r="O40">
-        <v>1.17e-006</v>
+        <v>1.17e-06</v>
       </c>
       <c r="P40">
-        <v>5.21e-006</v>
+        <v>5.21e-06</v>
       </c>
       <c r="Q40">
-        <v>2.01e-005</v>
+        <v>2.01e-05</v>
       </c>
       <c r="R40">
-        <v>6.889999999999999e-005</v>
+        <v>6.889999999999999e-05</v>
       </c>
       <c r="S40">
         <v>0.000309476</v>
@@ -113231,43 +113231,43 @@
         <v>18</v>
       </c>
       <c r="F41">
-        <v>4.2e-016</v>
+        <v>4.2e-16</v>
       </c>
       <c r="G41">
-        <v>1.01e-013</v>
+        <v>1.01e-13</v>
       </c>
       <c r="H41">
-        <v>1.08e-012</v>
+        <v>1.08e-12</v>
       </c>
       <c r="I41">
-        <v>1.09e-011</v>
+        <v>1.09e-11</v>
       </c>
       <c r="J41">
-        <v>9.83e-011</v>
+        <v>9.83e-11</v>
       </c>
       <c r="K41">
-        <v>7.76e-010</v>
+        <v>7.76e-10</v>
       </c>
       <c r="L41">
-        <v>5.43e-009</v>
+        <v>5.43e-09</v>
       </c>
       <c r="M41">
-        <v>3.36e-008</v>
+        <v>3.36e-08</v>
       </c>
       <c r="N41">
-        <v>1.84e-007</v>
+        <v>1.84e-07</v>
       </c>
       <c r="O41">
-        <v>8.92e-007</v>
+        <v>8.92e-07</v>
       </c>
       <c r="P41">
-        <v>3.84e-006</v>
+        <v>3.84e-06</v>
       </c>
       <c r="Q41">
-        <v>1.46e-005</v>
+        <v>1.46e-05</v>
       </c>
       <c r="R41">
-        <v>4.92e-005</v>
+        <v>4.92e-05</v>
       </c>
       <c r="S41">
         <v>0.000218751</v>
@@ -113325,43 +113325,43 @@
         <v>19</v>
       </c>
       <c r="F42">
-        <v>6.44e-016</v>
+        <v>6.44e-16</v>
       </c>
       <c r="G42">
-        <v>1.23e-013</v>
+        <v>1.23e-13</v>
       </c>
       <c r="H42">
-        <v>1.22e-012</v>
+        <v>1.22e-12</v>
       </c>
       <c r="I42">
-        <v>1.16e-011</v>
+        <v>1.16e-11</v>
       </c>
       <c r="J42">
-        <v>9.78e-011</v>
+        <v>9.78e-11</v>
       </c>
       <c r="K42">
-        <v>7.340000000000001e-010</v>
+        <v>7.340000000000001e-10</v>
       </c>
       <c r="L42">
-        <v>4.9e-009</v>
+        <v>4.9e-09</v>
       </c>
       <c r="M42">
-        <v>2.9e-008</v>
+        <v>2.9e-08</v>
       </c>
       <c r="N42">
-        <v>1.53e-007</v>
+        <v>1.53e-07</v>
       </c>
       <c r="O42">
-        <v>7.180000000000001e-007</v>
+        <v>7.180000000000001e-07</v>
       </c>
       <c r="P42">
-        <v>3.01e-006</v>
+        <v>3.01e-06</v>
       </c>
       <c r="Q42">
-        <v>1.12e-005</v>
+        <v>1.12e-05</v>
       </c>
       <c r="R42">
-        <v>3.71e-005</v>
+        <v>3.71e-05</v>
       </c>
       <c r="S42">
         <v>0.00016277</v>
@@ -113419,43 +113419,43 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <v>9.549999999999999e-016</v>
+        <v>9.549999999999999e-16</v>
       </c>
       <c r="G43">
-        <v>1.56e-013</v>
+        <v>1.56e-13</v>
       </c>
       <c r="H43">
-        <v>1.44e-012</v>
+        <v>1.44e-12</v>
       </c>
       <c r="I43">
-        <v>1.29e-011</v>
+        <v>1.29e-11</v>
       </c>
       <c r="J43">
-        <v>1.03e-010</v>
+        <v>1.03e-10</v>
       </c>
       <c r="K43">
-        <v>7.37e-010</v>
+        <v>7.37e-10</v>
       </c>
       <c r="L43">
-        <v>4.67e-009</v>
+        <v>4.67e-09</v>
       </c>
       <c r="M43">
-        <v>2.66e-008</v>
+        <v>2.66e-08</v>
       </c>
       <c r="N43">
-        <v>1.35e-007</v>
+        <v>1.35e-07</v>
       </c>
       <c r="O43">
-        <v>6.16e-007</v>
+        <v>6.16e-07</v>
       </c>
       <c r="P43">
-        <v>2.49e-006</v>
+        <v>2.49e-06</v>
       </c>
       <c r="Q43">
-        <v>9.07e-006</v>
+        <v>9.07e-06</v>
       </c>
       <c r="R43">
-        <v>2.96e-005</v>
+        <v>2.96e-05</v>
       </c>
       <c r="S43">
         <v>0.000127693</v>
@@ -113513,43 +113513,43 @@
         <v>21</v>
       </c>
       <c r="F44">
-        <v>1.45e-015</v>
+        <v>1.45e-15</v>
       </c>
       <c r="G44">
-        <v>2.05e-013</v>
+        <v>2.05e-13</v>
       </c>
       <c r="H44">
-        <v>1.76e-012</v>
+        <v>1.76e-12</v>
       </c>
       <c r="I44">
-        <v>1.49e-011</v>
+        <v>1.49e-11</v>
       </c>
       <c r="J44">
-        <v>1.13e-010</v>
+        <v>1.13e-10</v>
       </c>
       <c r="K44">
-        <v>7.67e-010</v>
+        <v>7.67e-10</v>
       </c>
       <c r="L44">
-        <v>4.67e-009</v>
+        <v>4.67e-09</v>
       </c>
       <c r="M44">
-        <v>2.56e-008</v>
+        <v>2.56e-08</v>
       </c>
       <c r="N44">
-        <v>1.25e-007</v>
+        <v>1.25e-07</v>
       </c>
       <c r="O44">
-        <v>5.51e-007</v>
+        <v>5.51e-07</v>
       </c>
       <c r="P44">
-        <v>2.18e-006</v>
+        <v>2.18e-06</v>
       </c>
       <c r="Q44">
-        <v>7.77e-006</v>
+        <v>7.77e-06</v>
       </c>
       <c r="R44">
-        <v>2.48e-005</v>
+        <v>2.48e-05</v>
       </c>
       <c r="S44">
         <v>0.000105218</v>

</xml_diff>

<commit_message>
moved to TMBad and updated MSE function for speed
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -29821,7 +29821,7 @@
         <v>20</v>
       </c>
       <c r="I332">
-        <v>4.61e-05</v>
+        <v>4.61E-05</v>
       </c>
     </row>
     <row r="333">
@@ -47308,7 +47308,7 @@
         <v>20</v>
       </c>
       <c r="I935">
-        <v>6e-05</v>
+        <v>6E-05</v>
       </c>
     </row>
     <row r="936">
@@ -79022,7 +79022,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>2060</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="6">
@@ -111636,7 +111636,7 @@
         <v>0.9999116</v>
       </c>
       <c r="G24">
-        <v>8.839999999999999e-05</v>
+        <v>8.839999999999999E-05</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -111742,13 +111742,13 @@
         <v>0.001538802</v>
       </c>
       <c r="K25">
-        <v>5.68e-06</v>
+        <v>5.68E-06</v>
       </c>
       <c r="L25">
-        <v>2.91e-09</v>
+        <v>2.91E-09</v>
       </c>
       <c r="M25">
-        <v>1.97e-13</v>
+        <v>1.97E-13</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -111821,7 +111821,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>7.36e-08</v>
+        <v>7.36E-08</v>
       </c>
       <c r="G26">
         <v>0.000825826</v>
@@ -111848,16 +111848,16 @@
         <v>0.001564913</v>
       </c>
       <c r="O26">
-        <v>3.62e-05</v>
+        <v>3.62E-05</v>
       </c>
       <c r="P26">
-        <v>3.01e-07</v>
+        <v>3.01E-07</v>
       </c>
       <c r="Q26">
-        <v>8.77e-10</v>
+        <v>8.77E-10</v>
       </c>
       <c r="R26">
-        <v>8.96e-13</v>
+        <v>8.96E-13</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -111915,13 +111915,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>4.36e-11</v>
+        <v>4.36E-11</v>
       </c>
       <c r="G27">
-        <v>8.27e-07</v>
+        <v>8.27E-07</v>
       </c>
       <c r="H27">
-        <v>3.67e-05</v>
+        <v>3.67E-05</v>
       </c>
       <c r="I27">
         <v>0.000812507</v>
@@ -111954,16 +111954,16 @@
         <v>0.000690862</v>
       </c>
       <c r="S27">
-        <v>3.23e-05</v>
+        <v>3.23E-05</v>
       </c>
       <c r="T27">
-        <v>2.74e-07</v>
+        <v>2.74E-07</v>
       </c>
       <c r="U27">
-        <v>2.3e-10</v>
+        <v>2.3E-10</v>
       </c>
       <c r="V27">
-        <v>4.39e-14</v>
+        <v>4.39E-14</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -112009,16 +112009,16 @@
         <v>5</v>
       </c>
       <c r="F28">
-        <v>3.07e-13</v>
+        <v>3.07E-13</v>
       </c>
       <c r="G28">
-        <v>4.26e-09</v>
+        <v>4.26E-09</v>
       </c>
       <c r="H28">
-        <v>2.16e-07</v>
+        <v>2.16E-07</v>
       </c>
       <c r="I28">
-        <v>6.55e-06</v>
+        <v>6.55E-06</v>
       </c>
       <c r="J28">
         <v>0.000118811</v>
@@ -112057,16 +112057,16 @@
         <v>0.00035841</v>
       </c>
       <c r="V28">
-        <v>5.47e-06</v>
+        <v>5.47E-06</v>
       </c>
       <c r="W28">
-        <v>3.01e-08</v>
+        <v>3.01E-08</v>
       </c>
       <c r="X28">
-        <v>5.92e-11</v>
+        <v>5.92E-11</v>
       </c>
       <c r="Y28">
-        <v>4.14e-14</v>
+        <v>4.14E-14</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -112103,22 +112103,22 @@
         <v>6</v>
       </c>
       <c r="F29">
-        <v>1.12e-14</v>
+        <v>1.12E-14</v>
       </c>
       <c r="G29">
-        <v>9.42e-11</v>
+        <v>9.42E-11</v>
       </c>
       <c r="H29">
-        <v>4.42e-09</v>
+        <v>4.42E-09</v>
       </c>
       <c r="I29">
-        <v>1.4e-07</v>
+        <v>1.4E-07</v>
       </c>
       <c r="J29">
-        <v>2.91e-06</v>
+        <v>2.91E-06</v>
       </c>
       <c r="K29">
-        <v>4.07e-05</v>
+        <v>4.07E-05</v>
       </c>
       <c r="L29">
         <v>0.000381616</v>
@@ -112157,13 +112157,13 @@
         <v>0.00057203</v>
       </c>
       <c r="X29">
-        <v>1.82e-05</v>
+        <v>1.82E-05</v>
       </c>
       <c r="Y29">
-        <v>2.7e-07</v>
+        <v>2.7E-07</v>
       </c>
       <c r="Z29">
-        <v>1.9e-09</v>
+        <v>1.9E-09</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -112197,25 +112197,25 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>1.19e-15</v>
+        <v>1.19E-15</v>
       </c>
       <c r="G30">
-        <v>6.13e-12</v>
+        <v>6.13E-12</v>
       </c>
       <c r="H30">
-        <v>2.49e-10</v>
+        <v>2.49E-10</v>
       </c>
       <c r="I30">
-        <v>7.33e-09</v>
+        <v>7.33E-09</v>
       </c>
       <c r="J30">
-        <v>1.54e-07</v>
+        <v>1.54E-07</v>
       </c>
       <c r="K30">
-        <v>2.31e-06</v>
+        <v>2.31E-06</v>
       </c>
       <c r="L30">
-        <v>2.49e-05</v>
+        <v>2.49E-05</v>
       </c>
       <c r="M30">
         <v>0.000194666</v>
@@ -112257,13 +112257,13 @@
         <v>0.00051173</v>
       </c>
       <c r="Z30">
-        <v>2.5e-05</v>
+        <v>2.5E-05</v>
       </c>
       <c r="AA30">
-        <v>1.87e-11</v>
+        <v>1.87E-11</v>
       </c>
       <c r="AB30">
-        <v>3.5e-14</v>
+        <v>3.5E-14</v>
       </c>
       <c r="AC30">
         <v>0</v>
@@ -112291,28 +112291,28 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <v>2.71e-16</v>
+        <v>2.71E-16</v>
       </c>
       <c r="G31">
-        <v>8.74e-13</v>
+        <v>8.74E-13</v>
       </c>
       <c r="H31">
-        <v>3e-11</v>
+        <v>3E-11</v>
       </c>
       <c r="I31">
-        <v>7.92e-10</v>
+        <v>7.92E-10</v>
       </c>
       <c r="J31">
-        <v>1.57e-08</v>
+        <v>1.57E-08</v>
       </c>
       <c r="K31">
-        <v>2.35e-07</v>
+        <v>2.35E-07</v>
       </c>
       <c r="L31">
-        <v>2.64e-06</v>
+        <v>2.64E-06</v>
       </c>
       <c r="M31">
-        <v>2.25e-05</v>
+        <v>2.25E-05</v>
       </c>
       <c r="N31">
         <v>0.00014589</v>
@@ -112354,13 +112354,13 @@
         <v>0.003249649</v>
       </c>
       <c r="AA31">
-        <v>8.52e-08</v>
+        <v>8.52E-08</v>
       </c>
       <c r="AB31">
-        <v>8.21e-10</v>
+        <v>8.21E-10</v>
       </c>
       <c r="AC31">
-        <v>4.23e-12</v>
+        <v>4.23E-12</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -112385,31 +112385,31 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>1.09e-16</v>
+        <v>1.09E-16</v>
       </c>
       <c r="G32">
-        <v>2.21e-13</v>
+        <v>2.21E-13</v>
       </c>
       <c r="H32">
-        <v>6.48e-12</v>
+        <v>6.48E-12</v>
       </c>
       <c r="I32">
-        <v>1.52e-10</v>
+        <v>1.52E-10</v>
       </c>
       <c r="J32">
-        <v>2.77e-09</v>
+        <v>2.77E-09</v>
       </c>
       <c r="K32">
-        <v>3.97e-08</v>
+        <v>3.97E-08</v>
       </c>
       <c r="L32">
-        <v>4.42e-07</v>
+        <v>4.42E-07</v>
       </c>
       <c r="M32">
-        <v>3.87e-06</v>
+        <v>3.87E-06</v>
       </c>
       <c r="N32">
-        <v>2.66e-05</v>
+        <v>2.66E-05</v>
       </c>
       <c r="O32">
         <v>0.00014379</v>
@@ -112448,16 +112448,16 @@
         <v>0.038845033</v>
       </c>
       <c r="AA32">
-        <v>1.47e-05</v>
+        <v>1.47E-05</v>
       </c>
       <c r="AB32">
-        <v>4.34e-07</v>
+        <v>4.34E-07</v>
       </c>
       <c r="AC32">
-        <v>7.499999999999999e-09</v>
+        <v>7.499999999999999E-09</v>
       </c>
       <c r="AD32">
-        <v>1.42e-11</v>
+        <v>1.42E-11</v>
       </c>
     </row>
     <row r="33">
@@ -112479,34 +112479,34 @@
         <v>10</v>
       </c>
       <c r="F33">
-        <v>5.82e-17</v>
+        <v>5.82E-17</v>
       </c>
       <c r="G33">
-        <v>9.02e-14</v>
+        <v>9.02E-14</v>
       </c>
       <c r="H33">
-        <v>2.27e-12</v>
+        <v>2.27E-12</v>
       </c>
       <c r="I33">
-        <v>4.71e-11</v>
+        <v>4.71E-11</v>
       </c>
       <c r="J33">
-        <v>7.89e-10</v>
+        <v>7.89E-10</v>
       </c>
       <c r="K33">
-        <v>1.06e-08</v>
+        <v>1.06E-08</v>
       </c>
       <c r="L33">
-        <v>1.14e-07</v>
+        <v>1.14E-07</v>
       </c>
       <c r="M33">
-        <v>9.86e-07</v>
+        <v>9.86E-07</v>
       </c>
       <c r="N33">
-        <v>6.91e-06</v>
+        <v>6.91E-06</v>
       </c>
       <c r="O33">
-        <v>3.9e-05</v>
+        <v>3.9E-05</v>
       </c>
       <c r="P33">
         <v>0.000178483</v>
@@ -112545,13 +112545,13 @@
         <v>0.000401548</v>
       </c>
       <c r="AB33">
-        <v>2.61e-05</v>
+        <v>2.61E-05</v>
       </c>
       <c r="AC33">
-        <v>1.08e-06</v>
+        <v>1.08E-06</v>
       </c>
       <c r="AD33">
-        <v>7.07e-09</v>
+        <v>7.07E-09</v>
       </c>
     </row>
     <row r="34">
@@ -112573,37 +112573,37 @@
         <v>11</v>
       </c>
       <c r="F34">
-        <v>6.86e-17</v>
+        <v>6.86E-17</v>
       </c>
       <c r="G34">
-        <v>5.58e-14</v>
+        <v>5.58E-14</v>
       </c>
       <c r="H34">
-        <v>1.22e-12</v>
+        <v>1.22E-12</v>
       </c>
       <c r="I34">
-        <v>2.26e-11</v>
+        <v>2.26E-11</v>
       </c>
       <c r="J34">
-        <v>3.45e-10</v>
+        <v>3.45E-10</v>
       </c>
       <c r="K34">
-        <v>4.32e-09</v>
+        <v>4.32E-09</v>
       </c>
       <c r="L34">
-        <v>4.44e-08</v>
+        <v>4.44E-08</v>
       </c>
       <c r="M34">
-        <v>3.73e-07</v>
+        <v>3.73E-07</v>
       </c>
       <c r="N34">
-        <v>2.6e-06</v>
+        <v>2.6E-06</v>
       </c>
       <c r="O34">
-        <v>1.49e-05</v>
+        <v>1.49E-05</v>
       </c>
       <c r="P34">
-        <v>7.02e-05</v>
+        <v>7.02E-05</v>
       </c>
       <c r="Q34">
         <v>0.000274962</v>
@@ -112642,10 +112642,10 @@
         <v>0.000448222</v>
       </c>
       <c r="AC34">
-        <v>3.51e-05</v>
+        <v>3.51E-05</v>
       </c>
       <c r="AD34">
-        <v>5.77e-07</v>
+        <v>5.77E-07</v>
       </c>
     </row>
     <row r="35">
@@ -112667,37 +112667,37 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <v>8.84e-17</v>
+        <v>8.84E-17</v>
       </c>
       <c r="G35">
-        <v>4.8e-14</v>
+        <v>4.8E-14</v>
       </c>
       <c r="H35">
-        <v>9.21e-13</v>
+        <v>9.21E-13</v>
       </c>
       <c r="I35">
-        <v>1.54e-11</v>
+        <v>1.54E-11</v>
       </c>
       <c r="J35">
-        <v>2.14e-10</v>
+        <v>2.14E-10</v>
       </c>
       <c r="K35">
-        <v>2.49e-09</v>
+        <v>2.49E-09</v>
       </c>
       <c r="L35">
-        <v>2.42e-08</v>
+        <v>2.42E-08</v>
       </c>
       <c r="M35">
-        <v>1.97e-07</v>
+        <v>1.97E-07</v>
       </c>
       <c r="N35">
-        <v>1.34e-06</v>
+        <v>1.34E-06</v>
       </c>
       <c r="O35">
-        <v>7.63e-06</v>
+        <v>7.63E-06</v>
       </c>
       <c r="P35">
-        <v>3.65e-05</v>
+        <v>3.65E-05</v>
       </c>
       <c r="Q35">
         <v>0.000146448</v>
@@ -112739,7 +112739,7 @@
         <v>0.000454477</v>
       </c>
       <c r="AD35">
-        <v>1.5e-05</v>
+        <v>1.5E-05</v>
       </c>
     </row>
     <row r="36">
@@ -112761,40 +112761,40 @@
         <v>13</v>
       </c>
       <c r="F36">
-        <v>1.16e-16</v>
+        <v>1.16E-16</v>
       </c>
       <c r="G36">
-        <v>5.07e-14</v>
+        <v>5.07E-14</v>
       </c>
       <c r="H36">
-        <v>8.66e-13</v>
+        <v>8.66E-13</v>
       </c>
       <c r="I36">
-        <v>1.31e-11</v>
+        <v>1.31E-11</v>
       </c>
       <c r="J36">
-        <v>1.67e-10</v>
+        <v>1.67E-10</v>
       </c>
       <c r="K36">
-        <v>1.81e-09</v>
+        <v>1.81E-09</v>
       </c>
       <c r="L36">
-        <v>1.66e-08</v>
+        <v>1.66E-08</v>
       </c>
       <c r="M36">
-        <v>1.3e-07</v>
+        <v>1.3E-07</v>
       </c>
       <c r="N36">
-        <v>8.53e-07</v>
+        <v>8.53E-07</v>
       </c>
       <c r="O36">
-        <v>4.8e-06</v>
+        <v>4.8E-06</v>
       </c>
       <c r="P36">
-        <v>2.29e-05</v>
+        <v>2.29E-05</v>
       </c>
       <c r="Q36">
-        <v>9.26e-05</v>
+        <v>9.26E-05</v>
       </c>
       <c r="R36">
         <v>0.000320283</v>
@@ -112855,40 +112855,40 @@
         <v>14</v>
       </c>
       <c r="F37">
-        <v>1.45e-16</v>
+        <v>1.45E-16</v>
       </c>
       <c r="G37">
-        <v>5.819999999999999e-14</v>
+        <v>5.819999999999999E-14</v>
       </c>
       <c r="H37">
-        <v>8.93e-13</v>
+        <v>8.93E-13</v>
       </c>
       <c r="I37">
-        <v>1.23e-11</v>
+        <v>1.23E-11</v>
       </c>
       <c r="J37">
-        <v>1.45e-10</v>
+        <v>1.45E-10</v>
       </c>
       <c r="K37">
-        <v>1.47e-09</v>
+        <v>1.47E-09</v>
       </c>
       <c r="L37">
-        <v>1.27e-08</v>
+        <v>1.27E-08</v>
       </c>
       <c r="M37">
-        <v>9.49e-08</v>
+        <v>9.49E-08</v>
       </c>
       <c r="N37">
-        <v>6.03e-07</v>
+        <v>6.03E-07</v>
       </c>
       <c r="O37">
-        <v>3.31e-06</v>
+        <v>3.31E-06</v>
       </c>
       <c r="P37">
-        <v>1.56e-05</v>
+        <v>1.56E-05</v>
       </c>
       <c r="Q37">
-        <v>6.3e-05</v>
+        <v>6.3E-05</v>
       </c>
       <c r="R37">
         <v>0.000219607</v>
@@ -112949,40 +112949,40 @@
         <v>15</v>
       </c>
       <c r="F38">
-        <v>1.61e-16</v>
+        <v>1.61E-16</v>
       </c>
       <c r="G38">
-        <v>6.71e-14</v>
+        <v>6.71E-14</v>
       </c>
       <c r="H38">
-        <v>9.300000000000001e-13</v>
+        <v>9.300000000000001E-13</v>
       </c>
       <c r="I38">
-        <v>1.17e-11</v>
+        <v>1.17E-11</v>
       </c>
       <c r="J38">
-        <v>1.29e-10</v>
+        <v>1.29E-10</v>
       </c>
       <c r="K38">
-        <v>1.22e-09</v>
+        <v>1.22E-09</v>
       </c>
       <c r="L38">
-        <v>9.980000000000001e-09</v>
+        <v>9.980000000000001E-09</v>
       </c>
       <c r="M38">
-        <v>7.08e-08</v>
+        <v>7.08E-08</v>
       </c>
       <c r="N38">
-        <v>4.35e-07</v>
+        <v>4.35E-07</v>
       </c>
       <c r="O38">
-        <v>2.32e-06</v>
+        <v>2.32E-06</v>
       </c>
       <c r="P38">
-        <v>1.07e-05</v>
+        <v>1.07E-05</v>
       </c>
       <c r="Q38">
-        <v>4.3e-05</v>
+        <v>4.3E-05</v>
       </c>
       <c r="R38">
         <v>0.000149742</v>
@@ -113043,40 +113043,40 @@
         <v>16</v>
       </c>
       <c r="F39">
-        <v>3.23e-16</v>
+        <v>3.23E-16</v>
       </c>
       <c r="G39">
-        <v>7.59e-14</v>
+        <v>7.59E-14</v>
       </c>
       <c r="H39">
-        <v>9.590000000000001e-13</v>
+        <v>9.590000000000001E-13</v>
       </c>
       <c r="I39">
-        <v>1.12e-11</v>
+        <v>1.12E-11</v>
       </c>
       <c r="J39">
-        <v>1.14e-10</v>
+        <v>1.14E-10</v>
       </c>
       <c r="K39">
-        <v>1.02e-09</v>
+        <v>1.02E-09</v>
       </c>
       <c r="L39">
-        <v>7.87e-09</v>
+        <v>7.87E-09</v>
       </c>
       <c r="M39">
-        <v>5.33e-08</v>
+        <v>5.33E-08</v>
       </c>
       <c r="N39">
-        <v>3.15e-07</v>
+        <v>3.15E-07</v>
       </c>
       <c r="O39">
-        <v>1.63e-06</v>
+        <v>1.63E-06</v>
       </c>
       <c r="P39">
-        <v>7.37e-06</v>
+        <v>7.37E-06</v>
       </c>
       <c r="Q39">
-        <v>2.91e-05</v>
+        <v>2.91E-05</v>
       </c>
       <c r="R39">
         <v>0.000100803</v>
@@ -113137,43 +113137,43 @@
         <v>17</v>
       </c>
       <c r="F40">
-        <v>3.04e-16</v>
+        <v>3.04E-16</v>
       </c>
       <c r="G40">
-        <v>8.65e-14</v>
+        <v>8.65E-14</v>
       </c>
       <c r="H40">
-        <v>1e-12</v>
+        <v>1E-12</v>
       </c>
       <c r="I40">
-        <v>1.09e-11</v>
+        <v>1.09E-11</v>
       </c>
       <c r="J40">
-        <v>1.04e-10</v>
+        <v>1.04E-10</v>
       </c>
       <c r="K40">
-        <v>8.67e-10</v>
+        <v>8.67E-10</v>
       </c>
       <c r="L40">
-        <v>6.38e-09</v>
+        <v>6.38E-09</v>
       </c>
       <c r="M40">
-        <v>4.13e-08</v>
+        <v>4.13E-08</v>
       </c>
       <c r="N40">
-        <v>2.35e-07</v>
+        <v>2.35E-07</v>
       </c>
       <c r="O40">
-        <v>1.17e-06</v>
+        <v>1.17E-06</v>
       </c>
       <c r="P40">
-        <v>5.21e-06</v>
+        <v>5.21E-06</v>
       </c>
       <c r="Q40">
-        <v>2.01e-05</v>
+        <v>2.01E-05</v>
       </c>
       <c r="R40">
-        <v>6.889999999999999e-05</v>
+        <v>6.889999999999999E-05</v>
       </c>
       <c r="S40">
         <v>0.000309476</v>
@@ -113231,43 +113231,43 @@
         <v>18</v>
       </c>
       <c r="F41">
-        <v>4.2e-16</v>
+        <v>4.2E-16</v>
       </c>
       <c r="G41">
-        <v>1.01e-13</v>
+        <v>1.01E-13</v>
       </c>
       <c r="H41">
-        <v>1.08e-12</v>
+        <v>1.08E-12</v>
       </c>
       <c r="I41">
-        <v>1.09e-11</v>
+        <v>1.09E-11</v>
       </c>
       <c r="J41">
-        <v>9.83e-11</v>
+        <v>9.83E-11</v>
       </c>
       <c r="K41">
-        <v>7.76e-10</v>
+        <v>7.76E-10</v>
       </c>
       <c r="L41">
-        <v>5.43e-09</v>
+        <v>5.43E-09</v>
       </c>
       <c r="M41">
-        <v>3.36e-08</v>
+        <v>3.36E-08</v>
       </c>
       <c r="N41">
-        <v>1.84e-07</v>
+        <v>1.84E-07</v>
       </c>
       <c r="O41">
-        <v>8.92e-07</v>
+        <v>8.92E-07</v>
       </c>
       <c r="P41">
-        <v>3.84e-06</v>
+        <v>3.84E-06</v>
       </c>
       <c r="Q41">
-        <v>1.46e-05</v>
+        <v>1.46E-05</v>
       </c>
       <c r="R41">
-        <v>4.92e-05</v>
+        <v>4.92E-05</v>
       </c>
       <c r="S41">
         <v>0.000218751</v>
@@ -113325,43 +113325,43 @@
         <v>19</v>
       </c>
       <c r="F42">
-        <v>6.44e-16</v>
+        <v>6.44E-16</v>
       </c>
       <c r="G42">
-        <v>1.23e-13</v>
+        <v>1.23E-13</v>
       </c>
       <c r="H42">
-        <v>1.22e-12</v>
+        <v>1.22E-12</v>
       </c>
       <c r="I42">
-        <v>1.16e-11</v>
+        <v>1.16E-11</v>
       </c>
       <c r="J42">
-        <v>9.78e-11</v>
+        <v>9.78E-11</v>
       </c>
       <c r="K42">
-        <v>7.340000000000001e-10</v>
+        <v>7.340000000000001E-10</v>
       </c>
       <c r="L42">
-        <v>4.9e-09</v>
+        <v>4.9E-09</v>
       </c>
       <c r="M42">
-        <v>2.9e-08</v>
+        <v>2.9E-08</v>
       </c>
       <c r="N42">
-        <v>1.53e-07</v>
+        <v>1.53E-07</v>
       </c>
       <c r="O42">
-        <v>7.180000000000001e-07</v>
+        <v>7.180000000000001E-07</v>
       </c>
       <c r="P42">
-        <v>3.01e-06</v>
+        <v>3.01E-06</v>
       </c>
       <c r="Q42">
-        <v>1.12e-05</v>
+        <v>1.12E-05</v>
       </c>
       <c r="R42">
-        <v>3.71e-05</v>
+        <v>3.71E-05</v>
       </c>
       <c r="S42">
         <v>0.00016277</v>
@@ -113419,43 +113419,43 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <v>9.549999999999999e-16</v>
+        <v>9.549999999999999E-16</v>
       </c>
       <c r="G43">
-        <v>1.56e-13</v>
+        <v>1.56E-13</v>
       </c>
       <c r="H43">
-        <v>1.44e-12</v>
+        <v>1.44E-12</v>
       </c>
       <c r="I43">
-        <v>1.29e-11</v>
+        <v>1.29E-11</v>
       </c>
       <c r="J43">
-        <v>1.03e-10</v>
+        <v>1.03E-10</v>
       </c>
       <c r="K43">
-        <v>7.37e-10</v>
+        <v>7.37E-10</v>
       </c>
       <c r="L43">
-        <v>4.67e-09</v>
+        <v>4.67E-09</v>
       </c>
       <c r="M43">
-        <v>2.66e-08</v>
+        <v>2.66E-08</v>
       </c>
       <c r="N43">
-        <v>1.35e-07</v>
+        <v>1.35E-07</v>
       </c>
       <c r="O43">
-        <v>6.16e-07</v>
+        <v>6.16E-07</v>
       </c>
       <c r="P43">
-        <v>2.49e-06</v>
+        <v>2.49E-06</v>
       </c>
       <c r="Q43">
-        <v>9.07e-06</v>
+        <v>9.07E-06</v>
       </c>
       <c r="R43">
-        <v>2.96e-05</v>
+        <v>2.96E-05</v>
       </c>
       <c r="S43">
         <v>0.000127693</v>
@@ -113513,43 +113513,43 @@
         <v>21</v>
       </c>
       <c r="F44">
-        <v>1.45e-15</v>
+        <v>1.45E-15</v>
       </c>
       <c r="G44">
-        <v>2.05e-13</v>
+        <v>2.05E-13</v>
       </c>
       <c r="H44">
-        <v>1.76e-12</v>
+        <v>1.76E-12</v>
       </c>
       <c r="I44">
-        <v>1.49e-11</v>
+        <v>1.49E-11</v>
       </c>
       <c r="J44">
-        <v>1.13e-10</v>
+        <v>1.13E-10</v>
       </c>
       <c r="K44">
-        <v>7.67e-10</v>
+        <v>7.67E-10</v>
       </c>
       <c r="L44">
-        <v>4.67e-09</v>
+        <v>4.67E-09</v>
       </c>
       <c r="M44">
-        <v>2.56e-08</v>
+        <v>2.56E-08</v>
       </c>
       <c r="N44">
-        <v>1.25e-07</v>
+        <v>1.25E-07</v>
       </c>
       <c r="O44">
-        <v>5.51e-07</v>
+        <v>5.51E-07</v>
       </c>
       <c r="P44">
-        <v>2.18e-06</v>
+        <v>2.18E-06</v>
       </c>
       <c r="Q44">
-        <v>7.77e-06</v>
+        <v>7.77E-06</v>
       </c>
       <c r="R44">
-        <v>2.48e-05</v>
+        <v>2.48E-05</v>
       </c>
       <c r="S44">
         <v>0.000105218</v>

</xml_diff>

<commit_message>
vector/matrix mult bug in TMB
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -29821,7 +29821,7 @@
         <v>20</v>
       </c>
       <c r="I332">
-        <v>4.61e-05</v>
+        <v>4.61E-05</v>
       </c>
     </row>
     <row r="333">
@@ -47308,7 +47308,7 @@
         <v>20</v>
       </c>
       <c r="I935">
-        <v>6e-05</v>
+        <v>6E-05</v>
       </c>
     </row>
     <row r="936">
@@ -111636,7 +111636,7 @@
         <v>0.9999116</v>
       </c>
       <c r="G24">
-        <v>8.839999999999999e-05</v>
+        <v>8.839999999999999E-05</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -111742,13 +111742,13 @@
         <v>0.001538802</v>
       </c>
       <c r="K25">
-        <v>5.68e-06</v>
+        <v>5.68E-06</v>
       </c>
       <c r="L25">
-        <v>2.91e-09</v>
+        <v>2.91E-09</v>
       </c>
       <c r="M25">
-        <v>1.97e-13</v>
+        <v>1.97E-13</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -111821,7 +111821,7 @@
         <v>3</v>
       </c>
       <c r="F26">
-        <v>7.36e-08</v>
+        <v>7.36E-08</v>
       </c>
       <c r="G26">
         <v>0.000825826</v>
@@ -111848,16 +111848,16 @@
         <v>0.001564913</v>
       </c>
       <c r="O26">
-        <v>3.62e-05</v>
+        <v>3.62E-05</v>
       </c>
       <c r="P26">
-        <v>3.01e-07</v>
+        <v>3.01E-07</v>
       </c>
       <c r="Q26">
-        <v>8.77e-10</v>
+        <v>8.77E-10</v>
       </c>
       <c r="R26">
-        <v>8.96e-13</v>
+        <v>8.96E-13</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -111915,13 +111915,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>4.36e-11</v>
+        <v>4.36E-11</v>
       </c>
       <c r="G27">
-        <v>8.27e-07</v>
+        <v>8.27E-07</v>
       </c>
       <c r="H27">
-        <v>3.67e-05</v>
+        <v>3.67E-05</v>
       </c>
       <c r="I27">
         <v>0.000812507</v>
@@ -111954,16 +111954,16 @@
         <v>0.000690862</v>
       </c>
       <c r="S27">
-        <v>3.23e-05</v>
+        <v>3.23E-05</v>
       </c>
       <c r="T27">
-        <v>2.74e-07</v>
+        <v>2.74E-07</v>
       </c>
       <c r="U27">
-        <v>2.3e-10</v>
+        <v>2.3E-10</v>
       </c>
       <c r="V27">
-        <v>4.39e-14</v>
+        <v>4.39E-14</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -112009,16 +112009,16 @@
         <v>5</v>
       </c>
       <c r="F28">
-        <v>3.07e-13</v>
+        <v>3.07E-13</v>
       </c>
       <c r="G28">
-        <v>4.26e-09</v>
+        <v>4.26E-09</v>
       </c>
       <c r="H28">
-        <v>2.16e-07</v>
+        <v>2.16E-07</v>
       </c>
       <c r="I28">
-        <v>6.55e-06</v>
+        <v>6.55E-06</v>
       </c>
       <c r="J28">
         <v>0.000118811</v>
@@ -112057,16 +112057,16 @@
         <v>0.00035841</v>
       </c>
       <c r="V28">
-        <v>5.47e-06</v>
+        <v>5.47E-06</v>
       </c>
       <c r="W28">
-        <v>3.01e-08</v>
+        <v>3.01E-08</v>
       </c>
       <c r="X28">
-        <v>5.92e-11</v>
+        <v>5.92E-11</v>
       </c>
       <c r="Y28">
-        <v>4.14e-14</v>
+        <v>4.14E-14</v>
       </c>
       <c r="Z28">
         <v>0</v>
@@ -112103,22 +112103,22 @@
         <v>6</v>
       </c>
       <c r="F29">
-        <v>1.12e-14</v>
+        <v>1.12E-14</v>
       </c>
       <c r="G29">
-        <v>9.42e-11</v>
+        <v>9.42E-11</v>
       </c>
       <c r="H29">
-        <v>4.42e-09</v>
+        <v>4.42E-09</v>
       </c>
       <c r="I29">
-        <v>1.4e-07</v>
+        <v>1.4E-07</v>
       </c>
       <c r="J29">
-        <v>2.91e-06</v>
+        <v>2.91E-06</v>
       </c>
       <c r="K29">
-        <v>4.07e-05</v>
+        <v>4.07E-05</v>
       </c>
       <c r="L29">
         <v>0.000381616</v>
@@ -112157,13 +112157,13 @@
         <v>0.00057203</v>
       </c>
       <c r="X29">
-        <v>1.82e-05</v>
+        <v>1.82E-05</v>
       </c>
       <c r="Y29">
-        <v>2.7e-07</v>
+        <v>2.7E-07</v>
       </c>
       <c r="Z29">
-        <v>1.9e-09</v>
+        <v>1.9E-09</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -112197,25 +112197,25 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>1.19e-15</v>
+        <v>1.19E-15</v>
       </c>
       <c r="G30">
-        <v>6.13e-12</v>
+        <v>6.13E-12</v>
       </c>
       <c r="H30">
-        <v>2.49e-10</v>
+        <v>2.49E-10</v>
       </c>
       <c r="I30">
-        <v>7.33e-09</v>
+        <v>7.33E-09</v>
       </c>
       <c r="J30">
-        <v>1.54e-07</v>
+        <v>1.54E-07</v>
       </c>
       <c r="K30">
-        <v>2.31e-06</v>
+        <v>2.31E-06</v>
       </c>
       <c r="L30">
-        <v>2.49e-05</v>
+        <v>2.49E-05</v>
       </c>
       <c r="M30">
         <v>0.000194666</v>
@@ -112257,13 +112257,13 @@
         <v>0.00051173</v>
       </c>
       <c r="Z30">
-        <v>2.5e-05</v>
+        <v>2.5E-05</v>
       </c>
       <c r="AA30">
-        <v>1.87e-11</v>
+        <v>1.87E-11</v>
       </c>
       <c r="AB30">
-        <v>3.5e-14</v>
+        <v>3.5E-14</v>
       </c>
       <c r="AC30">
         <v>0</v>
@@ -112291,28 +112291,28 @@
         <v>8</v>
       </c>
       <c r="F31">
-        <v>2.71e-16</v>
+        <v>2.71E-16</v>
       </c>
       <c r="G31">
-        <v>8.74e-13</v>
+        <v>8.74E-13</v>
       </c>
       <c r="H31">
-        <v>3e-11</v>
+        <v>3E-11</v>
       </c>
       <c r="I31">
-        <v>7.92e-10</v>
+        <v>7.92E-10</v>
       </c>
       <c r="J31">
-        <v>1.57e-08</v>
+        <v>1.57E-08</v>
       </c>
       <c r="K31">
-        <v>2.35e-07</v>
+        <v>2.35E-07</v>
       </c>
       <c r="L31">
-        <v>2.64e-06</v>
+        <v>2.64E-06</v>
       </c>
       <c r="M31">
-        <v>2.25e-05</v>
+        <v>2.25E-05</v>
       </c>
       <c r="N31">
         <v>0.00014589</v>
@@ -112354,13 +112354,13 @@
         <v>0.003249649</v>
       </c>
       <c r="AA31">
-        <v>8.52e-08</v>
+        <v>8.52E-08</v>
       </c>
       <c r="AB31">
-        <v>8.21e-10</v>
+        <v>8.21E-10</v>
       </c>
       <c r="AC31">
-        <v>4.23e-12</v>
+        <v>4.23E-12</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -112385,31 +112385,31 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>1.09e-16</v>
+        <v>1.09E-16</v>
       </c>
       <c r="G32">
-        <v>2.21e-13</v>
+        <v>2.21E-13</v>
       </c>
       <c r="H32">
-        <v>6.48e-12</v>
+        <v>6.48E-12</v>
       </c>
       <c r="I32">
-        <v>1.52e-10</v>
+        <v>1.52E-10</v>
       </c>
       <c r="J32">
-        <v>2.77e-09</v>
+        <v>2.77E-09</v>
       </c>
       <c r="K32">
-        <v>3.97e-08</v>
+        <v>3.97E-08</v>
       </c>
       <c r="L32">
-        <v>4.42e-07</v>
+        <v>4.42E-07</v>
       </c>
       <c r="M32">
-        <v>3.87e-06</v>
+        <v>3.87E-06</v>
       </c>
       <c r="N32">
-        <v>2.66e-05</v>
+        <v>2.66E-05</v>
       </c>
       <c r="O32">
         <v>0.00014379</v>
@@ -112448,16 +112448,16 @@
         <v>0.038845033</v>
       </c>
       <c r="AA32">
-        <v>1.47e-05</v>
+        <v>1.47E-05</v>
       </c>
       <c r="AB32">
-        <v>4.34e-07</v>
+        <v>4.34E-07</v>
       </c>
       <c r="AC32">
-        <v>7.499999999999999e-09</v>
+        <v>7.499999999999999E-09</v>
       </c>
       <c r="AD32">
-        <v>1.42e-11</v>
+        <v>1.42E-11</v>
       </c>
     </row>
     <row r="33">
@@ -112479,34 +112479,34 @@
         <v>10</v>
       </c>
       <c r="F33">
-        <v>5.82e-17</v>
+        <v>5.82E-17</v>
       </c>
       <c r="G33">
-        <v>9.02e-14</v>
+        <v>9.02E-14</v>
       </c>
       <c r="H33">
-        <v>2.27e-12</v>
+        <v>2.27E-12</v>
       </c>
       <c r="I33">
-        <v>4.71e-11</v>
+        <v>4.71E-11</v>
       </c>
       <c r="J33">
-        <v>7.89e-10</v>
+        <v>7.89E-10</v>
       </c>
       <c r="K33">
-        <v>1.06e-08</v>
+        <v>1.06E-08</v>
       </c>
       <c r="L33">
-        <v>1.14e-07</v>
+        <v>1.14E-07</v>
       </c>
       <c r="M33">
-        <v>9.86e-07</v>
+        <v>9.86E-07</v>
       </c>
       <c r="N33">
-        <v>6.91e-06</v>
+        <v>6.91E-06</v>
       </c>
       <c r="O33">
-        <v>3.9e-05</v>
+        <v>3.9E-05</v>
       </c>
       <c r="P33">
         <v>0.000178483</v>
@@ -112545,13 +112545,13 @@
         <v>0.000401548</v>
       </c>
       <c r="AB33">
-        <v>2.61e-05</v>
+        <v>2.61E-05</v>
       </c>
       <c r="AC33">
-        <v>1.08e-06</v>
+        <v>1.08E-06</v>
       </c>
       <c r="AD33">
-        <v>7.07e-09</v>
+        <v>7.07E-09</v>
       </c>
     </row>
     <row r="34">
@@ -112573,37 +112573,37 @@
         <v>11</v>
       </c>
       <c r="F34">
-        <v>6.86e-17</v>
+        <v>6.86E-17</v>
       </c>
       <c r="G34">
-        <v>5.58e-14</v>
+        <v>5.58E-14</v>
       </c>
       <c r="H34">
-        <v>1.22e-12</v>
+        <v>1.22E-12</v>
       </c>
       <c r="I34">
-        <v>2.26e-11</v>
+        <v>2.26E-11</v>
       </c>
       <c r="J34">
-        <v>3.45e-10</v>
+        <v>3.45E-10</v>
       </c>
       <c r="K34">
-        <v>4.32e-09</v>
+        <v>4.32E-09</v>
       </c>
       <c r="L34">
-        <v>4.44e-08</v>
+        <v>4.44E-08</v>
       </c>
       <c r="M34">
-        <v>3.73e-07</v>
+        <v>3.73E-07</v>
       </c>
       <c r="N34">
-        <v>2.6e-06</v>
+        <v>2.6E-06</v>
       </c>
       <c r="O34">
-        <v>1.49e-05</v>
+        <v>1.49E-05</v>
       </c>
       <c r="P34">
-        <v>7.02e-05</v>
+        <v>7.02E-05</v>
       </c>
       <c r="Q34">
         <v>0.000274962</v>
@@ -112642,10 +112642,10 @@
         <v>0.000448222</v>
       </c>
       <c r="AC34">
-        <v>3.51e-05</v>
+        <v>3.51E-05</v>
       </c>
       <c r="AD34">
-        <v>5.77e-07</v>
+        <v>5.77E-07</v>
       </c>
     </row>
     <row r="35">
@@ -112667,37 +112667,37 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <v>8.84e-17</v>
+        <v>8.84E-17</v>
       </c>
       <c r="G35">
-        <v>4.8e-14</v>
+        <v>4.8E-14</v>
       </c>
       <c r="H35">
-        <v>9.21e-13</v>
+        <v>9.21E-13</v>
       </c>
       <c r="I35">
-        <v>1.54e-11</v>
+        <v>1.54E-11</v>
       </c>
       <c r="J35">
-        <v>2.14e-10</v>
+        <v>2.14E-10</v>
       </c>
       <c r="K35">
-        <v>2.49e-09</v>
+        <v>2.49E-09</v>
       </c>
       <c r="L35">
-        <v>2.42e-08</v>
+        <v>2.42E-08</v>
       </c>
       <c r="M35">
-        <v>1.97e-07</v>
+        <v>1.97E-07</v>
       </c>
       <c r="N35">
-        <v>1.34e-06</v>
+        <v>1.34E-06</v>
       </c>
       <c r="O35">
-        <v>7.63e-06</v>
+        <v>7.63E-06</v>
       </c>
       <c r="P35">
-        <v>3.65e-05</v>
+        <v>3.65E-05</v>
       </c>
       <c r="Q35">
         <v>0.000146448</v>
@@ -112739,7 +112739,7 @@
         <v>0.000454477</v>
       </c>
       <c r="AD35">
-        <v>1.5e-05</v>
+        <v>1.5E-05</v>
       </c>
     </row>
     <row r="36">
@@ -112761,40 +112761,40 @@
         <v>13</v>
       </c>
       <c r="F36">
-        <v>1.16e-16</v>
+        <v>1.16E-16</v>
       </c>
       <c r="G36">
-        <v>5.07e-14</v>
+        <v>5.07E-14</v>
       </c>
       <c r="H36">
-        <v>8.66e-13</v>
+        <v>8.66E-13</v>
       </c>
       <c r="I36">
-        <v>1.31e-11</v>
+        <v>1.31E-11</v>
       </c>
       <c r="J36">
-        <v>1.67e-10</v>
+        <v>1.67E-10</v>
       </c>
       <c r="K36">
-        <v>1.81e-09</v>
+        <v>1.81E-09</v>
       </c>
       <c r="L36">
-        <v>1.66e-08</v>
+        <v>1.66E-08</v>
       </c>
       <c r="M36">
-        <v>1.3e-07</v>
+        <v>1.3E-07</v>
       </c>
       <c r="N36">
-        <v>8.53e-07</v>
+        <v>8.53E-07</v>
       </c>
       <c r="O36">
-        <v>4.8e-06</v>
+        <v>4.8E-06</v>
       </c>
       <c r="P36">
-        <v>2.29e-05</v>
+        <v>2.29E-05</v>
       </c>
       <c r="Q36">
-        <v>9.26e-05</v>
+        <v>9.26E-05</v>
       </c>
       <c r="R36">
         <v>0.000320283</v>
@@ -112855,40 +112855,40 @@
         <v>14</v>
       </c>
       <c r="F37">
-        <v>1.45e-16</v>
+        <v>1.45E-16</v>
       </c>
       <c r="G37">
-        <v>5.819999999999999e-14</v>
+        <v>5.819999999999999E-14</v>
       </c>
       <c r="H37">
-        <v>8.93e-13</v>
+        <v>8.93E-13</v>
       </c>
       <c r="I37">
-        <v>1.23e-11</v>
+        <v>1.23E-11</v>
       </c>
       <c r="J37">
-        <v>1.45e-10</v>
+        <v>1.45E-10</v>
       </c>
       <c r="K37">
-        <v>1.47e-09</v>
+        <v>1.47E-09</v>
       </c>
       <c r="L37">
-        <v>1.27e-08</v>
+        <v>1.27E-08</v>
       </c>
       <c r="M37">
-        <v>9.49e-08</v>
+        <v>9.49E-08</v>
       </c>
       <c r="N37">
-        <v>6.03e-07</v>
+        <v>6.03E-07</v>
       </c>
       <c r="O37">
-        <v>3.31e-06</v>
+        <v>3.31E-06</v>
       </c>
       <c r="P37">
-        <v>1.56e-05</v>
+        <v>1.56E-05</v>
       </c>
       <c r="Q37">
-        <v>6.3e-05</v>
+        <v>6.3E-05</v>
       </c>
       <c r="R37">
         <v>0.000219607</v>
@@ -112949,40 +112949,40 @@
         <v>15</v>
       </c>
       <c r="F38">
-        <v>1.61e-16</v>
+        <v>1.61E-16</v>
       </c>
       <c r="G38">
-        <v>6.71e-14</v>
+        <v>6.71E-14</v>
       </c>
       <c r="H38">
-        <v>9.300000000000001e-13</v>
+        <v>9.300000000000001E-13</v>
       </c>
       <c r="I38">
-        <v>1.17e-11</v>
+        <v>1.17E-11</v>
       </c>
       <c r="J38">
-        <v>1.29e-10</v>
+        <v>1.29E-10</v>
       </c>
       <c r="K38">
-        <v>1.22e-09</v>
+        <v>1.22E-09</v>
       </c>
       <c r="L38">
-        <v>9.980000000000001e-09</v>
+        <v>9.980000000000001E-09</v>
       </c>
       <c r="M38">
-        <v>7.08e-08</v>
+        <v>7.08E-08</v>
       </c>
       <c r="N38">
-        <v>4.35e-07</v>
+        <v>4.35E-07</v>
       </c>
       <c r="O38">
-        <v>2.32e-06</v>
+        <v>2.32E-06</v>
       </c>
       <c r="P38">
-        <v>1.07e-05</v>
+        <v>1.07E-05</v>
       </c>
       <c r="Q38">
-        <v>4.3e-05</v>
+        <v>4.3E-05</v>
       </c>
       <c r="R38">
         <v>0.000149742</v>
@@ -113043,40 +113043,40 @@
         <v>16</v>
       </c>
       <c r="F39">
-        <v>3.23e-16</v>
+        <v>3.23E-16</v>
       </c>
       <c r="G39">
-        <v>7.59e-14</v>
+        <v>7.59E-14</v>
       </c>
       <c r="H39">
-        <v>9.590000000000001e-13</v>
+        <v>9.590000000000001E-13</v>
       </c>
       <c r="I39">
-        <v>1.12e-11</v>
+        <v>1.12E-11</v>
       </c>
       <c r="J39">
-        <v>1.14e-10</v>
+        <v>1.14E-10</v>
       </c>
       <c r="K39">
-        <v>1.02e-09</v>
+        <v>1.02E-09</v>
       </c>
       <c r="L39">
-        <v>7.87e-09</v>
+        <v>7.87E-09</v>
       </c>
       <c r="M39">
-        <v>5.33e-08</v>
+        <v>5.33E-08</v>
       </c>
       <c r="N39">
-        <v>3.15e-07</v>
+        <v>3.15E-07</v>
       </c>
       <c r="O39">
-        <v>1.63e-06</v>
+        <v>1.63E-06</v>
       </c>
       <c r="P39">
-        <v>7.37e-06</v>
+        <v>7.37E-06</v>
       </c>
       <c r="Q39">
-        <v>2.91e-05</v>
+        <v>2.91E-05</v>
       </c>
       <c r="R39">
         <v>0.000100803</v>
@@ -113137,43 +113137,43 @@
         <v>17</v>
       </c>
       <c r="F40">
-        <v>3.04e-16</v>
+        <v>3.04E-16</v>
       </c>
       <c r="G40">
-        <v>8.65e-14</v>
+        <v>8.65E-14</v>
       </c>
       <c r="H40">
-        <v>1e-12</v>
+        <v>1E-12</v>
       </c>
       <c r="I40">
-        <v>1.09e-11</v>
+        <v>1.09E-11</v>
       </c>
       <c r="J40">
-        <v>1.04e-10</v>
+        <v>1.04E-10</v>
       </c>
       <c r="K40">
-        <v>8.67e-10</v>
+        <v>8.67E-10</v>
       </c>
       <c r="L40">
-        <v>6.38e-09</v>
+        <v>6.38E-09</v>
       </c>
       <c r="M40">
-        <v>4.13e-08</v>
+        <v>4.13E-08</v>
       </c>
       <c r="N40">
-        <v>2.35e-07</v>
+        <v>2.35E-07</v>
       </c>
       <c r="O40">
-        <v>1.17e-06</v>
+        <v>1.17E-06</v>
       </c>
       <c r="P40">
-        <v>5.21e-06</v>
+        <v>5.21E-06</v>
       </c>
       <c r="Q40">
-        <v>2.01e-05</v>
+        <v>2.01E-05</v>
       </c>
       <c r="R40">
-        <v>6.889999999999999e-05</v>
+        <v>6.889999999999999E-05</v>
       </c>
       <c r="S40">
         <v>0.000309476</v>
@@ -113231,43 +113231,43 @@
         <v>18</v>
       </c>
       <c r="F41">
-        <v>4.2e-16</v>
+        <v>4.2E-16</v>
       </c>
       <c r="G41">
-        <v>1.01e-13</v>
+        <v>1.01E-13</v>
       </c>
       <c r="H41">
-        <v>1.08e-12</v>
+        <v>1.08E-12</v>
       </c>
       <c r="I41">
-        <v>1.09e-11</v>
+        <v>1.09E-11</v>
       </c>
       <c r="J41">
-        <v>9.83e-11</v>
+        <v>9.83E-11</v>
       </c>
       <c r="K41">
-        <v>7.76e-10</v>
+        <v>7.76E-10</v>
       </c>
       <c r="L41">
-        <v>5.43e-09</v>
+        <v>5.43E-09</v>
       </c>
       <c r="M41">
-        <v>3.36e-08</v>
+        <v>3.36E-08</v>
       </c>
       <c r="N41">
-        <v>1.84e-07</v>
+        <v>1.84E-07</v>
       </c>
       <c r="O41">
-        <v>8.92e-07</v>
+        <v>8.92E-07</v>
       </c>
       <c r="P41">
-        <v>3.84e-06</v>
+        <v>3.84E-06</v>
       </c>
       <c r="Q41">
-        <v>1.46e-05</v>
+        <v>1.46E-05</v>
       </c>
       <c r="R41">
-        <v>4.92e-05</v>
+        <v>4.92E-05</v>
       </c>
       <c r="S41">
         <v>0.000218751</v>
@@ -113325,43 +113325,43 @@
         <v>19</v>
       </c>
       <c r="F42">
-        <v>6.44e-16</v>
+        <v>6.44E-16</v>
       </c>
       <c r="G42">
-        <v>1.23e-13</v>
+        <v>1.23E-13</v>
       </c>
       <c r="H42">
-        <v>1.22e-12</v>
+        <v>1.22E-12</v>
       </c>
       <c r="I42">
-        <v>1.16e-11</v>
+        <v>1.16E-11</v>
       </c>
       <c r="J42">
-        <v>9.78e-11</v>
+        <v>9.78E-11</v>
       </c>
       <c r="K42">
-        <v>7.340000000000001e-10</v>
+        <v>7.340000000000001E-10</v>
       </c>
       <c r="L42">
-        <v>4.9e-09</v>
+        <v>4.9E-09</v>
       </c>
       <c r="M42">
-        <v>2.9e-08</v>
+        <v>2.9E-08</v>
       </c>
       <c r="N42">
-        <v>1.53e-07</v>
+        <v>1.53E-07</v>
       </c>
       <c r="O42">
-        <v>7.180000000000001e-07</v>
+        <v>7.180000000000001E-07</v>
       </c>
       <c r="P42">
-        <v>3.01e-06</v>
+        <v>3.01E-06</v>
       </c>
       <c r="Q42">
-        <v>1.12e-05</v>
+        <v>1.12E-05</v>
       </c>
       <c r="R42">
-        <v>3.71e-05</v>
+        <v>3.71E-05</v>
       </c>
       <c r="S42">
         <v>0.00016277</v>
@@ -113419,43 +113419,43 @@
         <v>20</v>
       </c>
       <c r="F43">
-        <v>9.549999999999999e-16</v>
+        <v>9.549999999999999E-16</v>
       </c>
       <c r="G43">
-        <v>1.56e-13</v>
+        <v>1.56E-13</v>
       </c>
       <c r="H43">
-        <v>1.44e-12</v>
+        <v>1.44E-12</v>
       </c>
       <c r="I43">
-        <v>1.29e-11</v>
+        <v>1.29E-11</v>
       </c>
       <c r="J43">
-        <v>1.03e-10</v>
+        <v>1.03E-10</v>
       </c>
       <c r="K43">
-        <v>7.37e-10</v>
+        <v>7.37E-10</v>
       </c>
       <c r="L43">
-        <v>4.67e-09</v>
+        <v>4.67E-09</v>
       </c>
       <c r="M43">
-        <v>2.66e-08</v>
+        <v>2.66E-08</v>
       </c>
       <c r="N43">
-        <v>1.35e-07</v>
+        <v>1.35E-07</v>
       </c>
       <c r="O43">
-        <v>6.16e-07</v>
+        <v>6.16E-07</v>
       </c>
       <c r="P43">
-        <v>2.49e-06</v>
+        <v>2.49E-06</v>
       </c>
       <c r="Q43">
-        <v>9.07e-06</v>
+        <v>9.07E-06</v>
       </c>
       <c r="R43">
-        <v>2.96e-05</v>
+        <v>2.96E-05</v>
       </c>
       <c r="S43">
         <v>0.000127693</v>
@@ -113513,43 +113513,43 @@
         <v>21</v>
       </c>
       <c r="F44">
-        <v>1.45e-15</v>
+        <v>1.45E-15</v>
       </c>
       <c r="G44">
-        <v>2.05e-13</v>
+        <v>2.05E-13</v>
       </c>
       <c r="H44">
-        <v>1.76e-12</v>
+        <v>1.76E-12</v>
       </c>
       <c r="I44">
-        <v>1.49e-11</v>
+        <v>1.49E-11</v>
       </c>
       <c r="J44">
-        <v>1.13e-10</v>
+        <v>1.13E-10</v>
       </c>
       <c r="K44">
-        <v>7.67e-10</v>
+        <v>7.67E-10</v>
       </c>
       <c r="L44">
-        <v>4.67e-09</v>
+        <v>4.67E-09</v>
       </c>
       <c r="M44">
-        <v>2.56e-08</v>
+        <v>2.56E-08</v>
       </c>
       <c r="N44">
-        <v>1.25e-07</v>
+        <v>1.25E-07</v>
       </c>
       <c r="O44">
-        <v>5.51e-07</v>
+        <v>5.51E-07</v>
       </c>
       <c r="P44">
-        <v>2.18e-06</v>
+        <v>2.18E-06</v>
       </c>
       <c r="Q44">
-        <v>7.77e-06</v>
+        <v>7.77E-06</v>
       </c>
       <c r="R44">
-        <v>2.48e-05</v>
+        <v>2.48E-05</v>
       </c>
       <c r="S44">
         <v>0.000105218</v>

</xml_diff>

<commit_message>
Fleet_control to long format
Easier to read in excel. The model still uses it in wide format. The long format is converted to wide in the clean_data function in the 6_fit_mod script.
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -79229,7 +79229,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -79243,599 +79243,915 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Fleet_code</t>
+          <t>Pollock</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Fleet_type</t>
+          <t>Cod</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Species</t>
+          <t>ATF</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Selectivity_index</t>
+          <t>BT_Pollock</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Selectivity</t>
+          <t>BT_Cod</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Nselages</t>
+          <t>BT_ATF</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Time_varying_sel</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Sel_sd_prior</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Age_first_selected</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Accumatation_age_lower</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Accumatation_age_upper</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Weight1_Numbers2</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Weight_index</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Age_transition_index</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Q_index</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Estimate_q</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Q_prior</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Q_sd_prior</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Time_varying_q</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Time_varying_q_sd_prior</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Estimate_survey_sd</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Survey_sd_prior</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Estimate_catch_sd</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Catch_sd_prior</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Comp_weights</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>proj_F_prop</t>
+          <t>EIT_Pollock</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pollock</t>
-        </is>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <v>20</v>
-      </c>
-      <c r="I2">
-        <v>12.5</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
+          <t>Fleet_code</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cod</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>12.5</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
+          <t>Fleet_type</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ATF</t>
-        </is>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
-      </c>
-      <c r="I4">
-        <v>12.5</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>21</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>1</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
+          <t>Species</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BT_Pollock</t>
-        </is>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>10</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
+          <t>Selectivity_index</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BT_Cod</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>12</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
-      <c r="P6">
-        <v>2</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>1</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
+          <t>Selectivity</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BT_ATF</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>21</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>3</v>
-      </c>
-      <c r="O7">
-        <v>3</v>
-      </c>
-      <c r="P7">
-        <v>3</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>1</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
+          <t>Nselages</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EIT_Pollock</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>10</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>4</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>0.001227838466312996</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
+          <t>Time_varying_sel</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sel_sd_prior</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>12.5</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.0</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Age_first_selected</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Accumatation_age_lower</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Accumatation_age_upper</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Weight1_Numbers2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Weight_index</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Age_transition_index</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Q_index</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Estimate_q</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Q_prior</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1.000000000</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1.000000000</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1.000000000</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.001227838</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Q_sd_prior</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Time_varying_q</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Time_varying_q_sd_prior</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Estimate_survey_sd</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Survey_sd_prior</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Estimate_catch_sd</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Catch_sd_prior</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Comp_weights</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>proj_F_prop</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dirichlet multinomial and env-Q
Added dirichlet multinomial for composition likelihood
- Added "Comp_loglike" to fleet control
- Removed divide by max in selectivity calculation
- Added divide by selected age "Age_max_selected" which can be NA and no normalization happens

Removed accumation age
- Removed "Accumulation_age_upper/lower" from fleet control

Added Rogers et al (2024) catchability parameterization
- "Estimate_q" = 6

Annual/random walk selectivity deviates are no longer "mapped off" when there is no composition data for that year. Same with Q deviates.
- log_sel_slp for logistic is bounded between 0.01 and 10
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -788,12 +788,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Acuumulation_age_lower</t>
+          <t>Comp_loglike</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Ages below this will be grouped to this age for composition data. For example, if set to 2, comp data for age 2 will include 1 and 2 year olds.</t>
+          <t>Composition data distribution (0 = multinomial; 1 = dirichlet-multinomial)</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Acuumulation_age_upper</t>
+          <t>weight1_Numbers2</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Ages above this will be grouped to this age for composition data. For example, if set to 9 for a species with 10 ages, comp data for age 9 will include 9 and 10 year olds.</t>
+          <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
         </is>
       </c>
     </row>
@@ -858,12 +858,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>weight1_Numbers2</t>
+          <t>Weight_index</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
+          <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
         </is>
       </c>
     </row>
@@ -893,12 +893,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Weight_index</t>
+          <t>Age_transition_index</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
+          <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
         </is>
       </c>
     </row>
@@ -928,12 +928,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Age_transition_index</t>
+          <t>Q_index</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
+          <t>index to use if catchability coefficients are to be set the same</t>
         </is>
       </c>
     </row>
@@ -963,12 +963,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Q_index</t>
+          <t>Estimate_q</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>index to use if catchability coefficients are to be set the same</t>
+          <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
         </is>
       </c>
     </row>
@@ -998,12 +998,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Estimate_q</t>
+          <t>Q_prior</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
+          <t>Starting value or fixed value for catchability</t>
         </is>
       </c>
     </row>
@@ -1033,12 +1033,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Q_prior</t>
+          <t>Q_sd_prior</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Starting value or fixed value for catchability</t>
+          <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
         </is>
       </c>
     </row>
@@ -1068,12 +1068,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Q_sd_prior</t>
+          <t>Time_varying_q</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
+          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
         </is>
       </c>
     </row>
@@ -1098,12 +1098,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Time_varying_q</t>
+          <t>Time_varying_q_sd_prior</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
+          <t>The sd to use for the random walk of time varying q if set to 1</t>
         </is>
       </c>
     </row>
@@ -1128,12 +1128,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Time_varying_q_sd_prior</t>
+          <t>Estimate_survey_sd</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>The sd to use for the random walk of time varying q if set to 1</t>
+          <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
         </is>
       </c>
     </row>
@@ -1158,12 +1158,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Estimate_survey_sd</t>
+          <t>Survey_sd_prior</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+          <t>Starting value to be used if Estimate_sigma_index = 1</t>
         </is>
       </c>
     </row>
@@ -1188,12 +1188,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Survey_sd_prior</t>
+          <t>Estimate_catch_sd</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Starting value to be used if Estimate_sigma_index = 1</t>
+          <t>Estimate fishery variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
         </is>
       </c>
     </row>
@@ -1218,12 +1218,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Estimate_catch_sd</t>
+          <t>Catch_sd_prior</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Estimate fishery variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+          <t>Starting value to be used if Estimate_sigma_catch = 1</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Catch_sd_prior</t>
+          <t>Comp_weights</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Starting value to be used if Estimate_sigma_catch = 1</t>
+          <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
         </is>
       </c>
     </row>
@@ -1278,12 +1278,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Comp_weights</t>
+          <t>Catch_units</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
+          <t>Units used for survey: 1 = kg; 2 = numbers</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Catch_units</t>
+          <t>proj_F_prop</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Units used for survey: 1 = kg; 2 = numbers</t>
+          <t>The proportion of future fishing mortality assigned to this fleet</t>
         </is>
       </c>
     </row>
@@ -1334,16 +1334,6 @@
       <c r="E29" t="inlineStr">
         <is>
           <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>proj_F_prop</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>The proportion of future fishing mortality assigned to this fleet</t>
         </is>
       </c>
     </row>
@@ -79229,7 +79219,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -79243,915 +79233,586 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pollock</t>
+          <t>Fleet_code</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cod</t>
+          <t>Fleet_type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ATF</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>BT_Pollock</t>
+          <t>Selectivity_index</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>BT_Cod</t>
+          <t>Selectivity</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>BT_ATF</t>
+          <t>Nselages</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>EIT_Pollock</t>
+          <t>Time_varying_sel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Sel_sd_prior</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Age_first_selected</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Age_max_selected</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Comp_loglike</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Weight1_Numbers2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_index</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Age_transition_index</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Q_index</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Estimate_q</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Q_prior</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Q_sd_prior</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Time_varying_q</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Time_varying_q_sd_prior</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Estimate_survey_sd</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Survey_sd_prior</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Estimate_catch_sd</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Catch_sd_prior</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Comp_weights</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>proj_F_prop</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fleet_code</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+          <t>Pollock</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>12.5</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fleet_type</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+          <t>Cod</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>12.5</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>ATF</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>12.5</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Selectivity_index</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+          <t>BT_Pollock</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Selectivity</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>BT_Cod</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nselages</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8</t>
-        </is>
+          <t>BT_ATF</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Time_varying_sel</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+          <t>EIT_Pollock</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0.001227838</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sel_sd_prior</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Age_first_selected</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Accumatation_age_lower</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Accumatation_age_upper</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Weight1_Numbers2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Weight_index</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Age_transition_index</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Q_index</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 3</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Estimate_q</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Q_prior</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>1.000000000</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>1.000000000</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>1.000000000</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0.001227838</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Q_sd_prior</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Time_varying_q</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Time_varying_q_sd_prior</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Estimate_survey_sd</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Survey_sd_prior</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Estimate_catch_sd</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Catch_sd_prior</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Comp_weights</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>proj_F_prop</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added suitability calculation across specific years
suit_styr and suit_endyr are now adjust in "fit_mod"
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -21991,7 +21991,7 @@
         <v>20</v>
       </c>
       <c r="I62">
-        <v>0.09895631000000001</v>
+        <v>0.1160922</v>
       </c>
     </row>
     <row r="63">
@@ -22020,7 +22020,7 @@
         <v>20</v>
       </c>
       <c r="I63">
-        <v>0.01757422</v>
+        <v>0.000438354</v>
       </c>
     </row>
     <row r="64">
@@ -24079,7 +24079,7 @@
         <v>20</v>
       </c>
       <c r="I134">
-        <v>0.1671799</v>
+        <v>0.1830541</v>
       </c>
     </row>
     <row r="135">
@@ -24108,7 +24108,7 @@
         <v>20</v>
       </c>
       <c r="I135">
-        <v>0.01558352</v>
+        <v>0.001093588</v>
       </c>
     </row>
     <row r="136">
@@ -24166,7 +24166,7 @@
         <v>20</v>
       </c>
       <c r="I137">
-        <v>0.001442203</v>
+        <v>5.7E-05</v>
       </c>
     </row>
     <row r="138">
@@ -24311,7 +24311,7 @@
         <v>20</v>
       </c>
       <c r="I142">
-        <v>0.000840243</v>
+        <v>0.00084119</v>
       </c>
     </row>
     <row r="143">
@@ -36259,7 +36259,7 @@
         <v>20</v>
       </c>
       <c r="I554">
-        <v>0.06434811999999999</v>
+        <v>0.0658436</v>
       </c>
     </row>
     <row r="555">
@@ -36288,7 +36288,7 @@
         <v>20</v>
       </c>
       <c r="I555">
-        <v>0.001566085</v>
+        <v>7.059999999999999E-05</v>
       </c>
     </row>
     <row r="556">
@@ -36607,7 +36607,7 @@
         <v>20</v>
       </c>
       <c r="I566">
-        <v>0.04192643</v>
+        <v>0.06627416999999999</v>
       </c>
     </row>
     <row r="567">
@@ -36636,7 +36636,7 @@
         <v>20</v>
       </c>
       <c r="I567">
-        <v>0.01933132</v>
+        <v>0.003654754</v>
       </c>
     </row>
     <row r="568">
@@ -36665,7 +36665,7 @@
         <v>20</v>
       </c>
       <c r="I568">
-        <v>0.008836656999999999</v>
+        <v>0.000912173</v>
       </c>
     </row>
     <row r="569">
@@ -36694,7 +36694,7 @@
         <v>20</v>
       </c>
       <c r="I569">
-        <v>0.000810988</v>
+        <v>6.43E-05</v>
       </c>
     </row>
     <row r="570">
@@ -36955,7 +36955,7 @@
         <v>20</v>
       </c>
       <c r="I578">
-        <v>0.06092329</v>
+        <v>0.1287927</v>
       </c>
     </row>
     <row r="579">
@@ -36984,7 +36984,7 @@
         <v>20</v>
       </c>
       <c r="I579">
-        <v>0.06295646000000001</v>
+        <v>0.02520688</v>
       </c>
     </row>
     <row r="580">
@@ -37013,7 +37013,7 @@
         <v>20</v>
       </c>
       <c r="I580">
-        <v>0.02601113</v>
+        <v>0.007526698</v>
       </c>
     </row>
     <row r="581">
@@ -37042,7 +37042,7 @@
         <v>20</v>
       </c>
       <c r="I581">
-        <v>0.01165385</v>
+        <v>0.002320946</v>
       </c>
     </row>
     <row r="582">
@@ -37071,7 +37071,7 @@
         <v>20</v>
       </c>
       <c r="I582">
-        <v>0.001213887</v>
+        <v>0.000252341</v>
       </c>
     </row>
     <row r="583">
@@ -37100,7 +37100,7 @@
         <v>20</v>
       </c>
       <c r="I583">
-        <v>0.001600401</v>
+        <v>0.000259407</v>
       </c>
     </row>
     <row r="584">
@@ -37303,7 +37303,7 @@
         <v>20</v>
       </c>
       <c r="I590">
-        <v>0.0737371</v>
+        <v>0.1971279</v>
       </c>
     </row>
     <row r="591">
@@ -37332,7 +37332,7 @@
         <v>20</v>
       </c>
       <c r="I591">
-        <v>0.1060799</v>
+        <v>0.06845544000000001</v>
       </c>
     </row>
     <row r="592">
@@ -37361,7 +37361,7 @@
         <v>20</v>
       </c>
       <c r="I592">
-        <v>0.05921873</v>
+        <v>0.02587423</v>
       </c>
     </row>
     <row r="593">
@@ -37390,7 +37390,7 @@
         <v>20</v>
       </c>
       <c r="I593">
-        <v>0.04687594</v>
+        <v>0.01608599</v>
       </c>
     </row>
     <row r="594">
@@ -37419,7 +37419,7 @@
         <v>20</v>
       </c>
       <c r="I594">
-        <v>0.01285107</v>
+        <v>0.003715812</v>
       </c>
     </row>
     <row r="595">
@@ -37448,7 +37448,7 @@
         <v>20</v>
       </c>
       <c r="I595">
-        <v>0.007953175</v>
+        <v>0.002079272</v>
       </c>
     </row>
     <row r="596">
@@ -37477,7 +37477,7 @@
         <v>20</v>
       </c>
       <c r="I596">
-        <v>0.003801258</v>
+        <v>0.000675308</v>
       </c>
     </row>
     <row r="597">
@@ -37506,7 +37506,7 @@
         <v>20</v>
       </c>
       <c r="I597">
-        <v>0.001889661</v>
+        <v>0.000284664</v>
       </c>
     </row>
     <row r="598">
@@ -37535,7 +37535,7 @@
         <v>20</v>
       </c>
       <c r="I598">
-        <v>0.00237092</v>
+        <v>0.000479177</v>
       </c>
     </row>
     <row r="599">
@@ -37651,7 +37651,7 @@
         <v>20</v>
       </c>
       <c r="I602">
-        <v>0.06835767</v>
+        <v>0.2085426</v>
       </c>
     </row>
     <row r="603">
@@ -37680,7 +37680,7 @@
         <v>20</v>
       </c>
       <c r="I603">
-        <v>0.1231417</v>
+        <v>0.1185247</v>
       </c>
     </row>
     <row r="604">
@@ -37709,7 +37709,7 @@
         <v>20</v>
       </c>
       <c r="I604">
-        <v>0.1109186</v>
+        <v>0.06767671</v>
       </c>
     </row>
     <row r="605">
@@ -37738,7 +37738,7 @@
         <v>20</v>
       </c>
       <c r="I605">
-        <v>0.06913402</v>
+        <v>0.03316386</v>
       </c>
     </row>
     <row r="606">
@@ -37767,7 +37767,7 @@
         <v>20</v>
       </c>
       <c r="I606">
-        <v>0.03073256</v>
+        <v>0.01119253</v>
       </c>
     </row>
     <row r="607">
@@ -37796,7 +37796,7 @@
         <v>20</v>
       </c>
       <c r="I607">
-        <v>0.02015729</v>
+        <v>0.007328285</v>
       </c>
     </row>
     <row r="608">
@@ -37825,7 +37825,7 @@
         <v>20</v>
       </c>
       <c r="I608">
-        <v>0.01056381</v>
+        <v>0.003050313</v>
       </c>
     </row>
     <row r="609">
@@ -37854,7 +37854,7 @@
         <v>20</v>
       </c>
       <c r="I609">
-        <v>0.009181873</v>
+        <v>0.00256464</v>
       </c>
     </row>
     <row r="610">
@@ -37883,7 +37883,7 @@
         <v>20</v>
       </c>
       <c r="I610">
-        <v>0.004431573</v>
+        <v>0.001210306</v>
       </c>
     </row>
     <row r="611">
@@ -37970,7 +37970,7 @@
         <v>20</v>
       </c>
       <c r="I613">
-        <v>0.008167178000000001</v>
+        <v>0.001532236</v>
       </c>
     </row>
     <row r="614">
@@ -37999,7 +37999,7 @@
         <v>20</v>
       </c>
       <c r="I614">
-        <v>0.06848643</v>
+        <v>0.2322304</v>
       </c>
     </row>
     <row r="615">
@@ -38028,7 +38028,7 @@
         <v>20</v>
       </c>
       <c r="I615">
-        <v>0.1529236</v>
+        <v>0.1552988</v>
       </c>
     </row>
     <row r="616">
@@ -38057,7 +38057,7 @@
         <v>20</v>
       </c>
       <c r="I616">
-        <v>0.1479175</v>
+        <v>0.09657167</v>
       </c>
     </row>
     <row r="617">
@@ -38086,7 +38086,7 @@
         <v>20</v>
       </c>
       <c r="I617">
-        <v>0.08964778</v>
+        <v>0.04334795</v>
       </c>
     </row>
     <row r="618">
@@ -38115,7 +38115,7 @@
         <v>20</v>
       </c>
       <c r="I618">
-        <v>0.00912228</v>
+        <v>0.004000702</v>
       </c>
     </row>
     <row r="619">
@@ -38144,7 +38144,7 @@
         <v>20</v>
       </c>
       <c r="I619">
-        <v>0.0184799</v>
+        <v>0.006899033</v>
       </c>
     </row>
     <row r="620">
@@ -38173,7 +38173,7 @@
         <v>20</v>
       </c>
       <c r="I620">
-        <v>0.02597683</v>
+        <v>0.007913598000000001</v>
       </c>
     </row>
     <row r="621">
@@ -38202,7 +38202,7 @@
         <v>20</v>
       </c>
       <c r="I621">
-        <v>0.00460747</v>
+        <v>0.001411937</v>
       </c>
     </row>
     <row r="622">
@@ -38231,7 +38231,7 @@
         <v>20</v>
       </c>
       <c r="I622">
-        <v>0.01911641</v>
+        <v>0.004818165</v>
       </c>
     </row>
     <row r="623">
@@ -38318,7 +38318,7 @@
         <v>20</v>
       </c>
       <c r="I625">
-        <v>0.02015185</v>
+        <v>0.003937767</v>
       </c>
     </row>
     <row r="626">
@@ -38347,7 +38347,7 @@
         <v>20</v>
       </c>
       <c r="I626">
-        <v>0.079945</v>
+        <v>0.2639951</v>
       </c>
     </row>
     <row r="627">
@@ -38376,7 +38376,7 @@
         <v>20</v>
       </c>
       <c r="I627">
-        <v>0.1146123</v>
+        <v>0.1223224</v>
       </c>
     </row>
     <row r="628">
@@ -38405,7 +38405,7 @@
         <v>20</v>
       </c>
       <c r="I628">
-        <v>0.1166548</v>
+        <v>0.08598292</v>
       </c>
     </row>
     <row r="629">
@@ -38434,7 +38434,7 @@
         <v>20</v>
       </c>
       <c r="I629">
-        <v>0.1726959</v>
+        <v>0.09711562</v>
       </c>
     </row>
     <row r="630">
@@ -38463,7 +38463,7 @@
         <v>20</v>
       </c>
       <c r="I630">
-        <v>0.02629317</v>
+        <v>0.0121136</v>
       </c>
     </row>
     <row r="631">
@@ -38492,7 +38492,7 @@
         <v>20</v>
       </c>
       <c r="I631">
-        <v>0.0124982</v>
+        <v>0.00492871</v>
       </c>
     </row>
     <row r="632">
@@ -38521,7 +38521,7 @@
         <v>20</v>
       </c>
       <c r="I632">
-        <v>0.04184531</v>
+        <v>0.01514183</v>
       </c>
     </row>
     <row r="633">
@@ -38550,7 +38550,7 @@
         <v>20</v>
       </c>
       <c r="I633">
-        <v>0.01688839</v>
+        <v>0.005492585</v>
       </c>
     </row>
     <row r="634">
@@ -38579,7 +38579,7 @@
         <v>20</v>
       </c>
       <c r="I634">
-        <v>0.03582364</v>
+        <v>0.01016395</v>
       </c>
     </row>
     <row r="635">
@@ -38695,7 +38695,7 @@
         <v>20</v>
       </c>
       <c r="I638">
-        <v>0.03533393</v>
+        <v>0.1688953</v>
       </c>
     </row>
     <row r="639">
@@ -38724,7 +38724,7 @@
         <v>20</v>
       </c>
       <c r="I639">
-        <v>0.1695959</v>
+        <v>0.2031515</v>
       </c>
     </row>
     <row r="640">
@@ -38753,7 +38753,7 @@
         <v>20</v>
       </c>
       <c r="I640">
-        <v>0.1858036</v>
+        <v>0.1452255</v>
       </c>
     </row>
     <row r="641">
@@ -38782,7 +38782,7 @@
         <v>20</v>
       </c>
       <c r="I641">
-        <v>0.1012309</v>
+        <v>0.06140649</v>
       </c>
     </row>
     <row r="642">
@@ -38811,7 +38811,7 @@
         <v>20</v>
       </c>
       <c r="I642">
-        <v>0.07454122000000001</v>
+        <v>0.03633095</v>
       </c>
     </row>
     <row r="643">
@@ -38840,7 +38840,7 @@
         <v>20</v>
       </c>
       <c r="I643">
-        <v>0.04729706</v>
+        <v>0.02071951</v>
       </c>
     </row>
     <row r="644">
@@ -38869,7 +38869,7 @@
         <v>20</v>
       </c>
       <c r="I644">
-        <v>0.02177258</v>
+        <v>0.007774862</v>
       </c>
     </row>
     <row r="645">
@@ -38898,7 +38898,7 @@
         <v>20</v>
       </c>
       <c r="I645">
-        <v>0.01187798</v>
+        <v>0.003949147</v>
       </c>
     </row>
     <row r="646">
@@ -39043,7 +39043,7 @@
         <v>20</v>
       </c>
       <c r="I650">
-        <v>0.04425346</v>
+        <v>0.1918666</v>
       </c>
     </row>
     <row r="651">
@@ -39072,7 +39072,7 @@
         <v>20</v>
       </c>
       <c r="I651">
-        <v>0.1181582</v>
+        <v>0.1517578</v>
       </c>
     </row>
     <row r="652">
@@ -39101,7 +39101,7 @@
         <v>20</v>
       </c>
       <c r="I652">
-        <v>0.1634665</v>
+        <v>0.1367914</v>
       </c>
     </row>
     <row r="653">
@@ -39130,7 +39130,7 @@
         <v>20</v>
       </c>
       <c r="I653">
-        <v>0.1817283</v>
+        <v>0.1137431</v>
       </c>
     </row>
     <row r="654">
@@ -39159,7 +39159,7 @@
         <v>20</v>
       </c>
       <c r="I654">
-        <v>0.0443987</v>
+        <v>0.02065319</v>
       </c>
     </row>
     <row r="655">
@@ -39188,7 +39188,7 @@
         <v>20</v>
       </c>
       <c r="I655">
-        <v>0.04550604</v>
+        <v>0.02185077</v>
       </c>
     </row>
     <row r="656">
@@ -39246,7 +39246,7 @@
         <v>20</v>
       </c>
       <c r="I657">
-        <v>0.03757834</v>
+        <v>0.01496637</v>
       </c>
     </row>
     <row r="658">
@@ -39333,7 +39333,7 @@
         <v>20</v>
       </c>
       <c r="I660">
-        <v>0.02402286</v>
+        <v>0.007483185</v>
       </c>
     </row>
     <row r="661">
@@ -39391,7 +39391,7 @@
         <v>20</v>
       </c>
       <c r="I662">
-        <v>0.05095513</v>
+        <v>0.1181772</v>
       </c>
     </row>
     <row r="663">
@@ -39420,7 +39420,7 @@
         <v>20</v>
       </c>
       <c r="I663">
-        <v>0.1701628</v>
+        <v>0.22574</v>
       </c>
     </row>
     <row r="664">
@@ -39449,7 +39449,7 @@
         <v>20</v>
       </c>
       <c r="I664">
-        <v>0.1643761</v>
+        <v>0.1511225</v>
       </c>
     </row>
     <row r="665">
@@ -39478,7 +39478,7 @@
         <v>20</v>
       </c>
       <c r="I665">
-        <v>0.1826878</v>
+        <v>0.1175091</v>
       </c>
     </row>
     <row r="666">
@@ -39507,7 +39507,7 @@
         <v>20</v>
       </c>
       <c r="I666">
-        <v>0.07907031</v>
+        <v>0.04194785</v>
       </c>
     </row>
     <row r="667">
@@ -39565,7 +39565,7 @@
         <v>20</v>
       </c>
       <c r="I668">
-        <v>0.01396714</v>
+        <v>0.006722677</v>
       </c>
     </row>
     <row r="669">
@@ -39739,7 +39739,7 @@
         <v>20</v>
       </c>
       <c r="I674">
-        <v>0.0725937</v>
+        <v>0.1633956</v>
       </c>
     </row>
     <row r="675">
@@ -39768,7 +39768,7 @@
         <v>20</v>
       </c>
       <c r="I675">
-        <v>0.1477411</v>
+        <v>0.1672041</v>
       </c>
     </row>
     <row r="676">
@@ -39797,7 +39797,7 @@
         <v>20</v>
       </c>
       <c r="I676">
-        <v>0.1939442</v>
+        <v>0.1674946</v>
       </c>
     </row>
     <row r="677">
@@ -39826,7 +39826,7 @@
         <v>20</v>
       </c>
       <c r="I677">
-        <v>0.094915</v>
+        <v>0.06975533</v>
       </c>
     </row>
     <row r="678">
@@ -39855,7 +39855,7 @@
         <v>20</v>
       </c>
       <c r="I678">
-        <v>0.0395418</v>
+        <v>0.02493934</v>
       </c>
     </row>
     <row r="679">
@@ -39884,7 +39884,7 @@
         <v>20</v>
       </c>
       <c r="I679">
-        <v>0.05360619</v>
+        <v>0.02858403</v>
       </c>
     </row>
     <row r="680">
@@ -39913,7 +39913,7 @@
         <v>20</v>
       </c>
       <c r="I680">
-        <v>0.01385679</v>
+        <v>0.008423683</v>
       </c>
     </row>
     <row r="681">
@@ -39942,7 +39942,7 @@
         <v>20</v>
       </c>
       <c r="I681">
-        <v>0.03109857</v>
+        <v>0.02582586</v>
       </c>
     </row>
     <row r="682">
@@ -40029,7 +40029,7 @@
         <v>20</v>
       </c>
       <c r="I684">
-        <v>0.003631901</v>
+        <v>0.001392789</v>
       </c>
     </row>
     <row r="685">
@@ -40058,7 +40058,7 @@
         <v>20</v>
       </c>
       <c r="I685">
-        <v>0.008198973999999999</v>
+        <v>0.002112835</v>
       </c>
     </row>
     <row r="686">
@@ -41479,7 +41479,7 @@
         <v>20</v>
       </c>
       <c r="I734">
-        <v>0.006490083</v>
+        <v>0.006756326</v>
       </c>
     </row>
     <row r="735">
@@ -41508,7 +41508,7 @@
         <v>20</v>
       </c>
       <c r="I735">
-        <v>0.000448463</v>
+        <v>0.000182219</v>
       </c>
     </row>
     <row r="736">
@@ -41827,7 +41827,7 @@
         <v>20</v>
       </c>
       <c r="I746">
-        <v>0.002665869</v>
+        <v>0.006608447</v>
       </c>
     </row>
     <row r="747">
@@ -41856,7 +41856,7 @@
         <v>20</v>
       </c>
       <c r="I747">
-        <v>0.005991087</v>
+        <v>0.00204851</v>
       </c>
     </row>
     <row r="748">
@@ -46699,7 +46699,7 @@
         <v>20</v>
       </c>
       <c r="I914">
-        <v>0.000629519</v>
+        <v>0.001097397</v>
       </c>
     </row>
     <row r="915">
@@ -46757,7 +46757,7 @@
         <v>20</v>
       </c>
       <c r="I916">
-        <v>0.000943856</v>
+        <v>0.000475979</v>
       </c>
     </row>
     <row r="917">
@@ -54355,7 +54355,7 @@
         <v>20</v>
       </c>
       <c r="I1178">
-        <v>0.5632433999999999</v>
+        <v>0.583677</v>
       </c>
     </row>
     <row r="1179">
@@ -54384,7 +54384,7 @@
         <v>20</v>
       </c>
       <c r="I1179">
-        <v>0.02713798</v>
+        <v>0.006704278</v>
       </c>
     </row>
     <row r="1180">
@@ -54703,7 +54703,7 @@
         <v>20</v>
       </c>
       <c r="I1190">
-        <v>0.5120078</v>
+        <v>0.5677733</v>
       </c>
     </row>
     <row r="1191">
@@ -54732,7 +54732,7 @@
         <v>20</v>
       </c>
       <c r="I1191">
-        <v>0.07698066000000001</v>
+        <v>0.02121515</v>
       </c>
     </row>
     <row r="1192">
@@ -55051,7 +55051,7 @@
         <v>20</v>
       </c>
       <c r="I1202">
-        <v>0.2418501</v>
+        <v>0.4521797</v>
       </c>
     </row>
     <row r="1203">
@@ -55080,7 +55080,7 @@
         <v>20</v>
       </c>
       <c r="I1203">
-        <v>0.2569941</v>
+        <v>0.1121228</v>
       </c>
     </row>
     <row r="1204">
@@ -55109,7 +55109,7 @@
         <v>20</v>
       </c>
       <c r="I1204">
-        <v>0.05196077</v>
+        <v>0.01789932</v>
       </c>
     </row>
     <row r="1205">
@@ -55196,7 +55196,7 @@
         <v>20</v>
       </c>
       <c r="I1207">
-        <v>0.04054731</v>
+        <v>0.009150439</v>
       </c>
     </row>
     <row r="1208">
@@ -55399,7 +55399,7 @@
         <v>20</v>
       </c>
       <c r="I1214">
-        <v>0.2231361</v>
+        <v>0.4195472</v>
       </c>
     </row>
     <row r="1215">
@@ -55428,7 +55428,7 @@
         <v>20</v>
       </c>
       <c r="I1215">
-        <v>0.2635833</v>
+        <v>0.1385076</v>
       </c>
     </row>
     <row r="1216">
@@ -55457,7 +55457,7 @@
         <v>20</v>
       </c>
       <c r="I1216">
-        <v>0.1124028</v>
+        <v>0.0410674</v>
       </c>
     </row>
     <row r="1217">
@@ -55747,7 +55747,7 @@
         <v>20</v>
       </c>
       <c r="I1226">
-        <v>0.1915963</v>
+        <v>0.4157468</v>
       </c>
     </row>
     <row r="1227">
@@ -55776,7 +55776,7 @@
         <v>20</v>
       </c>
       <c r="I1227">
-        <v>0.3511788</v>
+        <v>0.1771132</v>
       </c>
     </row>
     <row r="1228">
@@ -55805,7 +55805,7 @@
         <v>20</v>
       </c>
       <c r="I1228">
-        <v>0.06721526</v>
+        <v>0.01713039</v>
       </c>
     </row>
     <row r="1229">
@@ -56095,7 +56095,7 @@
         <v>20</v>
       </c>
       <c r="I1238">
-        <v>0.1041778</v>
+        <v>0.2824108</v>
       </c>
     </row>
     <row r="1239">
@@ -56124,7 +56124,7 @@
         <v>20</v>
       </c>
       <c r="I1239">
-        <v>0.2576952</v>
+        <v>0.2015811</v>
       </c>
     </row>
     <row r="1240">
@@ -56153,7 +56153,7 @@
         <v>20</v>
       </c>
       <c r="I1240">
-        <v>0.1405023</v>
+        <v>0.08620998000000001</v>
       </c>
     </row>
     <row r="1241">
@@ -56182,7 +56182,7 @@
         <v>20</v>
       </c>
       <c r="I1241">
-        <v>0.1182218</v>
+        <v>0.05039527</v>
       </c>
     </row>
     <row r="1242">
@@ -56443,7 +56443,7 @@
         <v>20</v>
       </c>
       <c r="I1250">
-        <v>0.2159569</v>
+        <v>0.3930405</v>
       </c>
     </row>
     <row r="1251">
@@ -56472,7 +56472,7 @@
         <v>20</v>
       </c>
       <c r="I1251">
-        <v>0.2457174</v>
+        <v>0.1572162</v>
       </c>
     </row>
     <row r="1252">
@@ -56501,7 +56501,7 @@
         <v>20</v>
       </c>
       <c r="I1252">
-        <v>0.1671905</v>
+        <v>0.0786081</v>
       </c>
     </row>
     <row r="1253">
@@ -56791,7 +56791,7 @@
         <v>20</v>
       </c>
       <c r="I1262">
-        <v>0.1160984</v>
+        <v>0.2883931</v>
       </c>
     </row>
     <row r="1263">
@@ -56820,7 +56820,7 @@
         <v>20</v>
       </c>
       <c r="I1263">
-        <v>0.1239925</v>
+        <v>0.1153572</v>
       </c>
     </row>
     <row r="1264">
@@ -56849,7 +56849,7 @@
         <v>20</v>
       </c>
       <c r="I1264">
-        <v>0.3943739</v>
+        <v>0.2307145</v>
       </c>
     </row>
     <row r="1265">
@@ -57139,7 +57139,7 @@
         <v>20</v>
       </c>
       <c r="I1274">
-        <v>0.04485665</v>
+        <v>0.1417422</v>
       </c>
     </row>
     <row r="1275">
@@ -57168,7 +57168,7 @@
         <v>20</v>
       </c>
       <c r="I1275">
-        <v>0.1077685</v>
+        <v>0.1417422</v>
       </c>
     </row>
     <row r="1276">
@@ -57197,7 +57197,7 @@
         <v>20</v>
       </c>
       <c r="I1276">
-        <v>0.4852147</v>
+        <v>0.3543555</v>
       </c>
     </row>
     <row r="1277">
@@ -57487,7 +57487,7 @@
         <v>20</v>
       </c>
       <c r="I1286">
-        <v>0.2297915</v>
+        <v>0.3838252</v>
       </c>
     </row>
     <row r="1287">
@@ -57516,7 +57516,7 @@
         <v>20</v>
       </c>
       <c r="I1287">
-        <v>0.1184886</v>
+        <v>0.1279417</v>
       </c>
     </row>
     <row r="1288">
@@ -57574,7 +57574,7 @@
         <v>20</v>
       </c>
       <c r="I1289">
-        <v>0.2914285</v>
+        <v>0.1279417</v>
       </c>
     </row>
     <row r="1290">
@@ -58183,7 +58183,7 @@
         <v>20</v>
       </c>
       <c r="I1310">
-        <v>0.08334769</v>
+        <v>0.1831537</v>
       </c>
     </row>
     <row r="1311">
@@ -58212,7 +58212,7 @@
         <v>20</v>
       </c>
       <c r="I1311">
-        <v>0.5576903</v>
+        <v>0.4578843</v>
       </c>
     </row>
     <row r="1312">
@@ -58531,7 +58531,7 @@
         <v>20</v>
       </c>
       <c r="I1322">
-        <v>0.04358869</v>
+        <v>0.1056715</v>
       </c>
     </row>
     <row r="1323">
@@ -58560,7 +58560,7 @@
         <v>20</v>
       </c>
       <c r="I1323">
-        <v>0.1765899</v>
+        <v>0.1819958</v>
       </c>
     </row>
     <row r="1324">
@@ -58589,7 +58589,7 @@
         <v>20</v>
       </c>
       <c r="I1324">
-        <v>0.1990513</v>
+        <v>0.2057152</v>
       </c>
     </row>
     <row r="1325">
@@ -58618,7 +58618,7 @@
         <v>20</v>
       </c>
       <c r="I1325">
-        <v>0.1524309</v>
+        <v>0.1127349</v>
       </c>
     </row>
     <row r="1326">
@@ -58647,7 +58647,7 @@
         <v>20</v>
       </c>
       <c r="I1326">
-        <v>0.02514058</v>
+        <v>0.0112851</v>
       </c>
     </row>
     <row r="1327">
@@ -58676,7 +58676,7 @@
         <v>20</v>
       </c>
       <c r="I1327">
-        <v>0.04425274</v>
+        <v>0.02365166</v>
       </c>
     </row>
     <row r="1328">
@@ -65839,7 +65839,7 @@
         <v>20</v>
       </c>
       <c r="I1574">
-        <v>0.00298037</v>
+        <v>0.00707053</v>
       </c>
     </row>
     <row r="1575">
@@ -65868,7 +65868,7 @@
         <v>20</v>
       </c>
       <c r="I1575">
-        <v>0.01116069</v>
+        <v>0.00707053</v>
       </c>
     </row>
     <row r="1576">
@@ -79022,7 +79022,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>2060</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
plot stock recruit fix
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -788,12 +788,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Comp_loglike</t>
+          <t>Age_max_selected</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Composition data distribution (0 = multinomial; 1 = dirichlet-multinomial)</t>
+          <t>Age at which selectivity = 1. If NA, it will not normalize selectivity. If &lt; 0, will normalize selectivity by the max.</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>weight1_Numbers2</t>
+          <t>Comp_loglike</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
+          <t>Composition data distribution (0 = multinomial; 1 = dirichlet-multinomial)</t>
         </is>
       </c>
     </row>
@@ -858,12 +858,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Weight_index</t>
+          <t>weight1_Numbers2</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
+          <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
         </is>
       </c>
     </row>
@@ -893,12 +893,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Age_transition_index</t>
+          <t>Weight_index</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
+          <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
         </is>
       </c>
     </row>
@@ -928,12 +928,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Q_index</t>
+          <t>Age_transition_index</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>index to use if catchability coefficients are to be set the same</t>
+          <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
         </is>
       </c>
     </row>
@@ -963,12 +963,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Estimate_q</t>
+          <t>Q_index</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
+          <t>index to use if catchability coefficients are to be set the same</t>
         </is>
       </c>
     </row>
@@ -998,12 +998,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Q_prior</t>
+          <t>Estimate_q</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Starting value or fixed value for catchability</t>
+          <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
         </is>
       </c>
     </row>
@@ -1033,12 +1033,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Q_sd_prior</t>
+          <t>Q_prior</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
+          <t>Starting value or fixed value for catchability</t>
         </is>
       </c>
     </row>
@@ -1068,12 +1068,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Time_varying_q</t>
+          <t>Q_sd_prior</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
+          <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
         </is>
       </c>
     </row>
@@ -1098,12 +1098,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Time_varying_q_sd_prior</t>
+          <t>Time_varying_q</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>The sd to use for the random walk of time varying q if set to 1</t>
+          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
         </is>
       </c>
     </row>
@@ -1128,12 +1128,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Estimate_survey_sd</t>
+          <t>Time_varying_q_sd_prior</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Estimate survey variance (0 = use CV from index_data, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+          <t>The sd to use for the random walk of time varying q if set to 1</t>
         </is>
       </c>
     </row>
@@ -1158,12 +1158,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Survey_sd_prior</t>
+          <t>Estimate_survey_sd</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Starting value to be used if Estimate_sigma_index = 1</t>
+          <t>Estimate survey variance (0 = use CV from index_data, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
         </is>
       </c>
     </row>
@@ -1188,12 +1188,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Estimate_catch_sd</t>
+          <t>Survey_sd_prior</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Estimate fishery variance (0 = use CV from index_data, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+          <t>Starting value to be used if Estimate_sigma_index = 1</t>
         </is>
       </c>
     </row>
@@ -1218,12 +1218,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Catch_sd_prior</t>
+          <t>Estimate_catch_sd</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Starting value to be used if Estimate_sigma_catch = 1</t>
+          <t>Estimate fishery variance (0 = use CV from index_data, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Comp_weights</t>
+          <t>Catch_sd_prior</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
+          <t>Starting value to be used if Estimate_sigma_catch = 1</t>
         </is>
       </c>
     </row>
@@ -1278,12 +1278,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Catch_units</t>
+          <t>Comp_weights</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Units used for survey: 1 = kg; 2 = numbers</t>
+          <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>proj_F_prop</t>
+          <t>Catch_units</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>The proportion of future fishing mortality assigned to this fleet</t>
+          <t>Units used for survey: 1 = kg; 2 = numbers</t>
         </is>
       </c>
     </row>
@@ -1336,6 +1336,16 @@
           <t>fleet_control</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>proj_F_prop</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>The proportion of future fishing mortality assigned to this fleet</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -1351,14 +1361,9 @@
           <t>Percent female at age for each species</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>sex codes: 0=combined; 1=use female only; 2=use male only; 3 = joint female and male</t>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
         </is>
       </c>
     </row>
@@ -1374,6 +1379,16 @@
       <c r="D31" t="inlineStr">
         <is>
           <t>Residual natural mortality for each species</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>sex codes: 0=combined; 1=use female only; 2=use male only; 3 = joint female and male</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
names and update examples and suitability estimation
stom_prop -> diet
wt -> weight
pmature -> maturity

added data checks
EBS_projections giving some issues

added in suitability estimation
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -17,15 +17,14 @@
     <sheet name="NByageFixed" sheetId="8" r:id="rId8"/>
     <sheet name="age_trans_matrix" sheetId="9" r:id="rId9"/>
     <sheet name="age_error" sheetId="10" r:id="rId10"/>
-    <sheet name="wt" sheetId="11" r:id="rId11"/>
-    <sheet name="pmature" sheetId="12" r:id="rId12"/>
+    <sheet name="weight" sheetId="11" r:id="rId11"/>
+    <sheet name="maturity" sheetId="12" r:id="rId12"/>
     <sheet name="sex_ratio" sheetId="13" r:id="rId13"/>
     <sheet name="M1_base" sheetId="14" r:id="rId14"/>
-    <sheet name="aLW" sheetId="15" r:id="rId15"/>
-    <sheet name="bioenergetics_control" sheetId="16" r:id="rId16"/>
-    <sheet name="env_data" sheetId="17" r:id="rId17"/>
-    <sheet name="Pyrs" sheetId="18" r:id="rId18"/>
-    <sheet name="stom_prop_data" sheetId="19" r:id="rId19"/>
+    <sheet name="bioenergetics_control" sheetId="15" r:id="rId15"/>
+    <sheet name="env_data" sheetId="16" r:id="rId16"/>
+    <sheet name="Pyrs" sheetId="17" r:id="rId17"/>
+    <sheet name="diet_data" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -369,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,7 +623,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -633,12 +632,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R_sexr</t>
+          <t>nages</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Numeric: percent of recruitment that is female (ignored if nsex = 1)</t>
+          <t>Integer: number of ages of each species included in the hindcast</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -659,7 +658,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -668,12 +667,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>nages</t>
+          <t>minage</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Integer: number of ages of each species included in the hindcast</t>
+          <t>Numeric: minimum age for each population (i.e.does recruitment correspond to age 0, 1, 2?)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -694,7 +693,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -703,12 +702,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>minage</t>
+          <t>nlengths</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Numeric: minimum age for each population (i.e.does recruitment correspond to age 0, 1, 2?)</t>
+          <t>Integer: number of lengths of each species included in the hindcast</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -729,7 +728,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -738,12 +737,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>nlengths</t>
+          <t>pop_wt_index</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Integer: number of lengths of each species included in the hindcast</t>
+          <t>Integer: weight-at-age (wt) index to use for calculation of each species population derived quantities (SSB, Consumption/Ration, Suitability, etc)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -764,7 +763,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -773,12 +772,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>pop_wt_index</t>
+          <t>ssb_wt_index</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Integer: weight-at-age (wt) index to use for calculation of each species population derived quantities (SSB, Consumption/Ration, Suitability, etc)</t>
+          <t>Integer: weight-at-age (wt) index to use for calculation of each species spawning biomass</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -799,7 +798,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -808,12 +807,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ssb_wt_index</t>
+          <t>pop_age_transition_index</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Integer: weight-at-age (wt) index to use for calculation of each species spawning biomass</t>
+          <t>Integer: age transition matrix (e.g. growth trajectory) index to use for derived quantities of the population to convert age to length (also used in length-based predation estimation)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -834,7 +833,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -843,12 +842,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>pop_age_transition_index</t>
+          <t>sigma_rec_prior</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Integer: age transition matrix (e.g. growth trajectory) index to use for derived quantities of the population to convert age to length (also used in length-based predation estimation)</t>
+          <t>Numeric: fixed or initial value of standard deviation for recruitment deviates</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -869,7 +868,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -878,12 +877,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>sigma_rec_prior</t>
+          <t>other_food</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Numeric: fixed or initial value of standard deviation for recruitment deviates</t>
+          <t>Numeric: other food in the ecosystem for each species (kg)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -904,7 +903,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -913,12 +912,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>other_food</t>
+          <t>estDynamics</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Numeric: other food in the ecosystem for each species (kg)</t>
+          <t>Integer: switch to estimate or fix numbers-at-age: 0 = estimate dynamics, 1 = use input numbers-at-age in NbyageFixed, 2 = multiply input numbers-at-age (NbyageFixed) by a single scaling coefficient, 3 = multiply input numbers-at-age (NbyageFixed) by age specific scaling coefficient.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -939,21 +938,16 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
+        <v>13</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>estDynamics</t>
+          <t>fleet_control</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Integer: switch to estimate or fix numbers-at-age: 0 = estimate dynamics, 1 = use input numbers-at-age in NbyageFixed, 2 = multiply input numbers-at-age (NbyageFixed) by a single scaling coefficient, 3 = multiply input numbers-at-age (NbyageFixed) by age specific scaling coefficient.</t>
+          <t>Survey and fishery data specifications</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -974,21 +968,16 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
+        <v>14</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>proj_F</t>
+          <t>index_data</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Unused</t>
+          <t>Survey index in weight (kg) or numbers data</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1009,21 +998,16 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
+        <v>15</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>est_sex_ratio</t>
+          <t>catch_data</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Integer: is sex ration F/(M+F) to be included in the likelihood (assumed normal); 0 = no, 1 = use annual average across ages (uses 2nd age in propF data), 2 = age, and year specific (TBD)</t>
+          <t>Total catch in weight (kg) or numbers data</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1044,21 +1028,16 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Control</t>
-        </is>
+        <v>16</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>sex_ratio_sigma</t>
+          <t>comp_data</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Numeric: initial value or fixed value for sd of normal likelihood for sex ration. Not yet able to estimate.</t>
+          <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1079,16 +1058,16 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>fleet_control</t>
+          <t>emp_sel</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Survey and fishery data specifications</t>
+          <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1109,16 +1088,16 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>index_data</t>
+          <t>age_trans_matrix</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Survey index in weight (kg) or numbers data</t>
+          <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. Can have multiple matrices for a species specified by Age_transition_index.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1139,16 +1118,16 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>catch_data</t>
+          <t>age_error</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Total catch in weight (kg) or numbers data</t>
+          <t>Aging error matrices. Can have only one per species.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1169,16 +1148,16 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>comp_data</t>
+          <t>wt</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
+          <t>Weight-at-age (wt) to use for calculation of derived quantities (SSB, Consumption/Ration, Suitability, Total Catch, Survey Biomass, etc). Can have multiple weight-at-age data-sets for each species, but must be full for all years of the hindcast.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1199,16 +1178,16 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>emp_sel</t>
+          <t>pmature</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
+          <t>Maturity-at-age for each species</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1229,16 +1208,16 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>age_trans_matrix</t>
+          <t>propF</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. Can have multiple matrices for a species specified by Age_transition_index.</t>
+          <t>Percent female at age for each species</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1259,16 +1238,16 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>age_error</t>
+          <t>M1_base</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Aging error matrices. Can have only one per species.</t>
+          <t>Residual natural mortality for each species</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1289,16 +1268,16 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>wt</t>
+          <t>aLW</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Weight-at-age (wt) to use for calculation of derived quantities (SSB, Consumption/Ration, Suitability, Total Catch, Survey Biomass, etc). Can have multiple weight-at-age data-sets for each species, but must be full for all years of the hindcast.</t>
+          <t>Parameters for weight-at-length power function for each species. . Used when estimating time-variant length-based gamma suitability (suitMode = 2) or time-variant length-based lognormal suitability (suitMode = 5)</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1319,16 +1298,21 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>bioenergetics_control</t>
+        </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>pmature</t>
+          <t>Ceq</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Maturity-at-age for each species</t>
+          <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979); 4 = 1 for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1349,16 +1333,21 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>bioenergetics_control</t>
+        </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>propF</t>
+          <t>Cindex</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Percent female at age for each species</t>
+          <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1369,16 +1358,21 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>bioenergetics_control</t>
+        </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>M1_base</t>
+          <t>Pvalue</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Residual natural mortality for each species</t>
+          <t>Numeric: this scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1394,22 +1388,27 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>bioenergetics_control</t>
+        </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>aLW</t>
+          <t>fday</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Parameters for weight-at-length power function for each species. . Used when estimating time-variant length-based gamma suitability (suitMode = 2) or time-variant length-based lognormal suitability (suitMode = 5)</t>
+          <t>Numeric: number of foraging days per year for each species</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1418,12 +1417,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Ceq</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: 1 = Exponential (Stewart et al 1983), 2 = Temperature-dependendence for warm-water species (Kitchell et al 1977; sensu Holsman et al 2015), 3 = temperature dependence for cool and cold-water species (Thornton and Lessem 1979); 4 = 1 for direct input of consumption in Pyrs  where consumption at age = Wt * Pyrs (CA set to 1, fday set to 1, CB set to 0)</t>
+          <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1434,7 +1433,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1443,12 +1442,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Cindex</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
+          <t>Slope of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1459,7 +1458,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1468,12 +1467,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Pvalue</t>
+          <t>Qc</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Numeric: this scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
+          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1484,7 +1483,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1493,18 +1492,18 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>fday</t>
+          <t>Tco</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Numeric: number of foraging days per year for each species</t>
+          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1513,18 +1512,18 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>Tcm</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
+          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1533,18 +1532,18 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>Tcl</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Slope of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
+          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1553,7 +1552,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Qc</t>
+          <t>CK1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1564,7 +1563,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1573,7 +1572,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Tco</t>
+          <t>CK4</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1584,124 +1583,44 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>33</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>bioenergetics_control</t>
-        </is>
+        <v>37</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Tcm</t>
+          <t>env_data</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
+          <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5. Will use the mean for missing years. Temperature should be in celcius.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>34</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>bioenergetics_control</t>
-        </is>
+        <v>38</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Tcl</t>
+          <t>Pyrs</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
+          <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>35</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>bioenergetics_control</t>
-        </is>
+        <v>39</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CK1</t>
+          <t>stom_prop_data</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
-        <is>
-          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>36</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>bioenergetics_control</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>CK4</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>37</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>env_data</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5. Will use the mean for missing years. Temperature should be in celcius.</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>38</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Pyrs</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>39</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>UobsWtAge</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
         <is>
           <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
         </is>
@@ -12863,20 +12782,6 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13102,7 +13007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -13439,7 +13344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X118"/>
   <sheetViews>
@@ -20126,7 +20031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2026"/>
   <sheetViews>
@@ -78913,7 +78818,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -78978,7 +78883,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>2050</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="6">
@@ -79016,62 +78921,71 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>R_sexr</t>
-        </is>
+          <t>nages</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>nages</t>
+          <t>minage</t>
         </is>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>minage</t>
+          <t>nlengths</t>
         </is>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>nlengths</t>
+          <t>pop_wt_index</t>
         </is>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>pop_wt_index</t>
+          <t>ssb_wt_index</t>
         </is>
       </c>
       <c r="B12">
@@ -79087,7 +79001,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ssb_wt_index</t>
+          <t>pop_age_transition_index</t>
         </is>
       </c>
       <c r="B13">
@@ -79103,79 +79017,49 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>pop_age_transition_index</t>
+          <t>sigma_rec_prior</t>
         </is>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0.7071067811865476</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>0.7071067811865476</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>sigma_rec_prior</t>
+          <t>other_food</t>
         </is>
       </c>
       <c r="B15">
-        <v>0.7071067811865476</v>
+        <v>66300000</v>
       </c>
       <c r="C15">
-        <v>0.7071067811865476</v>
+        <v>66300000</v>
       </c>
       <c r="D15">
-        <v>0.7071067811865476</v>
+        <v>66300000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>other_food</t>
+          <t>estDynamics</t>
         </is>
       </c>
       <c r="B16">
-        <v>66300000</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>66300000</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>66300000</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>estDynamics</t>
-        </is>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>est_sex_ratio</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>sex_ratio_sigma</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TMBhelper and removed all non-differentiable bits
Moved fit_tmb to tmbhelper
Removed non-differentiable divide by zero checks and replaced with posfun
dplyr checks
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -368,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -873,10 +873,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>Age_max_selected_upper</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Upper age for selectivity normalization (default = NA). If NA, does not use the age range, If not NA, uses mean selectivity between `Age_max_selected` and `Age_max_selected_upper`</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>Comp_loglike</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Composition data distribution:_x000D_
 -1 = AFSC multinomial_x000D_
@@ -885,41 +902,24 @@
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr">
         <is>
           <t>fleet_control</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>weight1_Numbers2</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>1 = catch/index is weight (kg) the observation _x000D_
 2 = catch/index is in numbers</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Weight_index</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Weight index to use for calculation of derived quantities</t>
-        </is>
-      </c>
-    </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
@@ -928,12 +928,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Age_transition_index</t>
+          <t>Weight_index</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Age transition matrix (e.g. growth trajectory) index to used convert age to length</t>
+          <t>Weight index to use for calculation of derived quantities</t>
         </is>
       </c>
     </row>
@@ -945,12 +945,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Q_index</t>
+          <t>Age_transition_index</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>index to use if catchability coefficients are to be set the same</t>
+          <t>Age transition matrix (e.g. growth trajectory) index to used convert age to length</t>
         </is>
       </c>
     </row>
@@ -962,10 +962,27 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>Q_index</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>index to use if catchability coefficients are to be set the same</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>Estimate_q</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>0 = fixed at "Q_sd_prior" _x000D_
 1 = Estimate as free parameter; _x000D_
@@ -977,23 +994,6 @@
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Q_prior</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Starting value or fixed value for catchability</t>
-        </is>
-      </c>
-    </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
@@ -1002,12 +1002,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Q_sd_prior</t>
+          <t>Q_prior</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Standard deviation for q prior</t>
+          <t>Starting value or fixed value for catchability</t>
         </is>
       </c>
     </row>
@@ -1019,10 +1019,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>Q_sd_prior</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Standard deviation for q prior</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>Time_varying_q</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>0 = no_x000D_
 1 = penalized deviate or random effect _x000D_
@@ -1033,23 +1050,6 @@
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Time_varying_q_sd_prior</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>starting or fixed sd to use for the random walk of time varying q if set to 1</t>
-        </is>
-      </c>
-    </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
@@ -1058,10 +1058,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>Time_varying_q_sd_prior</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>starting or fixed sd to use for the random walk of time varying q if set to 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>Estimate_index_sd</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>0 = use input "Log_sd" from index_data_x000D_
 1 = estimate as free parameter_x000D_
@@ -1069,23 +1086,6 @@
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Index_sd_prior</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Starting value to be used if "Estimate_index_sd" = 1</t>
-        </is>
-      </c>
-    </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
@@ -1094,10 +1094,27 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>Index_sd_prior</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Starting value to be used if "Estimate_index_sd" = 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>Estimate_catch_sd</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>0 = use input "Log_sd" from catch_data_x000D_
 1 = estimate as free parameter_x000D_
@@ -1105,23 +1122,6 @@
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Catch_sd_prior</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Starting value to be used if Estimate_catch_sd = 1</t>
-        </is>
-      </c>
-    </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
@@ -1130,167 +1130,184 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>Catch_sd_prior</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Starting value to be used if Estimate_catch_sd = 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>Comp_weights</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>Composition weights for composition likelihood. _x000D_
 After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>proj_F_prop</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>The proportion of future fishing mortality assigned to this fleet</t>
-        </is>
-      </c>
-    </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>index_data</t>
+          <t>fleet_control</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>proj_F_prop</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Survey index or fishery indices in weight (kg) or numbers</t>
+          <t>The proportion of future fishing mortality assigned to this fleet</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>catch_data</t>
+          <t>index_data</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Total catch in weight (kg) or numbers data</t>
+          <t>Survey index or fishery indices in weight (kg) or numbers</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>comp_data</t>
+          <t>catch_data</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
+          <t>Total catch in weight (kg) or numbers data</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>emp_sel</t>
+          <t>comp_data</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
+          <t>Survey/fishery age or length composition data. Note if sex is 3, put female composition data then male composition data (similar to SS).</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>emp_sel</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Empirical/fixed selectivity for surveys and fisheries (leave empty if not used)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
           <t>age_trans_matrix</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>Age transition matrix (e.g. growth trajectory) used to convert age to length for length comp data. _x000D_
 Can have multiple matrices for a species specified by Age_transition_index.</t>
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>age_error</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Aging error matrices. Can have only one per species.</t>
-        </is>
-      </c>
-    </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>age_error</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Aging error matrices. Can have only one per species.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>weight</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>Time-invariant or -varying empirical weight-at-age for calculation of derived quantities (SSB, Consumption/Ration, Suitability, Total Catch, Survey Biomass, etc). _x000D_
 Can have multiple weight-at-age data-sets for each species.</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>maturity</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Maturity-at-age for each species</t>
-        </is>
-      </c>
-    </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>sex_ratio</t>
+          <t>maturity</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Percent female at age for each species</t>
+          <t>Maturity-at-age for each species</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>sex_ratio</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Percent female at age for each species</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>M1_base</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>Residual natural mortality for each species</t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="57">
+      <c r="A57" t="inlineStr">
         <is>
           <t>bioenergetics_control</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B57" t="inlineStr">
         <is>
           <t>Ceq</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>Integer: switch for which bioenergetics equation to use for each species for ft to scale max consumtion: _x000D_
 1 = Exponential (Stewart et al 1983)_x000D_
@@ -1300,23 +1317,6 @@
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>bioenergetics_control</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Cindex</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
-        </is>
-      </c>
-    </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Pvalue</t>
+          <t>Cindex</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Numeric: this scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
+          <t>Integer: which environmental index in env_data to use to drive bioenergetics</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>fday</t>
+          <t>Pvalue</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Numeric: number of foraging days per year for each species</t>
+          <t>Numeric: this scales the maximum consumption used for ration for each species; Pvalue is in Cmax*fT*Pvalue*Pyrs</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>fday</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
+          <t>Numeric: number of foraging days per year for each species</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>CB</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Slope of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
+          <t>Intercept of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Qc</t>
+          <t>CB</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
+          <t>Slope of allometric mass function for calculating maximum consumption: CA * Weight ^ CB</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Tco</t>
+          <t>Qc</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Tcm</t>
+          <t>Tco</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Tcl</t>
+          <t>Tcm</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CK1</t>
+          <t>Tcl</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>CK4</t>
+          <t>CK1</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1490,46 +1490,63 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>env_data</t>
+          <t>bioenergetics_control</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>CK4</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5 or 6. Will use the mean for missing years. Temperature should be in celcius.</t>
+          <t>Parameter for temperature scaling function of maximum consumption specified by Ceq</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ration_data</t>
+          <t>env_data</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
+          <t>Environmental indices such as bottom temperature data to incorporate into ration equation specificed by Ceq and Cindex. Also used to drive catchability if Estimate_q = 5 or 6. Will use the mean for missing years. Temperature should be in celcius.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>ration_data</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Annual relative foraging rate by age. Multiplied by pvalue and fday to scale maximum consumption to the number of days in a year that foraging occurs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>diet_data</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
         </is>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
+    <row r="74">
+      <c r="A74" t="inlineStr">
         <is>
           <t>Sex</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>0 = combined_x000D_
 1 = use female only _x000D_
@@ -1538,22 +1555,22 @@
         </is>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>NOTE: Most objects are ordered by species code if not specified</t>
-        </is>
-      </c>
-    </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>NOTE: Lengths are index 1 through nlenths</t>
+          <t>NOTE: Most objects are ordered by species code if not specified</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
+        <is>
+          <t>NOTE: Lengths are index 1 through nlenths</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
         <is>
           <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
         </is>

</xml_diff>

<commit_message>
env linkages and rec test
test: beverton and holt recruitment
test: env linkage and mean rec
test: env linkage and M1 (sex/ and sex-nvariant)
test: differential M1_model for species
fix: M1 env linkage dimension in map
</commit_message>
<xml_diff>
--- a/BS2017SS.xlsx
+++ b/BS2017SS.xlsx
@@ -368,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Survey index or fishery indices in weight (kg) or numbers</t>
+          <t>Survey index or fishery indices in weight (kg) or numbers.</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1536,16 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Can also be year specific by including the column, "Year"</t>
+          <t>Stomach proportion by weight for each predator, prey, predator age, prey age combination. Multiple diet-data formats can be included:_x000D_
+_x000D_
+1) If Pred_age &gt;= 0 and Prey_age &gt;= 0, data is assumed to be  diet proportion of prey-at-age/sex in predator-at-age/sex. _x000D_
+2) If Pred_age &gt;= 0 and Prey_age &lt; 0, data is assumed to be mean diet proportion of prey-spp in predator-at-age/sex (sum across prey ages and sexes)_x000D_
+3) If Pred_age &lt; 0 and Prey_age &lt; 0, data is assumed to be  mean diet proportion of prey-spp in predator-spp (sum across prey ages/sexes and take mean across predator ages/sexes)_x000D_
+4) If Pred_age &lt; -500 and Prey_age &lt; 0, data is assumed to be weighted mean diet proportion of prey-spp in predator-spp (sum across prey ages/sexes and take weighted mean across predator ages/sexes). Weights are estimated predators-at-age._x000D_
+_x000D_
+If "Year = 0", the the diet will be assumed to be the average between "suit_styr" and "suit_endyr". _x000D_
+_x000D_
+Only diet-data type 1 can be used for MSVPA based suitability</t>
         </is>
       </c>
     </row>
@@ -1573,6 +1582,20 @@
       <c r="A78" t="inlineStr">
         <is>
           <t>NOTE: Columns for ages are index by 1 trhough nages, but are place holders.</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>NOTE: For catch, index, and comp data, if "Year" is negative, it will predict for that year, but not include the data in the likelihood.</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>NOTE: For emp_sel, weight, and ration_data, if "Year" == 0, those data will be used for all years</t>
         </is>
       </c>
     </row>

</xml_diff>